<commit_message>
Best for 6 and 8
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_3_5.xlsx
+++ b/TestMNIST/MatlabCodes/final_3_5.xlsx
@@ -411,3202 +411,3202 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-0.52729971609210091</v>
+        <v>0.47893404952806951</v>
       </c>
       <c r="B1">
-        <v>0.75407000534145874</v>
+        <v>0.63451543743998229</v>
       </c>
       <c r="C1">
-        <v>-0.77363930831142014</v>
+        <v>-0.49675148066890196</v>
       </c>
       <c r="D1">
-        <v>0.3521444601531909</v>
+        <v>1.7271370535973621E-2</v>
       </c>
       <c r="E1">
-        <v>0.56468266863461658</v>
+        <v>0.69612709297261643</v>
       </c>
       <c r="F1">
-        <v>-0.52618504957387269</v>
+        <v>0.32049810550772623</v>
       </c>
       <c r="G1">
-        <v>-0.979888329160859</v>
+        <v>-0.84456722775048443</v>
       </c>
       <c r="H1">
-        <v>-0.82641714163161284</v>
+        <v>0.22611249960817736</v>
       </c>
       <c r="I1">
-        <v>0.66151809293543562</v>
+        <v>0.68406912221118121</v>
       </c>
       <c r="J1">
-        <v>-0.8906032250040381</v>
+        <v>0.17200321076764863</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7.6190004107140802E-2</v>
+        <v>0.39005417806237358</v>
       </c>
       <c r="B2">
-        <v>-0.5343589266138169</v>
+        <v>0.88326701081561387</v>
       </c>
       <c r="C2">
-        <v>0.62358440352214739</v>
+        <v>-5.0865853260672847E-2</v>
       </c>
       <c r="D2">
-        <v>-0.66596123456805045</v>
+        <v>-0.79883760133551973</v>
       </c>
       <c r="E2">
-        <v>0.38012903635482431</v>
+        <v>0.37531568905468743</v>
       </c>
       <c r="F2">
-        <v>0.18857964602566593</v>
+        <v>0.34451176425764551</v>
       </c>
       <c r="G2">
-        <v>0.44000142707383261</v>
+        <v>0.40876072575518102</v>
       </c>
       <c r="H2">
-        <v>0.21152460842349738</v>
+        <v>-0.38377860959800508</v>
       </c>
       <c r="I2">
-        <v>-0.66103011195827133</v>
+        <v>-0.3892665034175527</v>
       </c>
       <c r="J2">
-        <v>0.46911752574712651</v>
+        <v>-0.88932151400424275</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.17753155875239546</v>
+        <v>-0.59258690998774677</v>
       </c>
       <c r="B3">
-        <v>0.54978243360342249</v>
+        <v>-0.85339266815549519</v>
       </c>
       <c r="C3">
-        <v>-0.20573652029485254</v>
+        <v>-0.89845758438538315</v>
       </c>
       <c r="D3">
-        <v>-0.26418324788728254</v>
+        <v>-0.40255528490340459</v>
       </c>
       <c r="E3">
-        <v>-0.59646751243148877</v>
+        <v>-0.35497734002538017</v>
       </c>
       <c r="F3">
-        <v>0.10469799195015618</v>
+        <v>-0.3733309206200458</v>
       </c>
       <c r="G3">
-        <v>0.26415258854094409</v>
+        <v>0.73044647005154562</v>
       </c>
       <c r="H3">
-        <v>-3.5574209225477792E-2</v>
+        <v>-2.5055163475082198E-2</v>
       </c>
       <c r="I3">
-        <v>-0.43368641393530477</v>
+        <v>0.47631817328723181</v>
       </c>
       <c r="J3">
-        <v>-0.5706870340075304</v>
+        <v>0.64036484848520858</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-0.28578755627405794</v>
+        <v>-0.97648687881693563</v>
       </c>
       <c r="B4">
-        <v>-0.10125603797445784</v>
+        <v>-0.84994126776468448</v>
       </c>
       <c r="C4">
-        <v>2.7327025679142018E-2</v>
+        <v>-0.97836951975356767</v>
       </c>
       <c r="D4">
-        <v>0.42230952960934964</v>
+        <v>0.67289284429168694</v>
       </c>
       <c r="E4">
-        <v>-7.6856782296546841E-2</v>
+        <v>0.99103932217584412</v>
       </c>
       <c r="F4">
-        <v>-3.5400860898099316E-2</v>
+        <v>-0.94813505263717768</v>
       </c>
       <c r="G4">
-        <v>-3.9096790659881753E-2</v>
+        <v>0.90521530230868086</v>
       </c>
       <c r="H4">
-        <v>7.4308760359170251E-2</v>
+        <v>-0.95565204878822851</v>
       </c>
       <c r="I4">
-        <v>0.61332993296867611</v>
+        <v>0.98900453855010162</v>
       </c>
       <c r="J4">
-        <v>0.18225409448252983</v>
+        <v>0.85097320760403516</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>-0.77347903320618605</v>
+        <v>0.17588323719132051</v>
       </c>
       <c r="B5">
-        <v>0.7966163762526205</v>
+        <v>-0.1088086451260713</v>
       </c>
       <c r="C5">
-        <v>-0.57843311749226023</v>
+        <v>0.81226871005839762</v>
       </c>
       <c r="D5">
-        <v>-0.35543714298271151</v>
+        <v>-0.84959258307283814</v>
       </c>
       <c r="E5">
-        <v>-5.4489244369409419E-2</v>
+        <v>-0.8632150354334035</v>
       </c>
       <c r="F5">
-        <v>-0.72616515199078602</v>
+        <v>0.61178450740822754</v>
       </c>
       <c r="G5">
-        <v>0.2277304990886026</v>
+        <v>-0.80816391821990252</v>
       </c>
       <c r="H5">
-        <v>0.20870726967770464</v>
+        <v>-0.1802265086493271</v>
       </c>
       <c r="I5">
-        <v>0.43700828550746995</v>
+        <v>-0.84700010210732146</v>
       </c>
       <c r="J5">
-        <v>-0.40069659157024112</v>
+        <v>-0.72882910872527495</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-0.24534156797587392</v>
+        <v>-0.34576730431727254</v>
       </c>
       <c r="B6">
-        <v>0.55034871536016972</v>
+        <v>-0.58030147343862537</v>
       </c>
       <c r="C6">
-        <v>0.56139096024473678</v>
+        <v>-0.41222492973943664</v>
       </c>
       <c r="D6">
-        <v>-0.40260441458313817</v>
+        <v>0.84968514129805306</v>
       </c>
       <c r="E6">
-        <v>-0.66005005914744042</v>
+        <v>0.76611774982081471</v>
       </c>
       <c r="F6">
-        <v>-0.9596043343766244</v>
+        <v>-0.17807090701207187</v>
       </c>
       <c r="G6">
-        <v>0.24904580732827716</v>
+        <v>-0.12872843460168829</v>
       </c>
       <c r="H6">
-        <v>-0.87036959047262752</v>
+        <v>-1.7900483534769873E-2</v>
       </c>
       <c r="I6">
-        <v>-0.43665158979072777</v>
+        <v>-0.94019062053388369</v>
       </c>
       <c r="J6">
-        <v>0.61537300836634778</v>
+        <v>-0.76819604475055847</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-0.52734014908984661</v>
+        <v>-0.163089227686989</v>
       </c>
       <c r="B7">
-        <v>0.42300806297257493</v>
+        <v>0.14833309868032829</v>
       </c>
       <c r="C7">
-        <v>0.66600370014512511</v>
+        <v>-0.45950599800763048</v>
       </c>
       <c r="D7">
-        <v>0.23371313644827349</v>
+        <v>0.93678515034370824</v>
       </c>
       <c r="E7">
-        <v>0.5077314580692085</v>
+        <v>0.65919594190944553</v>
       </c>
       <c r="F7">
-        <v>-0.34918747763638242</v>
+        <v>-0.95163644591905361</v>
       </c>
       <c r="G7">
-        <v>0.4039989042180287</v>
+        <v>0.28088297296877868</v>
       </c>
       <c r="H7">
-        <v>0.71986439295074578</v>
+        <v>2.2837918713293185E-3</v>
       </c>
       <c r="I7">
-        <v>0.8431662714753746</v>
+        <v>0.36818720054135412</v>
       </c>
       <c r="J7">
-        <v>-0.23576511451219667</v>
+        <v>0.99256228568399485</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-2.2546271290211424E-2</v>
+        <v>-0.89343183791187308</v>
       </c>
       <c r="B8">
-        <v>0.56210750972904688</v>
+        <v>0.37030933939666877</v>
       </c>
       <c r="C8">
-        <v>-0.45219417109792681</v>
+        <v>-0.73885589101648164</v>
       </c>
       <c r="D8">
-        <v>0.61580688711744791</v>
+        <v>0.97234143985759791</v>
       </c>
       <c r="E8">
-        <v>0.67462393954077937</v>
+        <v>0.85913842221938763</v>
       </c>
       <c r="F8">
-        <v>0.53462843307087315</v>
+        <v>-0.65670728530379219</v>
       </c>
       <c r="G8">
-        <v>-0.92430675464106993</v>
+        <v>0.92525826396407185</v>
       </c>
       <c r="H8">
-        <v>0.39610735358354821</v>
+        <v>-0.8830280988999939</v>
       </c>
       <c r="I8">
-        <v>0.23847822606474073</v>
+        <v>0.33844916059263058</v>
       </c>
       <c r="J8">
-        <v>-0.86339486677265931</v>
+        <v>-0.43017242880637285</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.35605623648274648</v>
+        <v>-0.60505711859959566</v>
       </c>
       <c r="B9">
-        <v>-0.76505747285115555</v>
+        <v>-0.88332283711139403</v>
       </c>
       <c r="C9">
-        <v>0.44278591357627567</v>
+        <v>-0.72533079614754647</v>
       </c>
       <c r="D9">
-        <v>-0.43430010957265597</v>
+        <v>0.95397910894923155</v>
       </c>
       <c r="E9">
-        <v>-0.13601900905854666</v>
+        <v>0.71871812152518533</v>
       </c>
       <c r="F9">
-        <v>0.33067755256772702</v>
+        <v>-0.78539168254933012</v>
       </c>
       <c r="G9">
-        <v>9.2233841860878407E-2</v>
+        <v>0.95145693655511765</v>
       </c>
       <c r="H9">
-        <v>0.57103502792344984</v>
+        <v>-0.71706825646575789</v>
       </c>
       <c r="I9">
-        <v>0.44758704750698075</v>
+        <v>0.50525338926587049</v>
       </c>
       <c r="J9">
-        <v>0.50664642355080103</v>
+        <v>0.17196329795124077</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>-0.65073665709831086</v>
+        <v>0.34457806210266129</v>
       </c>
       <c r="B10">
-        <v>0.92059823538066166</v>
+        <v>-0.87977458492194871</v>
       </c>
       <c r="C10">
-        <v>7.7590108440991068E-3</v>
+        <v>-0.50851490206056571</v>
       </c>
       <c r="D10">
-        <v>0.90534618402066935</v>
+        <v>-0.97060797773494778</v>
       </c>
       <c r="E10">
-        <v>0.91012004492139809</v>
+        <v>-4.5090659235929031E-2</v>
       </c>
       <c r="F10">
-        <v>0.79850484457539461</v>
+        <v>0.23139288801917895</v>
       </c>
       <c r="G10">
-        <v>-0.18630028947714111</v>
+        <v>-7.5098709924474677E-2</v>
       </c>
       <c r="H10">
-        <v>0.27082985571581958</v>
+        <v>-0.3439447431327623</v>
       </c>
       <c r="I10">
-        <v>0.45536884896312652</v>
+        <v>0.51568989224409789</v>
       </c>
       <c r="J10">
-        <v>-1.9305780779607453E-2</v>
+        <v>0.57526398316566285</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-0.42003437066941995</v>
+        <v>-0.87544897220282758</v>
       </c>
       <c r="B11">
-        <v>-1.9694337564577571E-2</v>
+        <v>-0.59358959047151916</v>
       </c>
       <c r="C11">
-        <v>-0.94741168312925816</v>
+        <v>-0.73124753008550325</v>
       </c>
       <c r="D11">
-        <v>0.48556916671198963</v>
+        <v>-0.80410182353173454</v>
       </c>
       <c r="E11">
-        <v>0.76195925277254239</v>
+        <v>0.87356579819645352</v>
       </c>
       <c r="F11">
-        <v>0.93303503797666376</v>
+        <v>-0.96333655872397639</v>
       </c>
       <c r="G11">
-        <v>0.35014258456229369</v>
+        <v>0.96340543606581175</v>
       </c>
       <c r="H11">
-        <v>0.73546924022604976</v>
+        <v>-0.94483968801061846</v>
       </c>
       <c r="I11">
-        <v>0.73155992440136441</v>
+        <v>0.95195513484850469</v>
       </c>
       <c r="J11">
-        <v>-0.4585628568843314</v>
+        <v>0.78377823133255875</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.85816860583113075</v>
+        <v>-0.72329012291404815</v>
       </c>
       <c r="B12">
-        <v>-0.35279288313537943</v>
+        <v>0.40080780495943591</v>
       </c>
       <c r="C12">
-        <v>-0.35877094586522634</v>
+        <v>-0.65137771636958286</v>
       </c>
       <c r="D12">
-        <v>6.2535928127214882E-2</v>
+        <v>0.92390036458762226</v>
       </c>
       <c r="E12">
-        <v>-0.9209836881964566</v>
+        <v>0.32135889180659971</v>
       </c>
       <c r="F12">
-        <v>0.20179860258043497</v>
+        <v>-0.85089743504218562</v>
       </c>
       <c r="G12">
-        <v>0.77367840251728504</v>
+        <v>0.16696896600215486</v>
       </c>
       <c r="H12">
-        <v>-0.53927753408538459</v>
+        <v>-0.51014637625585968</v>
       </c>
       <c r="I12">
-        <v>-0.14873946025253248</v>
+        <v>9.3335822625785034E-2</v>
       </c>
       <c r="J12">
-        <v>0.6152446814690441</v>
+        <v>-0.11346734656588442</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-0.32856477982465426</v>
+        <v>-0.78308342548456245</v>
       </c>
       <c r="B13">
-        <v>0.98139063348843636</v>
+        <v>0.13037580542269683</v>
       </c>
       <c r="C13">
-        <v>-0.6744531689178781</v>
+        <v>8.6974435596050087E-2</v>
       </c>
       <c r="D13">
-        <v>0.84117202243714218</v>
+        <v>0.53177351472246992</v>
       </c>
       <c r="E13">
-        <v>0.75977448748916177</v>
+        <v>0.84333410013780807</v>
       </c>
       <c r="F13">
-        <v>0.93633594671985088</v>
+        <v>-0.87544186819285486</v>
       </c>
       <c r="G13">
-        <v>-0.64588255666674599</v>
+        <v>0.85597685091649511</v>
       </c>
       <c r="H13">
-        <v>-0.44654656083741601</v>
+        <v>-5.1679722627040979E-2</v>
       </c>
       <c r="I13">
-        <v>0.8563357749977244</v>
+        <v>0.87893867564211736</v>
       </c>
       <c r="J13">
-        <v>-0.38523873144049459</v>
+        <v>0.63658239527184701</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-0.5701969942789904</v>
+        <v>0.83971482032943923</v>
       </c>
       <c r="B14">
-        <v>0.53297304545248247</v>
+        <v>-0.16079677713976273</v>
       </c>
       <c r="C14">
-        <v>0.44435690971485126</v>
+        <v>0.88220010627261547</v>
       </c>
       <c r="D14">
-        <v>0.75655988358731219</v>
+        <v>-0.82384521991105641</v>
       </c>
       <c r="E14">
-        <v>0.59456016604642303</v>
+        <v>-0.54195274743211974</v>
       </c>
       <c r="F14">
-        <v>0.39717498540803226</v>
+        <v>0.38285759268908237</v>
       </c>
       <c r="G14">
-        <v>-0.47033217204815336</v>
+        <v>0.3413471440989303</v>
       </c>
       <c r="H14">
-        <v>0.83517863300757345</v>
+        <v>0.23474722517588983</v>
       </c>
       <c r="I14">
-        <v>0.75272405619136362</v>
+        <v>-4.9410242673714466E-2</v>
       </c>
       <c r="J14">
-        <v>-0.65477577471951398</v>
+        <v>-4.5193593200361669E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.86945468911741808</v>
+        <v>-0.59480352452038676</v>
       </c>
       <c r="B15">
-        <v>-0.8567215465849809</v>
+        <v>-0.95551989319590291</v>
       </c>
       <c r="C15">
-        <v>0.8229051238021744</v>
+        <v>-0.92523460151179682</v>
       </c>
       <c r="D15">
-        <v>-0.25071990175998937</v>
+        <v>-0.13661511735081974</v>
       </c>
       <c r="E15">
-        <v>-0.52082511093062789</v>
+        <v>0.91908899561305657</v>
       </c>
       <c r="F15">
-        <v>-0.6615528292310342</v>
+        <v>-0.85847017099216705</v>
       </c>
       <c r="G15">
-        <v>0.81154943910698008</v>
+        <v>0.97418386162368931</v>
       </c>
       <c r="H15">
-        <v>-0.50272766260183843</v>
+        <v>-0.95188019282191338</v>
       </c>
       <c r="I15">
-        <v>-0.33414613988706637</v>
+        <v>0.80767290619531629</v>
       </c>
       <c r="J15">
-        <v>0.91020748895373216</v>
+        <v>0.94303294439167562</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.83271429036267919</v>
+        <v>-2.9547806907341038E-2</v>
       </c>
       <c r="B16">
-        <v>-0.36248461797953008</v>
+        <v>-0.89497751991806274</v>
       </c>
       <c r="C16">
-        <v>-8.824117442532689E-2</v>
+        <v>-0.8200463802860456</v>
       </c>
       <c r="D16">
-        <v>-0.74841794462745959</v>
+        <v>-0.20938894141805384</v>
       </c>
       <c r="E16">
-        <v>-0.9073968931287365</v>
+        <v>0.267575663176496</v>
       </c>
       <c r="F16">
-        <v>0.66777301164537917</v>
+        <v>-0.88297293616013661</v>
       </c>
       <c r="G16">
-        <v>-3.3600934611078097E-2</v>
+        <v>0.4743798328125225</v>
       </c>
       <c r="H16">
-        <v>-0.4274130063722123</v>
+        <v>-0.66801005949456416</v>
       </c>
       <c r="I16">
-        <v>-0.6174625172388396</v>
+        <v>0.87895542106471936</v>
       </c>
       <c r="J16">
-        <v>0.73955706489748319</v>
+        <v>0.58977788308917178</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>5.6241166905678444E-2</v>
+        <v>-0.45461239394652669</v>
       </c>
       <c r="B17">
-        <v>0.94603095141436289</v>
+        <v>0.93937267142738834</v>
       </c>
       <c r="C17">
-        <v>-0.72780006619167026</v>
+        <v>0.81985135268813047</v>
       </c>
       <c r="D17">
-        <v>0.89918220474851285</v>
+        <v>0.45883735195903602</v>
       </c>
       <c r="E17">
-        <v>0.32825415332786106</v>
+        <v>-0.14959763220954431</v>
       </c>
       <c r="F17">
-        <v>-0.73620737741273501</v>
+        <v>0.1983630090239672</v>
       </c>
       <c r="G17">
-        <v>-0.7491700310572379</v>
+        <v>-0.4482458657832385</v>
       </c>
       <c r="H17">
-        <v>-4.3264814282750232E-2</v>
+        <v>0.3631646592052945</v>
       </c>
       <c r="I17">
-        <v>0.89352542525110412</v>
+        <v>-0.56009601596722935</v>
       </c>
       <c r="J17">
-        <v>-0.88455024351619194</v>
+        <v>-0.46594933834461161</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.43805447274287418</v>
+        <v>0.92695272801735251</v>
       </c>
       <c r="B18">
-        <v>-0.83527680400273274</v>
+        <v>-0.39061643578279864</v>
       </c>
       <c r="C18">
-        <v>0.62449321349630327</v>
+        <v>-0.13961263766886886</v>
       </c>
       <c r="D18">
-        <v>-0.86690348476233914</v>
+        <v>0.30519112421465744</v>
       </c>
       <c r="E18">
-        <v>-0.67826440998744264</v>
+        <v>-0.99275103636583328</v>
       </c>
       <c r="F18">
-        <v>0.3071592202866486</v>
+        <v>0.52045325146778243</v>
       </c>
       <c r="G18">
-        <v>0.86066518260956348</v>
+        <v>-0.70949303341143377</v>
       </c>
       <c r="H18">
-        <v>-0.6039930775186203</v>
+        <v>0.90992918991195293</v>
       </c>
       <c r="I18">
-        <v>-0.45745493649027058</v>
+        <v>0.41397881068528197</v>
       </c>
       <c r="J18">
-        <v>0.92214713589189756</v>
+        <v>-0.2430949944122987</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-0.78858667733460774</v>
+        <v>-0.92740949348790291</v>
       </c>
       <c r="B19">
-        <v>-0.42105144252261839</v>
+        <v>-0.5774602371936286</v>
       </c>
       <c r="C19">
-        <v>0.2194204840241519</v>
+        <v>-0.79152898636992086</v>
       </c>
       <c r="D19">
-        <v>-0.46752919146037764</v>
+        <v>-3.4062636742107799E-2</v>
       </c>
       <c r="E19">
-        <v>-0.89719041527581911</v>
+        <v>0.85137394983770409</v>
       </c>
       <c r="F19">
-        <v>-0.72590287865570013</v>
+        <v>-0.95106592042765836</v>
       </c>
       <c r="G19">
-        <v>0.31330894905538725</v>
+        <v>-0.16993864534045408</v>
       </c>
       <c r="H19">
-        <v>-0.80976631967772927</v>
+        <v>-0.71532450509428369</v>
       </c>
       <c r="I19">
-        <v>-0.42934495003891293</v>
+        <v>0.93423100208335341</v>
       </c>
       <c r="J19">
-        <v>-0.14716299087245951</v>
+        <v>0.70814518025220519</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-0.71121764189286019</v>
+        <v>8.8940816125759492E-2</v>
       </c>
       <c r="B20">
-        <v>0.74868429083093468</v>
+        <v>-0.25214889538545843</v>
       </c>
       <c r="C20">
-        <v>-0.6160424057541396</v>
+        <v>-0.72943422586841278</v>
       </c>
       <c r="D20">
-        <v>0.54457743628200672</v>
+        <v>0.88280989313822789</v>
       </c>
       <c r="E20">
-        <v>-0.49755630878581109</v>
+        <v>5.3656372733669674E-3</v>
       </c>
       <c r="F20">
-        <v>0.19863149123961127</v>
+        <v>0.5027349676746462</v>
       </c>
       <c r="G20">
-        <v>0.52707206445526533</v>
+        <v>0.72701486886408817</v>
       </c>
       <c r="H20">
-        <v>-0.78543053149533426</v>
+        <v>5.5781860820391195E-2</v>
       </c>
       <c r="I20">
-        <v>0.43559452244381047</v>
+        <v>0.61195599173192672</v>
       </c>
       <c r="J20">
-        <v>-0.63507452976650125</v>
+        <v>0.84043247140420241</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-4.8310656663110109E-2</v>
+        <v>-4.465279797969475E-2</v>
       </c>
       <c r="B21">
-        <v>-0.60517361320802565</v>
+        <v>0.21515072622511111</v>
       </c>
       <c r="C21">
-        <v>0.70176097762251521</v>
+        <v>-0.45720342090012533</v>
       </c>
       <c r="D21">
-        <v>0.20550839521831391</v>
+        <v>0.68654091928743</v>
       </c>
       <c r="E21">
-        <v>-0.53979847500319156</v>
+        <v>-1.0358890065737951E-2</v>
       </c>
       <c r="F21">
-        <v>-0.85502379637958825</v>
+        <v>0.57954423560407775</v>
       </c>
       <c r="G21">
-        <v>-0.25596483468582681</v>
+        <v>0.9073542848591819</v>
       </c>
       <c r="H21">
-        <v>-0.47620228197917153</v>
+        <v>-0.17487904085486539</v>
       </c>
       <c r="I21">
-        <v>0.24057321511912111</v>
+        <v>-0.34630280059579699</v>
       </c>
       <c r="J21">
-        <v>0.36943305498942891</v>
+        <v>-0.51982405225501827</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-0.63162498767727981</v>
+        <v>-0.29712329782841296</v>
       </c>
       <c r="B22">
-        <v>0.97740198122127142</v>
+        <v>0.12657530654363516</v>
       </c>
       <c r="C22">
-        <v>-0.36318334568458627</v>
+        <v>9.6263400136429287E-4</v>
       </c>
       <c r="D22">
-        <v>0.88844238138278986</v>
+        <v>-0.78937980521126183</v>
       </c>
       <c r="E22">
-        <v>0.83243730818051875</v>
+        <v>0.65685830164085512</v>
       </c>
       <c r="F22">
-        <v>-0.87819956916709385</v>
+        <v>0.25074418188329312</v>
       </c>
       <c r="G22">
-        <v>-0.88910527427924169</v>
+        <v>0.18035456776379727</v>
       </c>
       <c r="H22">
-        <v>0.79145115322161397</v>
+        <v>-0.50396542593151239</v>
       </c>
       <c r="I22">
-        <v>0.96335837562080862</v>
+        <v>0.26904749975880526</v>
       </c>
       <c r="J22">
-        <v>-0.72100948699029488</v>
+        <v>0.98047623065404887</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.11310753346050409</v>
+        <v>-0.40606361968874993</v>
       </c>
       <c r="B23">
-        <v>0.63292192627654764</v>
+        <v>-0.39772385697303886</v>
       </c>
       <c r="C23">
-        <v>0.20718953085545874</v>
+        <v>-0.51796557823957967</v>
       </c>
       <c r="D23">
-        <v>0.58921322948060451</v>
+        <v>-2.7658957121307667E-2</v>
       </c>
       <c r="E23">
-        <v>0.77788557747962728</v>
+        <v>0.19945878786137636</v>
       </c>
       <c r="F23">
-        <v>0.13652136752830524</v>
+        <v>-0.18753122900388258</v>
       </c>
       <c r="G23">
-        <v>-0.86669273441707784</v>
+        <v>0.77755600860101404</v>
       </c>
       <c r="H23">
-        <v>-8.005854690565678E-2</v>
+        <v>-0.2892150626065465</v>
       </c>
       <c r="I23">
-        <v>0.49977190901888507</v>
+        <v>0.82193441570275039</v>
       </c>
       <c r="J23">
-        <v>-0.19850346486724049</v>
+        <v>-0.21838729911504179</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.77343567345347775</v>
+        <v>0.21919589190199043</v>
       </c>
       <c r="B24">
-        <v>-0.39767121732450961</v>
+        <v>-0.58596222191502856</v>
       </c>
       <c r="C24">
-        <v>0.61938589802597077</v>
+        <v>-0.45583246029395569</v>
       </c>
       <c r="D24">
-        <v>-0.4797977091191119</v>
+        <v>-0.40942714499442279</v>
       </c>
       <c r="E24">
-        <v>-0.33129484271521176</v>
+        <v>-6.9257943242546319E-2</v>
       </c>
       <c r="F24">
-        <v>-0.97959379778678046</v>
+        <v>-8.1396977507689733E-2</v>
       </c>
       <c r="G24">
-        <v>-0.27861331979476955</v>
+        <v>-0.33472343592094189</v>
       </c>
       <c r="H24">
-        <v>-0.86979144201015379</v>
+        <v>-0.36094368899668899</v>
       </c>
       <c r="I24">
-        <v>-0.90093695355795567</v>
+        <v>-0.72531397205800685</v>
       </c>
       <c r="J24">
-        <v>0.91724705499711723</v>
+        <v>-0.56487384854132316</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-0.96435145452824655</v>
+        <v>0.11004228580800743</v>
       </c>
       <c r="B25">
-        <v>0.64625067591301288</v>
+        <v>0.67868437524004688</v>
       </c>
       <c r="C25">
-        <v>-0.80515196443216541</v>
+        <v>0.59316384433038538</v>
       </c>
       <c r="D25">
-        <v>0.919203124994877</v>
+        <v>0.57383656379427483</v>
       </c>
       <c r="E25">
-        <v>0.95137051843432363</v>
+        <v>-0.64790125123869446</v>
       </c>
       <c r="F25">
-        <v>7.4546962534140768E-2</v>
+        <v>0.86476941580251732</v>
       </c>
       <c r="G25">
-        <v>0.51666657354004064</v>
+        <v>-0.88581197349092644</v>
       </c>
       <c r="H25">
-        <v>0.18813802329360069</v>
+        <v>0.56499203663858266</v>
       </c>
       <c r="I25">
-        <v>0.98783233483180455</v>
+        <v>-0.61517458336331921</v>
       </c>
       <c r="J25">
-        <v>-0.52969817783814166</v>
+        <v>-0.38666654199803968</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3.3908602783560712E-2</v>
+        <v>-0.24664301143991627</v>
       </c>
       <c r="B26">
-        <v>-0.24650973114434335</v>
+        <v>0.64347103023010277</v>
       </c>
       <c r="C26">
-        <v>0.76130282080824974</v>
+        <v>-9.3222187998720771E-2</v>
       </c>
       <c r="D26">
-        <v>-0.58389096874208157</v>
+        <v>-0.35409184539249822</v>
       </c>
       <c r="E26">
-        <v>0.34444669639236358</v>
+        <v>-0.53158030303722248</v>
       </c>
       <c r="F26">
-        <v>0.67724819758480681</v>
+        <v>0.63481418130459721</v>
       </c>
       <c r="G26">
-        <v>0.87409682486483864</v>
+        <v>0.72566456868001838</v>
       </c>
       <c r="H26">
-        <v>9.2283929066583975E-2</v>
+        <v>-0.14765227140303386</v>
       </c>
       <c r="I26">
-        <v>-0.41522612272465853</v>
+        <v>-1.2708192254261794E-2</v>
       </c>
       <c r="J26">
-        <v>0.41160561934223033</v>
+        <v>0.23965923331567746</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.92349246463071077</v>
+        <v>0.61385554215933502</v>
       </c>
       <c r="B27">
-        <v>-0.30024114618316783</v>
+        <v>0.29720215951933915</v>
       </c>
       <c r="C27">
-        <v>0.83567374989041543</v>
+        <v>-0.56348639831063718</v>
       </c>
       <c r="D27">
-        <v>-0.85110859133815353</v>
+        <v>-0.59304510216225115</v>
       </c>
       <c r="E27">
-        <v>-0.65646639216611491</v>
+        <v>0.91151110589237716</v>
       </c>
       <c r="F27">
-        <v>0.5298643720281383</v>
+        <v>7.2938511525060284E-2</v>
       </c>
       <c r="G27">
-        <v>0.61802090374496721</v>
+        <v>-0.90326879529832105</v>
       </c>
       <c r="H27">
-        <v>0.18015144472166478</v>
+        <v>0.55434906371895931</v>
       </c>
       <c r="I27">
-        <v>0.17989819655280634</v>
+        <v>0.62723856966587266</v>
       </c>
       <c r="J27">
-        <v>0.83627211683424618</v>
+        <v>-0.38776020234901126</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>-0.69222738763788516</v>
+        <v>0.94640250138814552</v>
       </c>
       <c r="B28">
-        <v>0.52635619296880232</v>
+        <v>0.96428971231050542</v>
       </c>
       <c r="C28">
-        <v>-0.83071100957170796</v>
+        <v>0.91380491282653231</v>
       </c>
       <c r="D28">
-        <v>0.50360442448934073</v>
+        <v>0.59698837602152988</v>
       </c>
       <c r="E28">
-        <v>0.65676966824273852</v>
+        <v>-0.76453274498520429</v>
       </c>
       <c r="F28">
-        <v>-0.38310474191816057</v>
+        <v>0.96056657507537602</v>
       </c>
       <c r="G28">
-        <v>-0.4679053827690326</v>
+        <v>-0.4438454297931701</v>
       </c>
       <c r="H28">
-        <v>0.97924752400509318</v>
+        <v>0.85669438273641796</v>
       </c>
       <c r="I28">
-        <v>0.48212445658013486</v>
+        <v>-0.44369127109159556</v>
       </c>
       <c r="J28">
-        <v>0.30989812832670066</v>
+        <v>-0.43824810627686728</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>-0.91198805570692221</v>
+        <v>0.77630570521874442</v>
       </c>
       <c r="B29">
-        <v>-0.43555830481276775</v>
+        <v>-0.413122562674472</v>
       </c>
       <c r="C29">
-        <v>-0.92648328061622154</v>
+        <v>0.95893759692062941</v>
       </c>
       <c r="D29">
-        <v>6.3219571116421208E-2</v>
+        <v>-0.48907980357665964</v>
       </c>
       <c r="E29">
-        <v>0.46482157095352905</v>
+        <v>-0.77595800605374277</v>
       </c>
       <c r="F29">
-        <v>0.94110104712685916</v>
+        <v>-0.36944307100424395</v>
       </c>
       <c r="G29">
-        <v>-0.9358656654302715</v>
+        <v>0.62390498792109372</v>
       </c>
       <c r="H29">
-        <v>0.85622907060616327</v>
+        <v>0.49406660218279291</v>
       </c>
       <c r="I29">
-        <v>0.65249342150019229</v>
+        <v>-0.39150072259469459</v>
       </c>
       <c r="J29">
-        <v>-0.9064361919628352</v>
+        <v>4.6202559708945747E-2</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.86300583039864565</v>
+        <v>0.93261451149719887</v>
       </c>
       <c r="B30">
-        <v>-0.8897552897257287</v>
+        <v>0.77579272243638897</v>
       </c>
       <c r="C30">
-        <v>0.90125415831986622</v>
+        <v>0.9429474155421127</v>
       </c>
       <c r="D30">
-        <v>-0.75684644916752852</v>
+        <v>-0.62402356553553662</v>
       </c>
       <c r="E30">
-        <v>-0.98477821980337199</v>
+        <v>-0.65207585731747708</v>
       </c>
       <c r="F30">
-        <v>-0.77798733641740159</v>
+        <v>0.77209818875952063</v>
       </c>
       <c r="G30">
-        <v>0.84873908103942397</v>
+        <v>6.356381840990967E-2</v>
       </c>
       <c r="H30">
-        <v>-0.68168974671962512</v>
+        <v>0.98080069222321076</v>
       </c>
       <c r="I30">
-        <v>-0.85841184202287635</v>
+        <v>-0.64513891499879938</v>
       </c>
       <c r="J30">
-        <v>0.82742161076899112</v>
+        <v>-0.82361474341511531</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.5827737659882487</v>
+        <v>-0.93348158257231084</v>
       </c>
       <c r="B31">
-        <v>-0.92454136849772894</v>
+        <v>-0.80102870707478646</v>
       </c>
       <c r="C31">
-        <v>0.33683337498246646</v>
+        <v>-0.79698466701879733</v>
       </c>
       <c r="D31">
-        <v>-0.893716937194445</v>
+        <v>-0.32874701684739965</v>
       </c>
       <c r="E31">
-        <v>-0.541307905525927</v>
+        <v>-7.6655666254893421E-3</v>
       </c>
       <c r="F31">
-        <v>0.90909965017019179</v>
+        <v>-0.30489639574525962</v>
       </c>
       <c r="G31">
-        <v>0.78405320481402452</v>
+        <v>-0.73425930867025413</v>
       </c>
       <c r="H31">
-        <v>-0.61620023885517961</v>
+        <v>-0.931748208856367</v>
       </c>
       <c r="I31">
-        <v>-0.75255853614492063</v>
+        <v>0.4711415839582605</v>
       </c>
       <c r="J31">
-        <v>0.12464732850715711</v>
+        <v>0.91850097547848175</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-0.72669615385397257</v>
+        <v>0.80534582592292747</v>
       </c>
       <c r="B32">
-        <v>0.54051521549346815</v>
+        <v>-0.26083984215720113</v>
       </c>
       <c r="C32">
-        <v>-0.81172170607889826</v>
+        <v>0.39110438072359288</v>
       </c>
       <c r="D32">
-        <v>0.83864961501202395</v>
+        <v>-0.76570617406351693</v>
       </c>
       <c r="E32">
-        <v>-8.2679116501781169E-2</v>
+        <v>0.1344207443711406</v>
       </c>
       <c r="F32">
-        <v>0.88747248954314861</v>
+        <v>0.55470682294450158</v>
       </c>
       <c r="G32">
-        <v>-0.70776308016248457</v>
+        <v>-0.18361438869763394</v>
       </c>
       <c r="H32">
-        <v>0.87819245931600332</v>
+        <v>-0.37372232339787287</v>
       </c>
       <c r="I32">
-        <v>2.6138196780084381E-2</v>
+        <v>0.87421196426490166</v>
       </c>
       <c r="J32">
-        <v>-0.93877038770638166</v>
+        <v>-0.54612191234142604</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.62491842656318231</v>
+        <v>0.95385329415510833</v>
       </c>
       <c r="B33">
-        <v>-0.38665646603563514</v>
+        <v>7.5053966480339643E-2</v>
       </c>
       <c r="C33">
-        <v>-0.15931972270172459</v>
+        <v>0.79463012025468394</v>
       </c>
       <c r="D33">
-        <v>-7.7849952553787335E-2</v>
+        <v>0.71115450694812721</v>
       </c>
       <c r="E33">
-        <v>0.47791563134221071</v>
+        <v>-0.87916494360901931</v>
       </c>
       <c r="F33">
-        <v>0.9514193201137906</v>
+        <v>0.94591965869763917</v>
       </c>
       <c r="G33">
-        <v>0.64415902801730451</v>
+        <v>-0.23782491484319079</v>
       </c>
       <c r="H33">
-        <v>-0.55273404090829714</v>
+        <v>0.93958015366115899</v>
       </c>
       <c r="I33">
-        <v>-0.38828405200684801</v>
+        <v>-0.62986198803031834</v>
       </c>
       <c r="J33">
-        <v>0.67937419351842798</v>
+        <v>0.62692500820095609</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>-0.57262484845371919</v>
+        <v>-0.20471124048778327</v>
       </c>
       <c r="B34">
-        <v>0.33250513291254902</v>
+        <v>0.33462886543847475</v>
       </c>
       <c r="C34">
-        <v>-0.70867702654524367</v>
+        <v>0.53075156340704255</v>
       </c>
       <c r="D34">
-        <v>-0.71852372387837515</v>
+        <v>0.63429229274577126</v>
       </c>
       <c r="E34">
-        <v>0.45886772382986579</v>
+        <v>0.7039224927307256</v>
       </c>
       <c r="F34">
-        <v>-0.471159629639195</v>
+        <v>-0.77993617623436795</v>
       </c>
       <c r="G34">
-        <v>-6.0426632730431806E-2</v>
+        <v>0.84547992785836734</v>
       </c>
       <c r="H34">
-        <v>-0.90763702404735036</v>
+        <v>-0.51148156866546435</v>
       </c>
       <c r="I34">
-        <v>0.62315666509880474</v>
+        <v>0.59351519395763075</v>
       </c>
       <c r="J34">
-        <v>0.1556711446333934</v>
+        <v>0.33969375939902952</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>-0.59994237060384881</v>
+        <v>0.86857886226797265</v>
       </c>
       <c r="B35">
-        <v>0.41258015339068549</v>
+        <v>0.10424440576447139</v>
       </c>
       <c r="C35">
-        <v>-0.45427101952290727</v>
+        <v>0.12991045363048215</v>
       </c>
       <c r="D35">
-        <v>0.42201651147546598</v>
+        <v>0.16460420310073745</v>
       </c>
       <c r="E35">
-        <v>0.38799683340110602</v>
+        <v>-0.60600821447205344</v>
       </c>
       <c r="F35">
-        <v>-0.69034381355479346</v>
+        <v>0.69553977484879637</v>
       </c>
       <c r="G35">
-        <v>-0.35610802235001604</v>
+        <v>-0.12540915165330796</v>
       </c>
       <c r="H35">
-        <v>0.90143668678904276</v>
+        <v>0.62470536906517837</v>
       </c>
       <c r="I35">
-        <v>0.46600012088242981</v>
+        <v>-0.98425488134845018</v>
       </c>
       <c r="J35">
-        <v>-0.73099115895569955</v>
+        <v>-0.61816068897134957</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.98992944395961846</v>
+        <v>0.93793844109780866</v>
       </c>
       <c r="B36">
-        <v>-0.99161814690322247</v>
+        <v>0.11365135140877103</v>
       </c>
       <c r="C36">
-        <v>0.99698490934903072</v>
+        <v>0.90333940902942711</v>
       </c>
       <c r="D36">
-        <v>-0.99450558034639436</v>
+        <v>0.66157983309282897</v>
       </c>
       <c r="E36">
-        <v>-0.94706366912721129</v>
+        <v>-0.94344553482384208</v>
       </c>
       <c r="F36">
-        <v>0.76885738659262104</v>
+        <v>0.7532230288379842</v>
       </c>
       <c r="G36">
-        <v>0.99772160336383076</v>
+        <v>-1.2745888752792861E-2</v>
       </c>
       <c r="H36">
-        <v>-0.69281552702874627</v>
+        <v>0.4796453679290138</v>
       </c>
       <c r="I36">
-        <v>-0.98049006492996582</v>
+        <v>-0.64226616204990494</v>
       </c>
       <c r="J36">
-        <v>0.97322986182406734</v>
+        <v>-0.22539671440499098</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>-0.34855854270930597</v>
+        <v>-0.93176706476306748</v>
       </c>
       <c r="B37">
-        <v>0.77687764314324192</v>
+        <v>0.90153876941670485</v>
       </c>
       <c r="C37">
-        <v>-0.11508878625921345</v>
+        <v>-0.43342989272240345</v>
       </c>
       <c r="D37">
-        <v>0.83556028758048329</v>
+        <v>-0.29273207590586031</v>
       </c>
       <c r="E37">
-        <v>0.93783896501984565</v>
+        <v>0.80010302786715326</v>
       </c>
       <c r="F37">
-        <v>0.69148470319745647</v>
+        <v>-0.64611464741573821</v>
       </c>
       <c r="G37">
-        <v>-0.67873903186721152</v>
+        <v>-0.38736234583853785</v>
       </c>
       <c r="H37">
-        <v>0.55969286677384178</v>
+        <v>-0.43882341309903344</v>
       </c>
       <c r="I37">
-        <v>0.95791813664393144</v>
+        <v>0.79321360646572181</v>
       </c>
       <c r="J37">
-        <v>-0.12646487698726597</v>
+        <v>-0.73361337794522163</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.18092168200496114</v>
+        <v>0.45879276690047011</v>
       </c>
       <c r="B38">
-        <v>-0.56280189216482612</v>
+        <v>0.91407252613579071</v>
       </c>
       <c r="C38">
-        <v>0.60145555511634829</v>
+        <v>0.63335769037468326</v>
       </c>
       <c r="D38">
-        <v>0.49204978996040916</v>
+        <v>-0.34266912552221329</v>
       </c>
       <c r="E38">
-        <v>0.5662792594895808</v>
+        <v>0.70158807426780667</v>
       </c>
       <c r="F38">
-        <v>5.9699877179848954E-2</v>
+        <v>0.65154294003998092</v>
       </c>
       <c r="G38">
-        <v>0.25255766075263664</v>
+        <v>-0.81706247305659496</v>
       </c>
       <c r="H38">
-        <v>0.91733596560251196</v>
+        <v>0.68706668671681481</v>
       </c>
       <c r="I38">
-        <v>-0.47643058698112856</v>
+        <v>-0.57547328832281897</v>
       </c>
       <c r="J38">
-        <v>-0.43718497490725811</v>
+        <v>-0.35864009475453429</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>-0.75757481964709739</v>
+        <v>-0.58953164732376029</v>
       </c>
       <c r="B39">
-        <v>0.48930214873947125</v>
+        <v>-0.46718638953448288</v>
       </c>
       <c r="C39">
-        <v>-0.8162815432329108</v>
+        <v>-0.57587287468893855</v>
       </c>
       <c r="D39">
-        <v>0.90290274850519114</v>
+        <v>0.50019510800001055</v>
       </c>
       <c r="E39">
-        <v>0.56659917530203641</v>
+        <v>0.12881201237707307</v>
       </c>
       <c r="F39">
-        <v>-0.31160315033201741</v>
+        <v>-0.78953298908624281</v>
       </c>
       <c r="G39">
-        <v>-0.80295169978011649</v>
+        <v>0.46332543041246399</v>
       </c>
       <c r="H39">
-        <v>-0.22123688207586559</v>
+        <v>-0.2916612471563092</v>
       </c>
       <c r="I39">
-        <v>-8.2332881019443513E-2</v>
+        <v>-0.38253193258701718</v>
       </c>
       <c r="J39">
-        <v>-0.91500972457102259</v>
+        <v>-0.26205754040065471</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>-0.86893222258848235</v>
+        <v>0.4964237176422065</v>
       </c>
       <c r="B40">
-        <v>0.32779136077902837</v>
+        <v>-0.89432904980332362</v>
       </c>
       <c r="C40">
-        <v>-0.49823009457028261</v>
+        <v>-0.79472374469235019</v>
       </c>
       <c r="D40">
-        <v>0.94012674054089174</v>
+        <v>-0.95597515925111642</v>
       </c>
       <c r="E40">
-        <v>-5.6315747780891524E-3</v>
+        <v>-0.71473407509520692</v>
       </c>
       <c r="F40">
-        <v>-8.0898567006184682E-2</v>
+        <v>-0.17295777423724915</v>
       </c>
       <c r="G40">
-        <v>-0.80067835342563953</v>
+        <v>0.87959653274456762</v>
       </c>
       <c r="H40">
-        <v>0.8005156349505812</v>
+        <v>-0.52733157470792758</v>
       </c>
       <c r="I40">
-        <v>-0.13397540557639925</v>
+        <v>0.39462973860122197</v>
       </c>
       <c r="J40">
-        <v>-0.48089267630526583</v>
+        <v>0.81676590083711331</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0.72469984906101959</v>
+        <v>-0.83333335678787057</v>
       </c>
       <c r="B41">
-        <v>-0.91293095867592289</v>
+        <v>-0.86033638436220283</v>
       </c>
       <c r="C41">
-        <v>0.85988244711568074</v>
+        <v>-0.85560547788021024</v>
       </c>
       <c r="D41">
-        <v>-0.39511387015484378</v>
+        <v>0.87412507116645444</v>
       </c>
       <c r="E41">
-        <v>-0.77325650625143649</v>
+        <v>-0.29820861150610128</v>
       </c>
       <c r="F41">
-        <v>-0.69040975077496158</v>
+        <v>-0.50830683334983562</v>
       </c>
       <c r="G41">
-        <v>0.86547438766834872</v>
+        <v>0.73182248633450542</v>
       </c>
       <c r="H41">
-        <v>-0.10780165596852009</v>
+        <v>-0.97194431503995038</v>
       </c>
       <c r="I41">
-        <v>-0.94838687803032562</v>
+        <v>3.9965755325599227E-2</v>
       </c>
       <c r="J41">
-        <v>0.77557431841672675</v>
+        <v>0.71501211654510899</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>-0.1033030528031457</v>
+        <v>0.57661796977304736</v>
       </c>
       <c r="B42">
-        <v>0.97667808703781889</v>
+        <v>0.64411734273935484</v>
       </c>
       <c r="C42">
-        <v>-0.44125134095110985</v>
+        <v>0.76844857762918095</v>
       </c>
       <c r="D42">
-        <v>0.97746536218015045</v>
+        <v>-0.60653841099721661</v>
       </c>
       <c r="E42">
-        <v>0.72897505041228272</v>
+        <v>-0.85980228392137659</v>
       </c>
       <c r="F42">
-        <v>-7.6855998965889641E-2</v>
+        <v>0.14800824885796665</v>
       </c>
       <c r="G42">
-        <v>-0.83329130508177573</v>
+        <v>-7.6099069433036792E-2</v>
       </c>
       <c r="H42">
-        <v>0.73761238664862983</v>
+        <v>0.44540445912808679</v>
       </c>
       <c r="I42">
-        <v>0.63423475943963159</v>
+        <v>0.5213549396200573</v>
       </c>
       <c r="J42">
-        <v>-0.80781322218260609</v>
+        <v>-0.19612511786182732</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>0.14695585479114706</v>
+        <v>-0.64345488061842959</v>
       </c>
       <c r="B43">
-        <v>-0.42177429323645271</v>
+        <v>-0.83145741860203448</v>
       </c>
       <c r="C43">
-        <v>0.16065214989249071</v>
+        <v>-0.77159072117301064</v>
       </c>
       <c r="D43">
-        <v>-0.6104999664106735</v>
+        <v>0.6593114576336403</v>
       </c>
       <c r="E43">
-        <v>2.1428354361952683E-2</v>
+        <v>0.70681297088480033</v>
       </c>
       <c r="F43">
-        <v>0.71454434951276768</v>
+        <v>-0.82180045597567686</v>
       </c>
       <c r="G43">
-        <v>-0.7500121549577905</v>
+        <v>0.57806813170712179</v>
       </c>
       <c r="H43">
-        <v>-0.44854385123802126</v>
+        <v>-0.81966512610362541</v>
       </c>
       <c r="I43">
-        <v>-0.66227753508641973</v>
+        <v>0.76180584323811174</v>
       </c>
       <c r="J43">
-        <v>-0.50459643253757247</v>
+        <v>0.28616461077877642</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0.19795215861419194</v>
+        <v>0.29242968704464511</v>
       </c>
       <c r="B44">
-        <v>-0.71115685331527123</v>
+        <v>0.92620314135020687</v>
       </c>
       <c r="C44">
-        <v>0.98674634849466336</v>
+        <v>0.65066349364521525</v>
       </c>
       <c r="D44">
-        <v>-0.61496445893983442</v>
+        <v>0.91601119654157159</v>
       </c>
       <c r="E44">
-        <v>-0.76978123559187028</v>
+        <v>-0.32727367679616115</v>
       </c>
       <c r="F44">
-        <v>-0.86528636561756567</v>
+        <v>-0.33196968437528379</v>
       </c>
       <c r="G44">
-        <v>0.8203947818846915</v>
+        <v>-0.98559864149196175</v>
       </c>
       <c r="H44">
-        <v>-0.89643849764074712</v>
+        <v>0.57550431946624314</v>
       </c>
       <c r="I44">
-        <v>-0.63780289241708887</v>
+        <v>-0.11234957885807774</v>
       </c>
       <c r="J44">
-        <v>0.83213471759689051</v>
+        <v>-0.87246687361560582</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0.11465923058903046</v>
+        <v>1.4739689231184086E-2</v>
       </c>
       <c r="B45">
-        <v>-0.47000807246086646</v>
+        <v>0.27575349886770339</v>
       </c>
       <c r="C45">
-        <v>0.91431386706236362</v>
+        <v>0.75472444867239896</v>
       </c>
       <c r="D45">
-        <v>-0.47538022512690048</v>
+        <v>-0.36381995506029957</v>
       </c>
       <c r="E45">
-        <v>-0.47391568213573043</v>
+        <v>-0.32936929390286718</v>
       </c>
       <c r="F45">
-        <v>-0.40473716035218393</v>
+        <v>0.55882692448877558</v>
       </c>
       <c r="G45">
-        <v>0.29846806165539858</v>
+        <v>-0.36242835491195724</v>
       </c>
       <c r="H45">
-        <v>0.26230288254517425</v>
+        <v>0.28275899197939758</v>
       </c>
       <c r="I45">
-        <v>2.1479051167341407E-2</v>
+        <v>-0.20004470406963842</v>
       </c>
       <c r="J45">
-        <v>-4.0188323989485422E-2</v>
+        <v>-0.73141431221651432</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>0.84925765719984447</v>
+        <v>-0.34042982679528422</v>
       </c>
       <c r="B46">
-        <v>-0.26328641014965665</v>
+        <v>0.12633842733816961</v>
       </c>
       <c r="C46">
-        <v>0.34944830208696243</v>
+        <v>-0.59661774716371052</v>
       </c>
       <c r="D46">
-        <v>-0.8333725077914047</v>
+        <v>7.1582787603688039E-2</v>
       </c>
       <c r="E46">
-        <v>-0.56981535281286011</v>
+        <v>0.7146301346170415</v>
       </c>
       <c r="F46">
-        <v>0.94426355901019787</v>
+        <v>-0.31271881684065167</v>
       </c>
       <c r="G46">
-        <v>0.71156819695360329</v>
+        <v>-0.47061178962777683</v>
       </c>
       <c r="H46">
-        <v>0.24394356725095073</v>
+        <v>-7.0530636041171033E-2</v>
       </c>
       <c r="I46">
-        <v>-0.94346299179531989</v>
+        <v>-0.10516618115120895</v>
       </c>
       <c r="J46">
-        <v>0.89375001612344207</v>
+        <v>0.36460695404977633</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>0.8405989597534087</v>
+        <v>-0.15228471969566085</v>
       </c>
       <c r="B47">
-        <v>-0.71047083112077658</v>
+        <v>-0.77078550469476137</v>
       </c>
       <c r="C47">
-        <v>0.29599864618890342</v>
+        <v>-0.62863284314449575</v>
       </c>
       <c r="D47">
-        <v>-2.0197297298445265E-3</v>
+        <v>-0.70865244012893025</v>
       </c>
       <c r="E47">
-        <v>-0.93804997846997629</v>
+        <v>0.40458844098477009</v>
       </c>
       <c r="F47">
-        <v>-0.92714647382908721</v>
+        <v>0.42827245354292481</v>
       </c>
       <c r="G47">
-        <v>0.25423392714247567</v>
+        <v>0.36446607656980018</v>
       </c>
       <c r="H47">
-        <v>0.19632958778518578</v>
+        <v>0.28141574814272702</v>
       </c>
       <c r="I47">
-        <v>-0.4672113347862033</v>
+        <v>0.43381606310427789</v>
       </c>
       <c r="J47">
-        <v>0.63731806404046221</v>
+        <v>0.76263951730584245</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>9.4620475209496818E-2</v>
+        <v>-0.22654280461286799</v>
       </c>
       <c r="B48">
-        <v>0.37422547947370294</v>
+        <v>0.31543291505919968</v>
       </c>
       <c r="C48">
-        <v>0.50659956278171958</v>
+        <v>0.92884690019090821</v>
       </c>
       <c r="D48">
-        <v>-0.13902541473008403</v>
+        <v>-0.34348918633445208</v>
       </c>
       <c r="E48">
-        <v>0.26635807072701967</v>
+        <v>-0.32710814806229666</v>
       </c>
       <c r="F48">
-        <v>0.27815632271081209</v>
+        <v>0.44494516934719358</v>
       </c>
       <c r="G48">
-        <v>-0.46955841062173698</v>
+        <v>-0.20464198812833362</v>
       </c>
       <c r="H48">
-        <v>2.40998620848005E-2</v>
+        <v>8.3661117427819912E-2</v>
       </c>
       <c r="I48">
-        <v>-0.44801605684612689</v>
+        <v>-0.27997943570675188</v>
       </c>
       <c r="J48">
-        <v>-0.20597473649998566</v>
+        <v>-0.48338079596212491</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>-7.2198726719242393E-2</v>
+        <v>-0.52578596759411689</v>
       </c>
       <c r="B49">
-        <v>-0.15031982485502546</v>
+        <v>-0.96559857818358119</v>
       </c>
       <c r="C49">
-        <v>0.67332287316813666</v>
+        <v>-0.76812898325692869</v>
       </c>
       <c r="D49">
-        <v>-0.85397593476147726</v>
+        <v>0.35981323680317706</v>
       </c>
       <c r="E49">
-        <v>-0.76204364415029702</v>
+        <v>0.25548328774760248</v>
       </c>
       <c r="F49">
-        <v>-0.94197387975611224</v>
+        <v>-0.8888409164941975</v>
       </c>
       <c r="G49">
-        <v>7.6015678350695552E-3</v>
+        <v>0.84698134041085682</v>
       </c>
       <c r="H49">
-        <v>-0.36153655052837641</v>
+        <v>-0.9757159961819124</v>
       </c>
       <c r="I49">
-        <v>-0.53350791346332971</v>
+        <v>0.77460507259342481</v>
       </c>
       <c r="J49">
-        <v>0.55008764904162077</v>
+        <v>0.90607474240020214</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>-0.90864936819232633</v>
+        <v>-0.93399007097971865</v>
       </c>
       <c r="B50">
-        <v>0.93313856391985894</v>
+        <v>0.29272890521606587</v>
       </c>
       <c r="C50">
-        <v>-0.93867777738757263</v>
+        <v>-0.32461712818963745</v>
       </c>
       <c r="D50">
-        <v>0.81909764078139957</v>
+        <v>-0.76024481992587778</v>
       </c>
       <c r="E50">
-        <v>0.80376798248645742</v>
+        <v>0.44312452889192694</v>
       </c>
       <c r="F50">
-        <v>0.91731585235015189</v>
+        <v>-0.33277474773882965</v>
       </c>
       <c r="G50">
-        <v>-0.68646794239225473</v>
+        <v>-0.32536992171867979</v>
       </c>
       <c r="H50">
-        <v>0.67672851561089098</v>
+        <v>-0.55762533061048969</v>
       </c>
       <c r="I50">
-        <v>0.75166644438447061</v>
+        <v>-8.5497652104381497E-2</v>
       </c>
       <c r="J50">
-        <v>-0.96870323713251882</v>
+        <v>-0.73530299458830151</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>-0.79889298509783335</v>
+        <v>-5.1594281296610742E-2</v>
       </c>
       <c r="B51">
-        <v>0.89420130599627479</v>
+        <v>0.57043795989667734</v>
       </c>
       <c r="C51">
-        <v>-0.84439691778296866</v>
+        <v>0.64885482044007603</v>
       </c>
       <c r="D51">
-        <v>0.84438885551130805</v>
+        <v>-0.82959026449212891</v>
       </c>
       <c r="E51">
-        <v>0.52816689297865127</v>
+        <v>-0.9463917515062038</v>
       </c>
       <c r="F51">
-        <v>0.81875880352782637</v>
+        <v>0.61435347374635896</v>
       </c>
       <c r="G51">
-        <v>-0.98402513538431324</v>
+        <v>-0.98117157587701775</v>
       </c>
       <c r="H51">
-        <v>0.93384749508890086</v>
+        <v>0.54609213391691092</v>
       </c>
       <c r="I51">
-        <v>0.97848932669385058</v>
+        <v>-0.78188159299598348</v>
       </c>
       <c r="J51">
-        <v>-0.90245981859303159</v>
+        <v>-0.60017957498350238</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>0.67998707660389768</v>
+        <v>-0.50247167016611793</v>
       </c>
       <c r="B52">
-        <v>7.3289690818829582E-3</v>
+        <v>-0.76328353128731141</v>
       </c>
       <c r="C52">
-        <v>0.93962843016336273</v>
+        <v>-0.3303527634735669</v>
       </c>
       <c r="D52">
-        <v>-0.53725022421544311</v>
+        <v>-0.81907570574338096</v>
       </c>
       <c r="E52">
-        <v>-0.93295618055306173</v>
+        <v>0.78192298085896828</v>
       </c>
       <c r="F52">
-        <v>-2.8405564509194379E-2</v>
+        <v>-0.62584839831798278</v>
       </c>
       <c r="G52">
-        <v>0.97456059547513263</v>
+        <v>0.58019930861511926</v>
       </c>
       <c r="H52">
-        <v>-0.80721894311919373</v>
+        <v>-0.74400596703681865</v>
       </c>
       <c r="I52">
-        <v>-0.5859306501948921</v>
+        <v>0.31038195940182289</v>
       </c>
       <c r="J52">
-        <v>0.95099315751450919</v>
+        <v>-0.51101392877257945</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>-0.66108460249087009</v>
+        <v>0.2690961615909096</v>
       </c>
       <c r="B53">
-        <v>0.20020162231413041</v>
+        <v>-0.44886883612138273</v>
       </c>
       <c r="C53">
-        <v>0.7557550207462792</v>
+        <v>0.40582688077236528</v>
       </c>
       <c r="D53">
-        <v>-5.1238667743663709E-2</v>
+        <v>-0.91845857068253434</v>
       </c>
       <c r="E53">
-        <v>-0.68951394760468809</v>
+        <v>-0.74799453248374326</v>
       </c>
       <c r="F53">
-        <v>0.27787994199278498</v>
+        <v>0.42095624041753738</v>
       </c>
       <c r="G53">
-        <v>0.81588639079457914</v>
+        <v>-0.73212156461708</v>
       </c>
       <c r="H53">
-        <v>-0.8806682167526535</v>
+        <v>0.40093730634838587</v>
       </c>
       <c r="I53">
-        <v>0.25835560709628075</v>
+        <v>-0.41878494765335045</v>
       </c>
       <c r="J53">
-        <v>0.8539500305278519</v>
+        <v>0.30883245693311356</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>0.24752806326731999</v>
+        <v>0.74780125331549563</v>
       </c>
       <c r="B54">
-        <v>0.31640117374051679</v>
+        <v>6.5202314153652061E-2</v>
       </c>
       <c r="C54">
-        <v>-0.76456681190125853</v>
+        <v>0.90909384814219862</v>
       </c>
       <c r="D54">
-        <v>0.635842043915685</v>
+        <v>-0.30619950610823454</v>
       </c>
       <c r="E54">
-        <v>3.5093550100160929E-2</v>
+        <v>-0.40700892097159808</v>
       </c>
       <c r="F54">
-        <v>-0.15477964043084413</v>
+        <v>0.75618772842165671</v>
       </c>
       <c r="G54">
-        <v>-0.58208011305816254</v>
+        <v>-0.52804506301595355</v>
       </c>
       <c r="H54">
-        <v>0.72019298791270658</v>
+        <v>-6.1884534261641727E-2</v>
       </c>
       <c r="I54">
-        <v>0.51583486281015023</v>
+        <v>-0.79627535303937214</v>
       </c>
       <c r="J54">
-        <v>-0.67445249466335411</v>
+        <v>-0.50650607391933755</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>0.66629890557835136</v>
+        <v>0.88298363685758363</v>
       </c>
       <c r="B55">
-        <v>-0.6662131186309882</v>
+        <v>0.89767226519854249</v>
       </c>
       <c r="C55">
-        <v>-0.15434753012412533</v>
+        <v>0.93855456891022826</v>
       </c>
       <c r="D55">
-        <v>-0.89939530865241435</v>
+        <v>-0.86604078666479578</v>
       </c>
       <c r="E55">
-        <v>-0.8062704406499448</v>
+        <v>-0.70745915087403788</v>
       </c>
       <c r="F55">
-        <v>0.756325639710131</v>
+        <v>0.73586674618944548</v>
       </c>
       <c r="G55">
-        <v>0.6493211919171058</v>
+        <v>0.44288024511989549</v>
       </c>
       <c r="H55">
-        <v>-0.98990617277457771</v>
+        <v>0.91149673929036867</v>
       </c>
       <c r="I55">
-        <v>-0.62004643251619262</v>
+        <v>-0.9702818122580873</v>
       </c>
       <c r="J55">
-        <v>0.87839591091103009</v>
+        <v>-0.97935654278856787</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>0.38500062425729242</v>
+        <v>-0.76296910736593904</v>
       </c>
       <c r="B56">
-        <v>0.37970843966057966</v>
+        <v>-0.57991065846432299</v>
       </c>
       <c r="C56">
-        <v>-6.4497188650056098E-3</v>
+        <v>-0.10571596572038085</v>
       </c>
       <c r="D56">
-        <v>8.302454237167764E-2</v>
+        <v>-0.38176546553773999</v>
       </c>
       <c r="E56">
-        <v>-0.80162362558576228</v>
+        <v>0.96850872302021052</v>
       </c>
       <c r="F56">
-        <v>-7.2471897441117983E-2</v>
+        <v>-0.85154455955878516</v>
       </c>
       <c r="G56">
-        <v>0.31927377501647136</v>
+        <v>0.98623747179679166</v>
       </c>
       <c r="H56">
-        <v>-0.83092613150952799</v>
+        <v>-0.84883833314465529</v>
       </c>
       <c r="I56">
-        <v>4.3266206998590635E-2</v>
+        <v>0.89151052084941396</v>
       </c>
       <c r="J56">
-        <v>0.88238735196227824</v>
+        <v>0.95212135018306698</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>-0.43517624644164188</v>
+        <v>-0.77730361502584988</v>
       </c>
       <c r="B57">
-        <v>0.65135454276429872</v>
+        <v>0.15551525599913954</v>
       </c>
       <c r="C57">
-        <v>-0.90725828114612184</v>
+        <v>-0.25460795723975516</v>
       </c>
       <c r="D57">
-        <v>0.70299332152364424</v>
+        <v>-0.78505898817304431</v>
       </c>
       <c r="E57">
-        <v>0.53850825795687574</v>
+        <v>3.144552623510076E-2</v>
       </c>
       <c r="F57">
-        <v>1.1894716024702979E-2</v>
+        <v>-0.4738625388906656</v>
       </c>
       <c r="G57">
-        <v>-0.24214260059779436</v>
+        <v>0.4241656196377766</v>
       </c>
       <c r="H57">
-        <v>0.94867032053349687</v>
+        <v>0.18558299220730368</v>
       </c>
       <c r="I57">
-        <v>0.77104060098645744</v>
+        <v>0.79838841551551476</v>
       </c>
       <c r="J57">
-        <v>-0.93878436348301553</v>
+        <v>-0.19229775220826034</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0.89610712386193425</v>
+        <v>0.79326028534590076</v>
       </c>
       <c r="B58">
-        <v>-0.68523636283073019</v>
+        <v>0.9434795107690418</v>
       </c>
       <c r="C58">
-        <v>0.31989638443296298</v>
+        <v>0.40377428285104866</v>
       </c>
       <c r="D58">
-        <v>-7.4295225827300665E-2</v>
+        <v>-4.506381855635179E-2</v>
       </c>
       <c r="E58">
-        <v>2.7889219091299971E-2</v>
+        <v>0.7116524614014994</v>
       </c>
       <c r="F58">
-        <v>-0.12556111987347743</v>
+        <v>0.57412749315944689</v>
       </c>
       <c r="G58">
-        <v>0.73669907372987464</v>
+        <v>-0.1182143310032307</v>
       </c>
       <c r="H58">
-        <v>-0.76379323022189749</v>
+        <v>0.5896003378195398</v>
       </c>
       <c r="I58">
-        <v>-0.68382167933630722</v>
+        <v>3.4289223730583795E-2</v>
       </c>
       <c r="J58">
-        <v>7.8305566594072673E-2</v>
+        <v>0.50070663679262106</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0.9242549087945181</v>
+        <v>0.40360571620644037</v>
       </c>
       <c r="B59">
-        <v>3.3968214201338963E-2</v>
+        <v>0.34721424094709918</v>
       </c>
       <c r="C59">
-        <v>1.7683582489178867E-2</v>
+        <v>0.10118205592643197</v>
       </c>
       <c r="D59">
-        <v>-0.56750660199485381</v>
+        <v>0.42048912455134335</v>
       </c>
       <c r="E59">
-        <v>-0.62004779510696217</v>
+        <v>0.83020633235269869</v>
       </c>
       <c r="F59">
-        <v>0.50362289669043603</v>
+        <v>-5.3109453473016335E-2</v>
       </c>
       <c r="G59">
-        <v>0.7420131797821774</v>
+        <v>0.36875931813802465</v>
       </c>
       <c r="H59">
-        <v>-0.86863062935492885</v>
+        <v>0.59771955298741131</v>
       </c>
       <c r="I59">
-        <v>0.61246621153024294</v>
+        <v>0.10255962408746179</v>
       </c>
       <c r="J59">
-        <v>0.35637677020963648</v>
+        <v>0.89585783171987854</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>-0.37839828923912683</v>
+        <v>0.72619191234890146</v>
       </c>
       <c r="B60">
-        <v>-0.3798414584578208</v>
+        <v>0.94867555753122135</v>
       </c>
       <c r="C60">
-        <v>-0.44251575673291121</v>
+        <v>0.95729747002432641</v>
       </c>
       <c r="D60">
-        <v>0.53421855921465156</v>
+        <v>0.38529309060503414</v>
       </c>
       <c r="E60">
-        <v>0.76410684951170171</v>
+        <v>-0.91576294787290091</v>
       </c>
       <c r="F60">
-        <v>-0.2308883184843939</v>
+        <v>0.97762580866253812</v>
       </c>
       <c r="G60">
-        <v>-0.1721147022866808</v>
+        <v>-0.63353182592887958</v>
       </c>
       <c r="H60">
-        <v>-0.18186876482006478</v>
+        <v>0.95959098456335878</v>
       </c>
       <c r="I60">
-        <v>-0.10145456359013313</v>
+        <v>-0.95126611478168133</v>
       </c>
       <c r="J60">
-        <v>-0.60261446411536268</v>
+        <v>-0.83540985979866567</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>0.19581784523738721</v>
+        <v>2.5191815855002752E-2</v>
       </c>
       <c r="B61">
-        <v>0.1004182873859301</v>
+        <v>0.38840020051851748</v>
       </c>
       <c r="C61">
-        <v>0.67035812836813402</v>
+        <v>0.92715068802753864</v>
       </c>
       <c r="D61">
-        <v>-0.55776962025037269</v>
+        <v>-0.31892551938500879</v>
       </c>
       <c r="E61">
-        <v>-0.30015983878843433</v>
+        <v>0.42294959378127817</v>
       </c>
       <c r="F61">
-        <v>-0.57151646319151128</v>
+        <v>0.59073505093925571</v>
       </c>
       <c r="G61">
-        <v>-0.16216292301382867</v>
+        <v>-0.73228773067875841</v>
       </c>
       <c r="H61">
-        <v>-0.45989767399000769</v>
+        <v>0.8051309606127296</v>
       </c>
       <c r="I61">
-        <v>-0.46934800125154419</v>
+        <v>0.24362725743332761</v>
       </c>
       <c r="J61">
-        <v>0.18805913403023539</v>
+        <v>0.47080614915239472</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>-0.82069178772287454</v>
+        <v>0.90435277447339157</v>
       </c>
       <c r="B62">
-        <v>0.34487373001638794</v>
+        <v>-0.5187432099344691</v>
       </c>
       <c r="C62">
-        <v>-0.81989212159391833</v>
+        <v>0.83058054886157129</v>
       </c>
       <c r="D62">
-        <v>0.21215079411620749</v>
+        <v>0.14921283830279145</v>
       </c>
       <c r="E62">
-        <v>0.32719630416177969</v>
+        <v>-0.17395510817132859</v>
       </c>
       <c r="F62">
-        <v>0.96956239701838809</v>
+        <v>0.60397057678775512</v>
       </c>
       <c r="G62">
-        <v>-0.22328096027854055</v>
+        <v>-0.15378253399366074</v>
       </c>
       <c r="H62">
-        <v>0.97507700631072625</v>
+        <v>0.53791379493424518</v>
       </c>
       <c r="I62">
-        <v>0.4036036884407454</v>
+        <v>-7.6838100230461392E-2</v>
       </c>
       <c r="J62">
-        <v>-0.6761155175492265</v>
+        <v>-0.71892472921693917</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>0.89078687927506917</v>
+        <v>-0.31901133414233218</v>
       </c>
       <c r="B63">
-        <v>-0.88943409096805959</v>
+        <v>-0.78430735412972896</v>
       </c>
       <c r="C63">
-        <v>0.24499220977924466</v>
+        <v>-0.64956239252308501</v>
       </c>
       <c r="D63">
-        <v>-0.93267480049150864</v>
+        <v>-0.85146734498811227</v>
       </c>
       <c r="E63">
-        <v>-0.90345708833871441</v>
+        <v>0.1741925592284253</v>
       </c>
       <c r="F63">
-        <v>-0.44282117578156832</v>
+        <v>-0.29063872954546588</v>
       </c>
       <c r="G63">
-        <v>0.86284613197980575</v>
+        <v>0.50432129033223583</v>
       </c>
       <c r="H63">
-        <v>-0.57778623394607831</v>
+        <v>-0.77391649248299688</v>
       </c>
       <c r="I63">
-        <v>-0.90813467309360663</v>
+        <v>0.26229683955639033</v>
       </c>
       <c r="J63">
-        <v>0.2706741955657434</v>
+        <v>0.24460419142584047</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>0.89742458138403047</v>
+        <v>0.63753288207421932</v>
       </c>
       <c r="B64">
-        <v>0.40708242277898776</v>
+        <v>0.22444248924416926</v>
       </c>
       <c r="C64">
-        <v>2.8860670878095972E-2</v>
+        <v>0.52160537964412645</v>
       </c>
       <c r="D64">
-        <v>0.23801995442650781</v>
+        <v>0.36386012386853112</v>
       </c>
       <c r="E64">
-        <v>0.47119132051740548</v>
+        <v>-0.106727633908137</v>
       </c>
       <c r="F64">
-        <v>-0.67163363306784929</v>
+        <v>3.3668945256767613E-2</v>
       </c>
       <c r="G64">
-        <v>-0.61829502240040568</v>
+        <v>9.6253371283106487E-2</v>
       </c>
       <c r="H64">
-        <v>0.81990690478687966</v>
+        <v>-0.48476055141927987</v>
       </c>
       <c r="I64">
-        <v>0.29533493363505731</v>
+        <v>-0.54983400673766913</v>
       </c>
       <c r="J64">
-        <v>-0.21006638051383306</v>
+        <v>-0.12771249787724975</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>0.74800722485033599</v>
+        <v>0.62387165964475799</v>
       </c>
       <c r="B65">
-        <v>-0.49951445155375751</v>
+        <v>0.9380662568491559</v>
       </c>
       <c r="C65">
-        <v>0.32823514931296849</v>
+        <v>0.65248251423387738</v>
       </c>
       <c r="D65">
-        <v>-0.80190882088510751</v>
+        <v>0.87343286774950013</v>
       </c>
       <c r="E65">
-        <v>0.13208461351386008</v>
+        <v>-0.79670169824977966</v>
       </c>
       <c r="F65">
-        <v>-0.51527976069047687</v>
+        <v>0.84911720310859118</v>
       </c>
       <c r="G65">
-        <v>0.17005432678609889</v>
+        <v>-0.63633515113745276</v>
       </c>
       <c r="H65">
-        <v>-0.23365869182400215</v>
+        <v>0.81876312177564459</v>
       </c>
       <c r="I65">
-        <v>-0.82078735486267795</v>
+        <v>-0.75340342705392283</v>
       </c>
       <c r="J65">
-        <v>1.9270775689584799E-2</v>
+        <v>-0.33033360200695255</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>-0.24399921400018637</v>
+        <v>0.34588238828979373</v>
       </c>
       <c r="B66">
-        <v>-0.10687236372938505</v>
+        <v>-0.36243182109976613</v>
       </c>
       <c r="C66">
-        <v>4.730065752224237E-2</v>
+        <v>5.796026804065231E-2</v>
       </c>
       <c r="D66">
-        <v>0.79639772402900166</v>
+        <v>-0.47689732299357201</v>
       </c>
       <c r="E66">
-        <v>0.87537584112126932</v>
+        <v>5.7347548639276574E-2</v>
       </c>
       <c r="F66">
-        <v>0.64347714489404706</v>
+        <v>-0.33279306110541779</v>
       </c>
       <c r="G66">
-        <v>0.37583010863353694</v>
+        <v>-0.50608416708708726</v>
       </c>
       <c r="H66">
-        <v>0.55189142435533545</v>
+        <v>-0.28814708582957571</v>
       </c>
       <c r="I66">
-        <v>0.54264437424854928</v>
+        <v>-0.12808459012326628</v>
       </c>
       <c r="J66">
-        <v>0.84349747384378804</v>
+        <v>-0.50971104227954556</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>0.59500149061163499</v>
+        <v>-0.27577633522946265</v>
       </c>
       <c r="B67">
-        <v>-0.69931070510486948</v>
+        <v>-0.63419271270152056</v>
       </c>
       <c r="C67">
-        <v>0.61190815785753239</v>
+        <v>-0.33002825293481403</v>
       </c>
       <c r="D67">
-        <v>-0.92546685502587545</v>
+        <v>-0.71213333166108173</v>
       </c>
       <c r="E67">
-        <v>-0.77813515604687555</v>
+        <v>-0.21798393605896974</v>
       </c>
       <c r="F67">
-        <v>0.59011337117072105</v>
+        <v>-0.81678756881518089</v>
       </c>
       <c r="G67">
-        <v>0.28186558030984354</v>
+        <v>-0.65256643386578572</v>
       </c>
       <c r="H67">
-        <v>-0.9025195247115283</v>
+        <v>-0.32780536938328297</v>
       </c>
       <c r="I67">
-        <v>-0.93987346907606528</v>
+        <v>0.86839031394729105</v>
       </c>
       <c r="J67">
-        <v>0.95760799454262124</v>
+        <v>0.80320764649435983</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>-0.28349978996724967</v>
+        <v>0.81445460338702658</v>
       </c>
       <c r="B68">
-        <v>0.43543307462153324</v>
+        <v>0.59091668206607895</v>
       </c>
       <c r="C68">
-        <v>-0.77666556565540268</v>
+        <v>1.411078416352649E-2</v>
       </c>
       <c r="D68">
-        <v>0.48546615270056531</v>
+        <v>0.78280210459455146</v>
       </c>
       <c r="E68">
-        <v>0.25391200224183791</v>
+        <v>-0.85302843774516512</v>
       </c>
       <c r="F68">
-        <v>-0.89758127885000383</v>
+        <v>0.90207628843311161</v>
       </c>
       <c r="G68">
-        <v>-0.57078838346225835</v>
+        <v>-0.8633631122237948</v>
       </c>
       <c r="H68">
-        <v>1.0342883947807973E-2</v>
+        <v>0.81512454610091178</v>
       </c>
       <c r="I68">
-        <v>-8.4675804605442953E-2</v>
+        <v>-0.20589501189559431</v>
       </c>
       <c r="J68">
-        <v>-0.80765499529380569</v>
+        <v>0.68663444533937479</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>0.82911645387756849</v>
+        <v>5.4984917729355258E-2</v>
       </c>
       <c r="B69">
-        <v>-0.88060209416529878</v>
+        <v>0.52366938959665155</v>
       </c>
       <c r="C69">
-        <v>-0.12485069782794062</v>
+        <v>-0.58945066177849359</v>
       </c>
       <c r="D69">
-        <v>-0.50851973592637989</v>
+        <v>0.69304876110438529</v>
       </c>
       <c r="E69">
-        <v>-4.6828101811076182E-2</v>
+        <v>0.32059280039804311</v>
       </c>
       <c r="F69">
-        <v>-0.29498540415109309</v>
+        <v>-0.79696929679344564</v>
       </c>
       <c r="G69">
-        <v>-0.65516825036107362</v>
+        <v>0.63069129049421424</v>
       </c>
       <c r="H69">
-        <v>-0.45542089830512811</v>
+        <v>-0.85164396953013832</v>
       </c>
       <c r="I69">
-        <v>-0.62523126254835026</v>
+        <v>0.9204701987396563</v>
       </c>
       <c r="J69">
-        <v>0.16612527333788485</v>
+        <v>0.69682584981425921</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>-0.45634445424079922</v>
+        <v>-0.42959533358636881</v>
       </c>
       <c r="B70">
-        <v>0.93185393467969468</v>
+        <v>-0.91433440677797195</v>
       </c>
       <c r="C70">
-        <v>-0.92308948393839219</v>
+        <v>-0.71840351298013116</v>
       </c>
       <c r="D70">
-        <v>0.95503982442337765</v>
+        <v>0.73940519050270859</v>
       </c>
       <c r="E70">
-        <v>0.9785476732470767</v>
+        <v>0.9433887676620234</v>
       </c>
       <c r="F70">
-        <v>-0.77934346390411291</v>
+        <v>-0.60878318437631473</v>
       </c>
       <c r="G70">
-        <v>-0.820441875850771</v>
+        <v>-0.10474300835130504</v>
       </c>
       <c r="H70">
-        <v>0.64653552013242233</v>
+        <v>-0.57630734402307759</v>
       </c>
       <c r="I70">
-        <v>0.85869497556817109</v>
+        <v>0.4086744010892005</v>
       </c>
       <c r="J70">
-        <v>-0.9814314833670067</v>
+        <v>0.87522646211919308</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>0.55674382317731386</v>
+        <v>0.92223081258861828</v>
       </c>
       <c r="B71">
-        <v>0.12464571209073046</v>
+        <v>-0.6188580335307301</v>
       </c>
       <c r="C71">
-        <v>-0.41761748432142604</v>
+        <v>-0.7075139524036278</v>
       </c>
       <c r="D71">
-        <v>-1.0293244558452888E-2</v>
+        <v>-0.29972793150260441</v>
       </c>
       <c r="E71">
-        <v>-0.13748903190876333</v>
+        <v>-0.27760691250504355</v>
       </c>
       <c r="F71">
-        <v>0.48954342003137752</v>
+        <v>0.23039082908313596</v>
       </c>
       <c r="G71">
-        <v>-0.52561289940589895</v>
+        <v>0.66986098703737029</v>
       </c>
       <c r="H71">
-        <v>-0.84841071622079856</v>
+        <v>-3.56680120126254E-2</v>
       </c>
       <c r="I71">
-        <v>-0.52787251873328866</v>
+        <v>-0.69341846630575754</v>
       </c>
       <c r="J71">
-        <v>0.73675437417534528</v>
+        <v>-0.74274070528635794</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>0.409009686614563</v>
+        <v>-0.91682813481876846</v>
       </c>
       <c r="B72">
-        <v>7.0163472033443516E-2</v>
+        <v>-0.83803781596074578</v>
       </c>
       <c r="C72">
-        <v>-0.64123308960119418</v>
+        <v>-0.16341045078473806</v>
       </c>
       <c r="D72">
-        <v>0.42639087819506655</v>
+        <v>-0.53413973613687005</v>
       </c>
       <c r="E72">
-        <v>0.28644717830520572</v>
+        <v>-0.38262095326604439</v>
       </c>
       <c r="F72">
-        <v>0.67886929579376332</v>
+        <v>0.14262031713024165</v>
       </c>
       <c r="G72">
-        <v>-0.76885628800155281</v>
+        <v>-0.58649732001358235</v>
       </c>
       <c r="H72">
-        <v>-0.19213067370351491</v>
+        <v>0.48283703853449494</v>
       </c>
       <c r="I72">
-        <v>0.38172393851032965</v>
+        <v>-0.36050288127755142</v>
       </c>
       <c r="J72">
-        <v>-0.32991838213458674</v>
+        <v>0.193389874152012</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>-0.42048990008686776</v>
+        <v>-0.55871754936442675</v>
       </c>
       <c r="B73">
-        <v>0.8345541918769861</v>
+        <v>-0.53879063471681488</v>
       </c>
       <c r="C73">
-        <v>-0.81579018941814774</v>
+        <v>-0.79893044153135662</v>
       </c>
       <c r="D73">
-        <v>0.96461811632974903</v>
+        <v>-0.60674232499967751</v>
       </c>
       <c r="E73">
-        <v>0.93723553305079332</v>
+        <v>-0.93581569273424559</v>
       </c>
       <c r="F73">
-        <v>-6.1862950413921231E-2</v>
+        <v>-0.32918249324540616</v>
       </c>
       <c r="G73">
-        <v>-0.49488844137102672</v>
+        <v>-0.19613279707249934</v>
       </c>
       <c r="H73">
-        <v>0.14804787723715485</v>
+        <v>7.7229059956914411E-3</v>
       </c>
       <c r="I73">
-        <v>0.9210265465848968</v>
+        <v>-0.74000552509024409</v>
       </c>
       <c r="J73">
-        <v>-0.75868779556649313</v>
+        <v>0.16069044341516411</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>-0.17664150480403173</v>
+        <v>0.76113003774652332</v>
       </c>
       <c r="B74">
-        <v>8.9009617366484953E-2</v>
+        <v>0.57964969836553337</v>
       </c>
       <c r="C74">
-        <v>-0.14368052053242089</v>
+        <v>0.74571185231977555</v>
       </c>
       <c r="D74">
-        <v>0.57472145539991604</v>
+        <v>0.34885349247876069</v>
       </c>
       <c r="E74">
-        <v>0.62701240757616206</v>
+        <v>-0.69477297845079899</v>
       </c>
       <c r="F74">
-        <v>-0.38587103201902612</v>
+        <v>0.78053895770856974</v>
       </c>
       <c r="G74">
-        <v>0.36145240671889384</v>
+        <v>-0.77740474055686204</v>
       </c>
       <c r="H74">
-        <v>0.86499818639357506</v>
+        <v>0.83388540159391611</v>
       </c>
       <c r="I74">
-        <v>-0.74650606862319735</v>
+        <v>-0.75128787245321438</v>
       </c>
       <c r="J74">
-        <v>0.29479453304957665</v>
+        <v>0.70453636748377524</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>-0.69427731848362206</v>
+        <v>-0.79051932517349099</v>
       </c>
       <c r="B75">
-        <v>-0.23056768382438148</v>
+        <v>-0.74308749882865321</v>
       </c>
       <c r="C75">
-        <v>0.28773869536373686</v>
+        <v>-0.65924433630995405</v>
       </c>
       <c r="D75">
-        <v>-0.82114396175905036</v>
+        <v>-0.29679890169236806</v>
       </c>
       <c r="E75">
-        <v>-0.85417187184883137</v>
+        <v>-0.29000789388558718</v>
       </c>
       <c r="F75">
-        <v>-0.97323884865743893</v>
+        <v>-0.92917783308227553</v>
       </c>
       <c r="G75">
-        <v>0.4838247309017234</v>
+        <v>-0.13463838480453419</v>
       </c>
       <c r="H75">
-        <v>-0.44164225980431115</v>
+        <v>-0.57147314296872587</v>
       </c>
       <c r="I75">
-        <v>0.18193657128239143</v>
+        <v>-0.46893288157206181</v>
       </c>
       <c r="J75">
-        <v>0.27404510205873017</v>
+        <v>0.55462951012253636</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>-2.693026238910913E-2</v>
+        <v>-0.94012397389755165</v>
       </c>
       <c r="B76">
-        <v>0.44568917061449137</v>
+        <v>-0.13435905826502703</v>
       </c>
       <c r="C76">
-        <v>0.94879920215057945</v>
+        <v>-0.80875372764837439</v>
       </c>
       <c r="D76">
-        <v>-0.27159301136715236</v>
+        <v>0.28012811312309832</v>
       </c>
       <c r="E76">
-        <v>-0.40793290832660595</v>
+        <v>0.12558700123531644</v>
       </c>
       <c r="F76">
-        <v>0.91129979602196198</v>
+        <v>5.9584566767251095E-2</v>
       </c>
       <c r="G76">
-        <v>0.69825758962381379</v>
+        <v>0.21751581506118328</v>
       </c>
       <c r="H76">
-        <v>-0.63874239158698054</v>
+        <v>-0.6941669009305812</v>
       </c>
       <c r="I76">
-        <v>7.1736291471398275E-2</v>
+        <v>0.42455741335533165</v>
       </c>
       <c r="J76">
-        <v>0.69581274309199859</v>
+        <v>0.47027521667126981</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>-0.94602278338493118</v>
+        <v>-0.46404502889546773</v>
       </c>
       <c r="B77">
-        <v>0.30259816404996803</v>
+        <v>0.99129142026757433</v>
       </c>
       <c r="C77">
-        <v>-0.95106161353015406</v>
+        <v>0.89377878261429222</v>
       </c>
       <c r="D77">
-        <v>2.5555589310801066E-2</v>
+        <v>-0.10770690578203412</v>
       </c>
       <c r="E77">
-        <v>0.89071886313719795</v>
+        <v>0.74046726133038254</v>
       </c>
       <c r="F77">
-        <v>5.770623667806344E-2</v>
+        <v>0.22430496521482754</v>
       </c>
       <c r="G77">
-        <v>-0.73526962772276483</v>
+        <v>3.330584764423572E-2</v>
       </c>
       <c r="H77">
-        <v>0.37754377927200711</v>
+        <v>0.7953938331887811</v>
       </c>
       <c r="I77">
-        <v>0.27945819353919155</v>
+        <v>6.2909584567054824E-2</v>
       </c>
       <c r="J77">
-        <v>-0.84821853139351433</v>
+        <v>-0.53133217250376041</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>0.93364398752612565</v>
+        <v>-0.18480110453964921</v>
       </c>
       <c r="B78">
-        <v>-0.99607650292177052</v>
+        <v>0.32361450135642389</v>
       </c>
       <c r="C78">
-        <v>0.87974240256863911</v>
+        <v>0.6256337022950742</v>
       </c>
       <c r="D78">
-        <v>-0.97544123054583842</v>
+        <v>0.883856047354453</v>
       </c>
       <c r="E78">
-        <v>-0.84920730378486464</v>
+        <v>0.52501368509302082</v>
       </c>
       <c r="F78">
-        <v>-0.97441604361948941</v>
+        <v>0.54674386328034652</v>
       </c>
       <c r="G78">
-        <v>0.79706045438045059</v>
+        <v>0.58612681866320315</v>
       </c>
       <c r="H78">
-        <v>-0.95599118552409412</v>
+        <v>-0.42544385789541395</v>
       </c>
       <c r="I78">
-        <v>-0.98360844356840238</v>
+        <v>-0.55357130563710166</v>
       </c>
       <c r="J78">
-        <v>0.84778530118584916</v>
+        <v>-0.23754549211869175</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>-0.95468912987572729</v>
+        <v>0.88306068600422483</v>
       </c>
       <c r="B79">
-        <v>0.97999262314904634</v>
+        <v>0.78259369851966798</v>
       </c>
       <c r="C79">
-        <v>-0.96235135870671618</v>
+        <v>0.93222236658889879</v>
       </c>
       <c r="D79">
-        <v>0.95425357755551465</v>
+        <v>-0.89803547352005841</v>
       </c>
       <c r="E79">
-        <v>0.94678295947626512</v>
+        <v>-0.87432725113722587</v>
       </c>
       <c r="F79">
-        <v>0.59304626200345834</v>
+        <v>0.53765273393021862</v>
       </c>
       <c r="G79">
-        <v>-0.98425283487169035</v>
+        <v>-0.9371705952096635</v>
       </c>
       <c r="H79">
-        <v>0.84800052769643153</v>
+        <v>0.92192178998510954</v>
       </c>
       <c r="I79">
-        <v>0.84996087672822818</v>
+        <v>-0.9803738012958606</v>
       </c>
       <c r="J79">
-        <v>-0.9001286304731092</v>
+        <v>-0.83985136237004432</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>0.92380514437891514</v>
+        <v>0.80737388458194559</v>
       </c>
       <c r="B80">
-        <v>-0.90398219607740593</v>
+        <v>-0.49798447099437382</v>
       </c>
       <c r="C80">
-        <v>7.9855959918363154E-2</v>
+        <v>0.1621425763538748</v>
       </c>
       <c r="D80">
-        <v>-0.2703153365667238</v>
+        <v>0.98987048998962435</v>
       </c>
       <c r="E80">
-        <v>0.5720050046403683</v>
+        <v>0.25215405890736409</v>
       </c>
       <c r="F80">
-        <v>0.33916211902169441</v>
+        <v>0.72377350045744071</v>
       </c>
       <c r="G80">
-        <v>0.42774536092830784</v>
+        <v>-0.6950092797959988</v>
       </c>
       <c r="H80">
-        <v>0.76045455105900428</v>
+        <v>0.34533177834180767</v>
       </c>
       <c r="I80">
-        <v>0.56773646538315681</v>
+        <v>-0.19883787787493334</v>
       </c>
       <c r="J80">
-        <v>-0.24820589645141211</v>
+        <v>0.72014078967687212</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>-4.4375894668625397E-2</v>
+        <v>-0.85857683614223634</v>
       </c>
       <c r="B81">
-        <v>3.331814194687243E-2</v>
+        <v>-0.4439036366924215</v>
       </c>
       <c r="C81">
-        <v>-0.42533467239591544</v>
+        <v>-0.52178324840368595</v>
       </c>
       <c r="D81">
-        <v>-0.29121325989705815</v>
+        <v>0.68500643888109625</v>
       </c>
       <c r="E81">
-        <v>-0.32897596541207902</v>
+        <v>0.57838718780808207</v>
       </c>
       <c r="F81">
-        <v>0.75437640563890473</v>
+        <v>-0.44357208544908272</v>
       </c>
       <c r="G81">
-        <v>-0.48625988284244892</v>
+        <v>-0.36392539411191238</v>
       </c>
       <c r="H81">
-        <v>-0.72077677429094489</v>
+        <v>-0.4918344014344268</v>
       </c>
       <c r="I81">
-        <v>-0.12512579134137664</v>
+        <v>-0.42122243090597145</v>
       </c>
       <c r="J81">
-        <v>0.47458901437750833</v>
+        <v>-0.39790831825700151</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>0.32530766855005655</v>
+        <v>-0.99242063788154489</v>
       </c>
       <c r="B82">
-        <v>-2.7869460571860169E-2</v>
+        <v>-0.98700600034990682</v>
       </c>
       <c r="C82">
-        <v>-0.44928111885608124</v>
+        <v>-0.98524447378162583</v>
       </c>
       <c r="D82">
-        <v>0.63469145079079747</v>
+        <v>-0.87646609201743975</v>
       </c>
       <c r="E82">
-        <v>0.54949610541374871</v>
+        <v>0.98265396832519647</v>
       </c>
       <c r="F82">
-        <v>-0.94106078039619545</v>
+        <v>-0.98234354571753102</v>
       </c>
       <c r="G82">
-        <v>-5.161510740266502E-2</v>
+        <v>0.73490477519878095</v>
       </c>
       <c r="H82">
-        <v>0.49811099838999351</v>
+        <v>-0.98872304571722158</v>
       </c>
       <c r="I82">
-        <v>-0.58346715844023955</v>
+        <v>0.9903079056074171</v>
       </c>
       <c r="J82">
-        <v>-0.12469642795300546</v>
+        <v>0.13724161193379769</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>-2.8662593886112218E-2</v>
+        <v>0.10968524532607947</v>
       </c>
       <c r="B83">
-        <v>0.24047722584909872</v>
+        <v>-0.20983686254898457</v>
       </c>
       <c r="C83">
-        <v>-0.88459345282358282</v>
+        <v>-0.15787972496198568</v>
       </c>
       <c r="D83">
-        <v>0.51969689497657556</v>
+        <v>0.83171947607881291</v>
       </c>
       <c r="E83">
-        <v>0.37170971865625757</v>
+        <v>0.84983985357801384</v>
       </c>
       <c r="F83">
-        <v>-0.55541929830582737</v>
+        <v>-8.6750763293880095E-2</v>
       </c>
       <c r="G83">
-        <v>-0.48768947615036623</v>
+        <v>0.73673871186021145</v>
       </c>
       <c r="H83">
-        <v>0.55685912374760804</v>
+        <v>-0.34929023327725811</v>
       </c>
       <c r="I83">
-        <v>0.26563430163507368</v>
+        <v>-0.65096955566856884</v>
       </c>
       <c r="J83">
-        <v>0.10962318692507202</v>
+        <v>0.49381329875843349</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0.38413697634026189</v>
+        <v>0.45237825594628184</v>
       </c>
       <c r="B84">
-        <v>-0.15495386749656673</v>
+        <v>-0.41654391864850654</v>
       </c>
       <c r="C84">
-        <v>4.8328412019502855E-3</v>
+        <v>-0.24056542204541229</v>
       </c>
       <c r="D84">
-        <v>-0.48195556835120801</v>
+        <v>-0.43893610584140391</v>
       </c>
       <c r="E84">
-        <v>0.12930684928628172</v>
+        <v>-0.53006899635542837</v>
       </c>
       <c r="F84">
-        <v>-0.86258780129358525</v>
+        <v>-6.4053100289449827E-2</v>
       </c>
       <c r="G84">
-        <v>0.5662741290409018</v>
+        <v>0.32227772556889084</v>
       </c>
       <c r="H84">
-        <v>0.35112176960938357</v>
+        <v>0.66325008733541435</v>
       </c>
       <c r="I84">
-        <v>-0.45578912743098071</v>
+        <v>2.5005259351080937E-2</v>
       </c>
       <c r="J84">
-        <v>-0.22268734683033831</v>
+        <v>7.4050317324194259E-2</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>0.78654764102743013</v>
+        <v>-9.1402723133016395E-2</v>
       </c>
       <c r="B85">
-        <v>-0.29529429800565732</v>
+        <v>0.31109363355082176</v>
       </c>
       <c r="C85">
-        <v>0.19747013308896147</v>
+        <v>-4.5229112814403845E-2</v>
       </c>
       <c r="D85">
-        <v>-0.45866261595209984</v>
+        <v>0.93619567616041599</v>
       </c>
       <c r="E85">
-        <v>-0.68735824670173373</v>
+        <v>-0.12603434502916197</v>
       </c>
       <c r="F85">
-        <v>0.97402957961680614</v>
+        <v>0.55023887128604476</v>
       </c>
       <c r="G85">
-        <v>0.19770939846143323</v>
+        <v>-0.6344916211522118</v>
       </c>
       <c r="H85">
-        <v>-0.85679012044357139</v>
+        <v>-0.18286010738529168</v>
       </c>
       <c r="I85">
-        <v>-0.51574904324426607</v>
+        <v>0.48590340002369486</v>
       </c>
       <c r="J85">
-        <v>0.78352793285866018</v>
+        <v>-0.79453724878185439</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>0.82362335899635941</v>
+        <v>0.58053728877231092</v>
       </c>
       <c r="B86">
-        <v>-0.80638281930695244</v>
+        <v>8.9205222510666149E-2</v>
       </c>
       <c r="C86">
-        <v>0.85968239880701991</v>
+        <v>0.29371503077734429</v>
       </c>
       <c r="D86">
-        <v>8.9939132244128528E-2</v>
+        <v>-0.72278071122080356</v>
       </c>
       <c r="E86">
-        <v>-0.70448387288715419</v>
+        <v>-0.63876361921101676</v>
       </c>
       <c r="F86">
-        <v>0.39298073623395058</v>
+        <v>-0.68929348234827859</v>
       </c>
       <c r="G86">
-        <v>0.53411137995309466</v>
+        <v>-0.583188161823194</v>
       </c>
       <c r="H86">
-        <v>-0.54482093305299495</v>
+        <v>0.39305478181428116</v>
       </c>
       <c r="I86">
-        <v>-0.92927970013748862</v>
+        <v>-0.73034707790990372</v>
       </c>
       <c r="J86">
-        <v>0.39845319441902799</v>
+        <v>-0.71933286778990413</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>-0.40113463874872329</v>
+        <v>0.79744139981290263</v>
       </c>
       <c r="B87">
-        <v>0.77933957964573097</v>
+        <v>0.90850763586340511</v>
       </c>
       <c r="C87">
-        <v>-0.10073843703220936</v>
+        <v>0.18670779637129464</v>
       </c>
       <c r="D87">
-        <v>7.5926766190611747E-4</v>
+        <v>-0.33097075418890498</v>
       </c>
       <c r="E87">
-        <v>0.96839427054844707</v>
+        <v>-0.84895201066922465</v>
       </c>
       <c r="F87">
-        <v>-0.21325108902391127</v>
+        <v>0.93243858884639697</v>
       </c>
       <c r="G87">
-        <v>-0.85474723585507428</v>
+        <v>-0.93177536239758796</v>
       </c>
       <c r="H87">
-        <v>0.96459086829584262</v>
+        <v>0.86986104672782716</v>
       </c>
       <c r="I87">
-        <v>0.38541079215663482</v>
+        <v>-0.86846241248260481</v>
       </c>
       <c r="J87">
-        <v>-0.80432914338703332</v>
+        <v>-0.95374228635041258</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0.17363758688327774</v>
+        <v>0.98144776095887643</v>
       </c>
       <c r="B88">
-        <v>0.74605439394746864</v>
+        <v>0.96314656531232912</v>
       </c>
       <c r="C88">
-        <v>-0.23578739952657604</v>
+        <v>0.52476508678516964</v>
       </c>
       <c r="D88">
-        <v>0.4154704951564156</v>
+        <v>0.74794633105237407</v>
       </c>
       <c r="E88">
-        <v>0.67105259526106953</v>
+        <v>-0.91890076536353893</v>
       </c>
       <c r="F88">
-        <v>-0.15806136475627022</v>
+        <v>0.99458502301238194</v>
       </c>
       <c r="G88">
-        <v>-0.33053468228036442</v>
+        <v>-0.79994151756272436</v>
       </c>
       <c r="H88">
-        <v>0.7695163158502013</v>
+        <v>0.9880460769721704</v>
       </c>
       <c r="I88">
-        <v>0.47824046248488211</v>
+        <v>-0.42524823418842694</v>
       </c>
       <c r="J88">
-        <v>-0.67743909346946285</v>
+        <v>-0.86488901988693601</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>-6.2744691660498297E-3</v>
+        <v>-0.46111775465360494</v>
       </c>
       <c r="B89">
-        <v>-0.37803070222271079</v>
+        <v>-0.27154809561129378</v>
       </c>
       <c r="C89">
-        <v>0.78447581998188587</v>
+        <v>-0.3800050072618672</v>
       </c>
       <c r="D89">
-        <v>-0.68768165085579658</v>
+        <v>0.28178593968008725</v>
       </c>
       <c r="E89">
-        <v>-0.20211156699930405</v>
+        <v>0.66433978824142559</v>
       </c>
       <c r="F89">
-        <v>-0.29139641825838053</v>
+        <v>-0.4029588713685941</v>
       </c>
       <c r="G89">
-        <v>0.1338392189718049</v>
+        <v>0.70124988495295359</v>
       </c>
       <c r="H89">
-        <v>-0.51795058826338514</v>
+        <v>0.40096467165097738</v>
       </c>
       <c r="I89">
-        <v>-0.2389700382625736</v>
+        <v>0.67447344794749375</v>
       </c>
       <c r="J89">
-        <v>0.69597720680276931</v>
+        <v>0.46527945522930142</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0.51670901666961011</v>
+        <v>0.4302026293247776</v>
       </c>
       <c r="B90">
-        <v>-0.84925319955130674</v>
+        <v>0.4849453332764414</v>
       </c>
       <c r="C90">
-        <v>0.26159918885342021</v>
+        <v>0.83004860486597887</v>
       </c>
       <c r="D90">
-        <v>-0.9194794605524117</v>
+        <v>-0.58441316403215537</v>
       </c>
       <c r="E90">
-        <v>-0.94129592344332247</v>
+        <v>-0.66573330963675903</v>
       </c>
       <c r="F90">
-        <v>0.62531723140648821</v>
+        <v>0.93341156928392077</v>
       </c>
       <c r="G90">
-        <v>0.947304623363039</v>
+        <v>-0.79384217188090722</v>
       </c>
       <c r="H90">
-        <v>-0.37948811064817528</v>
+        <v>0.71116652152166238</v>
       </c>
       <c r="I90">
-        <v>-0.93749305756787416</v>
+        <v>-0.64675756522776884</v>
       </c>
       <c r="J90">
-        <v>0.8683378360436822</v>
+        <v>-0.21999415070045819</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>-0.43328222377125525</v>
+        <v>0.80757573062395671</v>
       </c>
       <c r="B91">
-        <v>0.68816153660190138</v>
+        <v>0.18275361617131097</v>
       </c>
       <c r="C91">
-        <v>-0.56421399026801977</v>
+        <v>0.65028281989987324</v>
       </c>
       <c r="D91">
-        <v>0.6629880983082691</v>
+        <v>-0.28609696337209123</v>
       </c>
       <c r="E91">
-        <v>0.65653141094128564</v>
+        <v>-0.52866645194451689</v>
       </c>
       <c r="F91">
-        <v>-0.77863957905019976</v>
+        <v>0.67657904623578591</v>
       </c>
       <c r="G91">
-        <v>-0.93441062934971231</v>
+        <v>0.90990952572994699</v>
       </c>
       <c r="H91">
-        <v>0.43838702407685914</v>
+        <v>0.90537976228358574</v>
       </c>
       <c r="I91">
-        <v>0.70598443400993083</v>
+        <v>-0.17999974015687994</v>
       </c>
       <c r="J91">
-        <v>-0.48636885653614764</v>
+        <v>0.89611095917997152</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>0.10787756318366526</v>
+        <v>-0.70062278863370298</v>
       </c>
       <c r="B92">
-        <v>-0.75439496302332554</v>
+        <v>-0.58239825157661684</v>
       </c>
       <c r="C92">
-        <v>0.79415691098031549</v>
+        <v>-0.92439850164838289</v>
       </c>
       <c r="D92">
-        <v>-0.89122300174639668</v>
+        <v>-0.84030982627378759</v>
       </c>
       <c r="E92">
-        <v>-0.90962355794858907</v>
+        <v>-0.28942511585908909</v>
       </c>
       <c r="F92">
-        <v>-0.14463647765240964</v>
+        <v>-0.84371446386677851</v>
       </c>
       <c r="G92">
-        <v>0.94365153319779549</v>
+        <v>0.10325434732835115</v>
       </c>
       <c r="H92">
-        <v>-0.84790053967158308</v>
+        <v>-0.87658082631981304</v>
       </c>
       <c r="I92">
-        <v>-0.90178895896479971</v>
+        <v>0.7166468083369395</v>
       </c>
       <c r="J92">
-        <v>-0.36795369421648139</v>
+        <v>0.88586182205070962</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>-2.1998907401592421E-2</v>
+        <v>-0.24760349227236406</v>
       </c>
       <c r="B93">
-        <v>-0.39603362433656281</v>
+        <v>0.70417093833261046</v>
       </c>
       <c r="C93">
-        <v>0.4411789535689935</v>
+        <v>0.83169109182004131</v>
       </c>
       <c r="D93">
-        <v>-0.87265621951484607</v>
+        <v>-0.87554359386510383</v>
       </c>
       <c r="E93">
-        <v>-0.2291503209177734</v>
+        <v>-0.95007733567333408</v>
       </c>
       <c r="F93">
-        <v>3.4914262543450031E-3</v>
+        <v>0.33292827878199244</v>
       </c>
       <c r="G93">
-        <v>0.25690590200095575</v>
+        <v>-0.75163959256209933</v>
       </c>
       <c r="H93">
-        <v>-0.73886745658424335</v>
+        <v>0.65525607888151616</v>
       </c>
       <c r="I93">
-        <v>-0.73803496619811593</v>
+        <v>-0.70551347790641528</v>
       </c>
       <c r="J93">
-        <v>0.30746733541171212</v>
+        <v>-0.98728547853547099</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>-0.55679885073188506</v>
+        <v>-0.57577615953378936</v>
       </c>
       <c r="B94">
-        <v>-0.3694832766717987</v>
+        <v>-0.438372801187076</v>
       </c>
       <c r="C94">
-        <v>-0.75635632990546997</v>
+        <v>-0.69121662677898787</v>
       </c>
       <c r="D94">
-        <v>-0.81839684543436575</v>
+        <v>-0.14735703793475594</v>
       </c>
       <c r="E94">
-        <v>-0.47405379205913978</v>
+        <v>-0.36800657871017195</v>
       </c>
       <c r="F94">
-        <v>-0.59990746002852713</v>
+        <v>-0.13475094716832656</v>
       </c>
       <c r="G94">
-        <v>-0.25835227635817537</v>
+        <v>-0.75824153187622323</v>
       </c>
       <c r="H94">
-        <v>-0.43072942907641754</v>
+        <v>0.13846597241062333</v>
       </c>
       <c r="I94">
-        <v>-0.33439874767525313</v>
+        <v>0.48678872944077639</v>
       </c>
       <c r="J94">
-        <v>0.19758594479986372</v>
+        <v>-0.89169943469286361</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>0.90376283738883512</v>
+        <v>4.1483564032397072E-2</v>
       </c>
       <c r="B95">
-        <v>-0.82497119667666263</v>
+        <v>-0.43170635105814259</v>
       </c>
       <c r="C95">
-        <v>0.82240998054414316</v>
+        <v>-0.22293810275537479</v>
       </c>
       <c r="D95">
-        <v>-0.31341490185123105</v>
+        <v>0.68400168190758837</v>
       </c>
       <c r="E95">
-        <v>-0.95106165841752632</v>
+        <v>-0.41443679713427517</v>
       </c>
       <c r="F95">
-        <v>0.53771937979873463</v>
+        <v>-0.56896302581776681</v>
       </c>
       <c r="G95">
-        <v>0.58679265880263154</v>
+        <v>0.13984111119342563</v>
       </c>
       <c r="H95">
-        <v>-0.8810477811595655</v>
+        <v>-0.7806797105705392</v>
       </c>
       <c r="I95">
-        <v>-0.61076551048083394</v>
+        <v>0.53464767996496554</v>
       </c>
       <c r="J95">
-        <v>0.90045635176232619</v>
+        <v>-3.2627621296688836E-2</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>-0.98745580326306981</v>
+        <v>-0.86562322096183286</v>
       </c>
       <c r="B96">
-        <v>0.51628446460098321</v>
+        <v>-0.82623970131162183</v>
       </c>
       <c r="C96">
-        <v>-0.21099246835218852</v>
+        <v>-0.68980125565648098</v>
       </c>
       <c r="D96">
-        <v>0.5683406768894611</v>
+        <v>-0.80130672177485296</v>
       </c>
       <c r="E96">
-        <v>-3.2105213075875744E-2</v>
+        <v>0.86350680924619228</v>
       </c>
       <c r="F96">
-        <v>-0.4147276112968647</v>
+        <v>-0.73266008373513902</v>
       </c>
       <c r="G96">
-        <v>-0.85403134575832917</v>
+        <v>-0.85738414384243278</v>
       </c>
       <c r="H96">
-        <v>0.36093379464582825</v>
+        <v>-0.67297110859568676</v>
       </c>
       <c r="I96">
-        <v>0.52196429110221421</v>
+        <v>0.59203186212724601</v>
       </c>
       <c r="J96">
-        <v>-0.7993825048700991</v>
+        <v>-0.52957432927781567</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>0.70506232416045256</v>
+        <v>-0.50729603824867409</v>
       </c>
       <c r="B97">
-        <v>-0.88072845357215113</v>
+        <v>-0.12740519423573393</v>
       </c>
       <c r="C97">
-        <v>0.93387677578020434</v>
+        <v>-0.44231018822369328</v>
       </c>
       <c r="D97">
-        <v>-0.62365722766910747</v>
+        <v>0.94781547362615781</v>
       </c>
       <c r="E97">
-        <v>0.40231362475522808</v>
+        <v>0.39777342920958603</v>
       </c>
       <c r="F97">
-        <v>0.89985043457967029</v>
+        <v>-0.59779251782022758</v>
       </c>
       <c r="G97">
-        <v>0.9146401718064594</v>
+        <v>-0.38319415115743999</v>
       </c>
       <c r="H97">
-        <v>0.82117567078262488</v>
+        <v>-0.82675564353561581</v>
       </c>
       <c r="I97">
-        <v>-0.79300024025267302</v>
+        <v>-0.54476539768995713</v>
       </c>
       <c r="J97">
-        <v>0.76081044812996912</v>
+        <v>-0.55129973499521501</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>-0.94120325371166103</v>
+        <v>-3.1634155336393778E-2</v>
       </c>
       <c r="B98">
-        <v>-0.46627384896903634</v>
+        <v>0.63191871383353393</v>
       </c>
       <c r="C98">
-        <v>0.74955105493983631</v>
+        <v>0.52042619331549556</v>
       </c>
       <c r="D98">
-        <v>-6.2428427367888905E-3</v>
+        <v>-0.65392317424613267</v>
       </c>
       <c r="E98">
-        <v>-0.42825922805829081</v>
+        <v>0.38781242260507831</v>
       </c>
       <c r="F98">
-        <v>0.11325816224336344</v>
+        <v>0.41721693772473833</v>
       </c>
       <c r="G98">
-        <v>-0.16367997716206953</v>
+        <v>-0.24196512699676626</v>
       </c>
       <c r="H98">
-        <v>0.36839832973327508</v>
+        <v>0.8267643367936568</v>
       </c>
       <c r="I98">
-        <v>0.84450013179506045</v>
+        <v>-0.88804195269489383</v>
       </c>
       <c r="J98">
-        <v>-0.34079064833031547</v>
+        <v>-0.35109994396445998</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>-0.96785399641028746</v>
+        <v>0.44669341070222324</v>
       </c>
       <c r="B99">
-        <v>0.4434090832277276</v>
+        <v>0.89607360469466601</v>
       </c>
       <c r="C99">
-        <v>-0.85495684391587667</v>
+        <v>0.96760417964636192</v>
       </c>
       <c r="D99">
-        <v>0.76965564521596053</v>
+        <v>0.95449093762105419</v>
       </c>
       <c r="E99">
-        <v>0.89292718702331664</v>
+        <v>-0.3485684264726997</v>
       </c>
       <c r="F99">
-        <v>-0.22017611459007091</v>
+        <v>0.91248342534647509</v>
       </c>
       <c r="G99">
-        <v>-0.45504994575647911</v>
+        <v>-0.88628336904688876</v>
       </c>
       <c r="H99">
-        <v>0.8928909820348665</v>
+        <v>0.7330618355224886</v>
       </c>
       <c r="I99">
-        <v>0.96551816307418559</v>
+        <v>-0.98907094530204787</v>
       </c>
       <c r="J99">
-        <v>-0.65664049644681788</v>
+        <v>-0.98791061152733894</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>-0.97686003686564415</v>
+        <v>0.19694235684470066</v>
       </c>
       <c r="B100">
-        <v>-0.19617455368886674</v>
+        <v>-0.28965559163792542</v>
       </c>
       <c r="C100">
-        <v>-0.80695823849022896</v>
+        <v>-0.84040889920945916</v>
       </c>
       <c r="D100">
-        <v>0.62332706612787514</v>
+        <v>-0.58080342259768925</v>
       </c>
       <c r="E100">
-        <v>0.79082634379046346</v>
+        <v>-0.36520915410310012</v>
       </c>
       <c r="F100">
-        <v>-0.73894227682525548</v>
+        <v>-0.65325240523188677</v>
       </c>
       <c r="G100">
-        <v>-0.11247412014738846</v>
+        <v>0.98591294147359954</v>
       </c>
       <c r="H100">
-        <v>0.74858630228639467</v>
+        <v>2.1048643125647949E-2</v>
       </c>
       <c r="I100">
-        <v>0.82976091799839602</v>
+        <v>0.87007334226768185</v>
       </c>
       <c r="J100">
-        <v>-0.92951135453384803</v>
+        <v>0.73286243967763476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit results so far
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_3_5.xlsx
+++ b/TestMNIST/MatlabCodes/final_3_5.xlsx
@@ -411,3202 +411,3202 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.47893404952806951</v>
+        <v>-0.68675714654297848</v>
       </c>
       <c r="B1">
-        <v>0.63451543743998229</v>
+        <v>0.5892830240401985</v>
       </c>
       <c r="C1">
-        <v>-0.49675148066890196</v>
+        <v>-0.84404812117587769</v>
       </c>
       <c r="D1">
-        <v>1.7271370535973621E-2</v>
+        <v>-0.92784380605611683</v>
       </c>
       <c r="E1">
-        <v>0.69612709297261643</v>
+        <v>-0.78362773510218275</v>
       </c>
       <c r="F1">
-        <v>0.32049810550772623</v>
+        <v>0.48737516110988316</v>
       </c>
       <c r="G1">
-        <v>-0.84456722775048443</v>
+        <v>0.33483937970102279</v>
       </c>
       <c r="H1">
-        <v>0.22611249960817736</v>
+        <v>-0.51200107299231479</v>
       </c>
       <c r="I1">
-        <v>0.68406912221118121</v>
+        <v>-0.11853310262447851</v>
       </c>
       <c r="J1">
-        <v>0.17200321076764863</v>
+        <v>-0.3276895950011568</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.39005417806237358</v>
+        <v>0.75970289754169329</v>
       </c>
       <c r="B2">
-        <v>0.88326701081561387</v>
+        <v>-0.11454807661416337</v>
       </c>
       <c r="C2">
-        <v>-5.0865853260672847E-2</v>
+        <v>-0.70881202505283769</v>
       </c>
       <c r="D2">
-        <v>-0.79883760133551973</v>
+        <v>-0.4087163383749014</v>
       </c>
       <c r="E2">
-        <v>0.37531568905468743</v>
+        <v>-0.30225722113986597</v>
       </c>
       <c r="F2">
-        <v>0.34451176425764551</v>
+        <v>-0.92242980378140293</v>
       </c>
       <c r="G2">
-        <v>0.40876072575518102</v>
+        <v>-0.52864632366270103</v>
       </c>
       <c r="H2">
-        <v>-0.38377860959800508</v>
+        <v>6.470176399966926E-2</v>
       </c>
       <c r="I2">
-        <v>-0.3892665034175527</v>
+        <v>-0.70289868471725647</v>
       </c>
       <c r="J2">
-        <v>-0.88932151400424275</v>
+        <v>-0.11484750634407831</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-0.59258690998774677</v>
+        <v>-0.86784397154399495</v>
       </c>
       <c r="B3">
-        <v>-0.85339266815549519</v>
+        <v>0.3055735283401167</v>
       </c>
       <c r="C3">
-        <v>-0.89845758438538315</v>
+        <v>0.94978366682590432</v>
       </c>
       <c r="D3">
-        <v>-0.40255528490340459</v>
+        <v>0.40453160623316331</v>
       </c>
       <c r="E3">
-        <v>-0.35497734002538017</v>
+        <v>-0.27767561394126178</v>
       </c>
       <c r="F3">
-        <v>-0.3733309206200458</v>
+        <v>-0.10112125016760576</v>
       </c>
       <c r="G3">
-        <v>0.73044647005154562</v>
+        <v>0.75013179861892754</v>
       </c>
       <c r="H3">
-        <v>-2.5055163475082198E-2</v>
+        <v>-0.40901721593004736</v>
       </c>
       <c r="I3">
-        <v>0.47631817328723181</v>
+        <v>-0.42212503510982324</v>
       </c>
       <c r="J3">
-        <v>0.64036484848520858</v>
+        <v>-0.65828788779542036</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-0.97648687881693563</v>
+        <v>0.2336591073997201</v>
       </c>
       <c r="B4">
-        <v>-0.84994126776468448</v>
+        <v>-0.54799433237204287</v>
       </c>
       <c r="C4">
-        <v>-0.97836951975356767</v>
+        <v>0.96364843931288657</v>
       </c>
       <c r="D4">
-        <v>0.67289284429168694</v>
+        <v>0.84984462396097316</v>
       </c>
       <c r="E4">
-        <v>0.99103932217584412</v>
+        <v>-0.64418883459378207</v>
       </c>
       <c r="F4">
-        <v>-0.94813505263717768</v>
+        <v>-0.43277967343214485</v>
       </c>
       <c r="G4">
-        <v>0.90521530230868086</v>
+        <v>0.59554834111282229</v>
       </c>
       <c r="H4">
-        <v>-0.95565204878822851</v>
+        <v>0.32231881472271456</v>
       </c>
       <c r="I4">
-        <v>0.98900453855010162</v>
+        <v>-0.41842868989126852</v>
       </c>
       <c r="J4">
-        <v>0.85097320760403516</v>
+        <v>0.29604865543719544</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.17588323719132051</v>
+        <v>-0.60257023153652112</v>
       </c>
       <c r="B5">
-        <v>-0.1088086451260713</v>
+        <v>-3.6309773090370118E-2</v>
       </c>
       <c r="C5">
-        <v>0.81226871005839762</v>
+        <v>-0.90011320718175758</v>
       </c>
       <c r="D5">
-        <v>-0.84959258307283814</v>
+        <v>0.86420425279583502</v>
       </c>
       <c r="E5">
-        <v>-0.8632150354334035</v>
+        <v>-0.6026065841796836</v>
       </c>
       <c r="F5">
-        <v>0.61178450740822754</v>
+        <v>0.42624258835384043</v>
       </c>
       <c r="G5">
-        <v>-0.80816391821990252</v>
+        <v>-0.20533370505948956</v>
       </c>
       <c r="H5">
-        <v>-0.1802265086493271</v>
+        <v>0.69740714169959694</v>
       </c>
       <c r="I5">
-        <v>-0.84700010210732146</v>
+        <v>0.40404608492701388</v>
       </c>
       <c r="J5">
-        <v>-0.72882910872527495</v>
+        <v>-0.22790570580149028</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-0.34576730431727254</v>
+        <v>-0.37583454264501182</v>
       </c>
       <c r="B6">
-        <v>-0.58030147343862537</v>
+        <v>0.27245216889457657</v>
       </c>
       <c r="C6">
-        <v>-0.41222492973943664</v>
+        <v>-0.84608723153196375</v>
       </c>
       <c r="D6">
-        <v>0.84968514129805306</v>
+        <v>0.42758076837298287</v>
       </c>
       <c r="E6">
-        <v>0.76611774982081471</v>
+        <v>0.56934340390160276</v>
       </c>
       <c r="F6">
-        <v>-0.17807090701207187</v>
+        <v>0.61978655218030176</v>
       </c>
       <c r="G6">
-        <v>-0.12872843460168829</v>
+        <v>-0.2038158242563779</v>
       </c>
       <c r="H6">
-        <v>-1.7900483534769873E-2</v>
+        <v>0.37443817122678613</v>
       </c>
       <c r="I6">
-        <v>-0.94019062053388369</v>
+        <v>0.16411732983029567</v>
       </c>
       <c r="J6">
-        <v>-0.76819604475055847</v>
+        <v>-0.90742029419640657</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-0.163089227686989</v>
+        <v>0.39445120850161097</v>
       </c>
       <c r="B7">
-        <v>0.14833309868032829</v>
+        <v>0.92444449569735609</v>
       </c>
       <c r="C7">
-        <v>-0.45950599800763048</v>
+        <v>-0.396984458050261</v>
       </c>
       <c r="D7">
-        <v>0.93678515034370824</v>
+        <v>-0.91824339497411378</v>
       </c>
       <c r="E7">
-        <v>0.65919594190944553</v>
+        <v>-0.74411062731049671</v>
       </c>
       <c r="F7">
-        <v>-0.95163644591905361</v>
+        <v>-0.40624542913596201</v>
       </c>
       <c r="G7">
-        <v>0.28088297296877868</v>
+        <v>0.10299699325606697</v>
       </c>
       <c r="H7">
-        <v>2.2837918713293185E-3</v>
+        <v>0.84720808996940233</v>
       </c>
       <c r="I7">
-        <v>0.36818720054135412</v>
+        <v>0.93308135574363749</v>
       </c>
       <c r="J7">
-        <v>0.99256228568399485</v>
+        <v>-0.75563039015505395</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-0.89343183791187308</v>
+        <v>8.7995469400324947E-2</v>
       </c>
       <c r="B8">
-        <v>0.37030933939666877</v>
+        <v>-0.54756761352518113</v>
       </c>
       <c r="C8">
-        <v>-0.73885589101648164</v>
+        <v>-0.30181377084141242</v>
       </c>
       <c r="D8">
-        <v>0.97234143985759791</v>
+        <v>-0.53883813984133977</v>
       </c>
       <c r="E8">
-        <v>0.85913842221938763</v>
+        <v>-0.32162967785595237</v>
       </c>
       <c r="F8">
-        <v>-0.65670728530379219</v>
+        <v>-0.49005194813186576</v>
       </c>
       <c r="G8">
-        <v>0.92525826396407185</v>
+        <v>-0.46386352517634694</v>
       </c>
       <c r="H8">
-        <v>-0.8830280988999939</v>
+        <v>0.57186236132782131</v>
       </c>
       <c r="I8">
-        <v>0.33844916059263058</v>
+        <v>9.6204737229435653E-3</v>
       </c>
       <c r="J8">
-        <v>-0.43017242880637285</v>
+        <v>0.81101222200952061</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-0.60505711859959566</v>
+        <v>0.69597104150757039</v>
       </c>
       <c r="B9">
-        <v>-0.88332283711139403</v>
+        <v>-0.50960135469433521</v>
       </c>
       <c r="C9">
-        <v>-0.72533079614754647</v>
+        <v>-8.005882305895401E-2</v>
       </c>
       <c r="D9">
-        <v>0.95397910894923155</v>
+        <v>-0.76611841354011956</v>
       </c>
       <c r="E9">
-        <v>0.71871812152518533</v>
+        <v>-0.40996231797932753</v>
       </c>
       <c r="F9">
-        <v>-0.78539168254933012</v>
+        <v>0.3106528721107214</v>
       </c>
       <c r="G9">
-        <v>0.95145693655511765</v>
+        <v>-0.44886376902478486</v>
       </c>
       <c r="H9">
-        <v>-0.71706825646575789</v>
+        <v>0.13015895683999354</v>
       </c>
       <c r="I9">
-        <v>0.50525338926587049</v>
+        <v>-1.111395816004186E-2</v>
       </c>
       <c r="J9">
-        <v>0.17196329795124077</v>
+        <v>4.4276801789452147E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.34457806210266129</v>
+        <v>-0.92076948259432745</v>
       </c>
       <c r="B10">
-        <v>-0.87977458492194871</v>
+        <v>0.19381187601124564</v>
       </c>
       <c r="C10">
-        <v>-0.50851490206056571</v>
+        <v>0.75745626763549012</v>
       </c>
       <c r="D10">
-        <v>-0.97060797773494778</v>
+        <v>-0.79669341199743027</v>
       </c>
       <c r="E10">
-        <v>-4.5090659235929031E-2</v>
+        <v>8.2025677886430379E-2</v>
       </c>
       <c r="F10">
-        <v>0.23139288801917895</v>
+        <v>8.8065787905987652E-2</v>
       </c>
       <c r="G10">
-        <v>-7.5098709924474677E-2</v>
+        <v>-0.51363222101053185</v>
       </c>
       <c r="H10">
-        <v>-0.3439447431327623</v>
+        <v>-0.9134797452864567</v>
       </c>
       <c r="I10">
-        <v>0.51568989224409789</v>
+        <v>-0.2501327245275744</v>
       </c>
       <c r="J10">
-        <v>0.57526398316566285</v>
+        <v>0.41742694511524309</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-0.87544897220282758</v>
+        <v>-0.92245023395702996</v>
       </c>
       <c r="B11">
-        <v>-0.59358959047151916</v>
+        <v>-0.53555850020043572</v>
       </c>
       <c r="C11">
-        <v>-0.73124753008550325</v>
+        <v>9.0119993773874377E-2</v>
       </c>
       <c r="D11">
-        <v>-0.80410182353173454</v>
+        <v>-0.2946165618151137</v>
       </c>
       <c r="E11">
-        <v>0.87356579819645352</v>
+        <v>-0.2613761660080397</v>
       </c>
       <c r="F11">
-        <v>-0.96333655872397639</v>
+        <v>0.69813882129271865</v>
       </c>
       <c r="G11">
-        <v>0.96340543606581175</v>
+        <v>0.7266250037399381</v>
       </c>
       <c r="H11">
-        <v>-0.94483968801061846</v>
+        <v>0.20513676821101129</v>
       </c>
       <c r="I11">
-        <v>0.95195513484850469</v>
+        <v>0.61325373850245035</v>
       </c>
       <c r="J11">
-        <v>0.78377823133255875</v>
+        <v>0.40594560052728962</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-0.72329012291404815</v>
+        <v>0.60615556508677648</v>
       </c>
       <c r="B12">
-        <v>0.40080780495943591</v>
+        <v>-0.84123126617054456</v>
       </c>
       <c r="C12">
-        <v>-0.65137771636958286</v>
+        <v>0.31408025316684823</v>
       </c>
       <c r="D12">
-        <v>0.92390036458762226</v>
+        <v>7.9460028014265841E-2</v>
       </c>
       <c r="E12">
-        <v>0.32135889180659971</v>
+        <v>-0.7264973002793802</v>
       </c>
       <c r="F12">
-        <v>-0.85089743504218562</v>
+        <v>-0.8536462119025805</v>
       </c>
       <c r="G12">
-        <v>0.16696896600215486</v>
+        <v>0.73103042889256276</v>
       </c>
       <c r="H12">
-        <v>-0.51014637625585968</v>
+        <v>-0.42527283929202425</v>
       </c>
       <c r="I12">
-        <v>9.3335822625785034E-2</v>
+        <v>-0.88884338140363695</v>
       </c>
       <c r="J12">
-        <v>-0.11346734656588442</v>
+        <v>0.31155569583364057</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-0.78308342548456245</v>
+        <v>-0.4986314648067246</v>
       </c>
       <c r="B13">
-        <v>0.13037580542269683</v>
+        <v>-0.42326340200816431</v>
       </c>
       <c r="C13">
-        <v>8.6974435596050087E-2</v>
+        <v>0.82002241675873699</v>
       </c>
       <c r="D13">
-        <v>0.53177351472246992</v>
+        <v>-0.39975589534958739</v>
       </c>
       <c r="E13">
-        <v>0.84333410013780807</v>
+        <v>-0.4930478898128321</v>
       </c>
       <c r="F13">
-        <v>-0.87544186819285486</v>
+        <v>-0.8465452078969985</v>
       </c>
       <c r="G13">
-        <v>0.85597685091649511</v>
+        <v>-0.24452399485670204</v>
       </c>
       <c r="H13">
-        <v>-5.1679722627040979E-2</v>
+        <v>-0.35099889028428882</v>
       </c>
       <c r="I13">
-        <v>0.87893867564211736</v>
+        <v>-0.46913337655766835</v>
       </c>
       <c r="J13">
-        <v>0.63658239527184701</v>
+        <v>0.62776478046550555</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.83971482032943923</v>
+        <v>0.95158864761739004</v>
       </c>
       <c r="B14">
-        <v>-0.16079677713976273</v>
+        <v>0.79849537956030359</v>
       </c>
       <c r="C14">
-        <v>0.88220010627261547</v>
+        <v>1.5765513196459559E-2</v>
       </c>
       <c r="D14">
-        <v>-0.82384521991105641</v>
+        <v>0.75240820183015322</v>
       </c>
       <c r="E14">
-        <v>-0.54195274743211974</v>
+        <v>-0.80977222648355773</v>
       </c>
       <c r="F14">
-        <v>0.38285759268908237</v>
+        <v>0.2109301543522123</v>
       </c>
       <c r="G14">
-        <v>0.3413471440989303</v>
+        <v>0.39227053904551512</v>
       </c>
       <c r="H14">
-        <v>0.23474722517588983</v>
+        <v>-0.1392714021438452</v>
       </c>
       <c r="I14">
-        <v>-4.9410242673714466E-2</v>
+        <v>0.40778854664264413</v>
       </c>
       <c r="J14">
-        <v>-4.5193593200361669E-2</v>
+        <v>0.49764904885297256</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-0.59480352452038676</v>
+        <v>-0.43994340348871641</v>
       </c>
       <c r="B15">
-        <v>-0.95551989319590291</v>
+        <v>0.98103558160739268</v>
       </c>
       <c r="C15">
-        <v>-0.92523460151179682</v>
+        <v>0.4986309013799799</v>
       </c>
       <c r="D15">
-        <v>-0.13661511735081974</v>
+        <v>0.97256565900433467</v>
       </c>
       <c r="E15">
-        <v>0.91908899561305657</v>
+        <v>9.948839361376572E-3</v>
       </c>
       <c r="F15">
-        <v>-0.85847017099216705</v>
+        <v>0.28902406726349583</v>
       </c>
       <c r="G15">
-        <v>0.97418386162368931</v>
+        <v>0.94387132751967906</v>
       </c>
       <c r="H15">
-        <v>-0.95188019282191338</v>
+        <v>-0.73649454925920543</v>
       </c>
       <c r="I15">
-        <v>0.80767290619531629</v>
+        <v>0.86320757901895395</v>
       </c>
       <c r="J15">
-        <v>0.94303294439167562</v>
+        <v>0.94571129388760367</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-2.9547806907341038E-2</v>
+        <v>-0.86769320715254983</v>
       </c>
       <c r="B16">
-        <v>-0.89497751991806274</v>
+        <v>0.8642309850457891</v>
       </c>
       <c r="C16">
-        <v>-0.8200463802860456</v>
+        <v>-0.53501330048135887</v>
       </c>
       <c r="D16">
-        <v>-0.20938894141805384</v>
+        <v>0.56354413811811976</v>
       </c>
       <c r="E16">
-        <v>0.267575663176496</v>
+        <v>0.86473371337856719</v>
       </c>
       <c r="F16">
-        <v>-0.88297293616013661</v>
+        <v>0.70444028957920846</v>
       </c>
       <c r="G16">
-        <v>0.4743798328125225</v>
+        <v>0.61268152901870165</v>
       </c>
       <c r="H16">
-        <v>-0.66801005949456416</v>
+        <v>0.32931286812121369</v>
       </c>
       <c r="I16">
-        <v>0.87895542106471936</v>
+        <v>0.86279783454770642</v>
       </c>
       <c r="J16">
-        <v>0.58977788308917178</v>
+        <v>0.46602787083354408</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-0.45461239394652669</v>
+        <v>0.77844830957572342</v>
       </c>
       <c r="B17">
-        <v>0.93937267142738834</v>
+        <v>-0.70160195682226234</v>
       </c>
       <c r="C17">
-        <v>0.81985135268813047</v>
+        <v>0.51079557391001729</v>
       </c>
       <c r="D17">
-        <v>0.45883735195903602</v>
+        <v>0.3578565198056361</v>
       </c>
       <c r="E17">
-        <v>-0.14959763220954431</v>
+        <v>0.90104923998310849</v>
       </c>
       <c r="F17">
-        <v>0.1983630090239672</v>
+        <v>0.25518767462591241</v>
       </c>
       <c r="G17">
-        <v>-0.4482458657832385</v>
+        <v>0.3578659141071911</v>
       </c>
       <c r="H17">
-        <v>0.3631646592052945</v>
+        <v>-0.415085613664118</v>
       </c>
       <c r="I17">
-        <v>-0.56009601596722935</v>
+        <v>-0.91716321941354173</v>
       </c>
       <c r="J17">
-        <v>-0.46594933834461161</v>
+        <v>-0.46766315241492801</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.92695272801735251</v>
+        <v>-0.69993373880554932</v>
       </c>
       <c r="B18">
-        <v>-0.39061643578279864</v>
+        <v>-0.58314642974228226</v>
       </c>
       <c r="C18">
-        <v>-0.13961263766886886</v>
+        <v>0.92253596299254481</v>
       </c>
       <c r="D18">
-        <v>0.30519112421465744</v>
+        <v>0.43212446434166341</v>
       </c>
       <c r="E18">
-        <v>-0.99275103636583328</v>
+        <v>-0.42794259789323835</v>
       </c>
       <c r="F18">
-        <v>0.52045325146778243</v>
+        <v>-0.8164395675614029</v>
       </c>
       <c r="G18">
-        <v>-0.70949303341143377</v>
+        <v>-0.89902016203602853</v>
       </c>
       <c r="H18">
-        <v>0.90992918991195293</v>
+        <v>0.1522239481743832</v>
       </c>
       <c r="I18">
-        <v>0.41397881068528197</v>
+        <v>0.25170675349618638</v>
       </c>
       <c r="J18">
-        <v>-0.2430949944122987</v>
+        <v>0.95160100371750955</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-0.92740949348790291</v>
+        <v>0.49344207256833678</v>
       </c>
       <c r="B19">
-        <v>-0.5774602371936286</v>
+        <v>-0.86469265257636418</v>
       </c>
       <c r="C19">
-        <v>-0.79152898636992086</v>
+        <v>0.69792997908812704</v>
       </c>
       <c r="D19">
-        <v>-3.4062636742107799E-2</v>
+        <v>0.67020760193587303</v>
       </c>
       <c r="E19">
-        <v>0.85137394983770409</v>
+        <v>-0.15299530233308606</v>
       </c>
       <c r="F19">
-        <v>-0.95106592042765836</v>
+        <v>-0.6760725279411075</v>
       </c>
       <c r="G19">
-        <v>-0.16993864534045408</v>
+        <v>0.36084324785263538</v>
       </c>
       <c r="H19">
-        <v>-0.71532450509428369</v>
+        <v>0.36413803693451297</v>
       </c>
       <c r="I19">
-        <v>0.93423100208335341</v>
+        <v>0.52679515597821291</v>
       </c>
       <c r="J19">
-        <v>0.70814518025220519</v>
+        <v>-0.80917914908770683</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8.8940816125759492E-2</v>
+        <v>0.7878164038772868</v>
       </c>
       <c r="B20">
-        <v>-0.25214889538545843</v>
+        <v>0.27187350603544119</v>
       </c>
       <c r="C20">
-        <v>-0.72943422586841278</v>
+        <v>0.58886957589322086</v>
       </c>
       <c r="D20">
-        <v>0.88280989313822789</v>
+        <v>0.81549919441514573</v>
       </c>
       <c r="E20">
-        <v>5.3656372733669674E-3</v>
+        <v>-0.3683747595191238</v>
       </c>
       <c r="F20">
-        <v>0.5027349676746462</v>
+        <v>0.57668295889744525</v>
       </c>
       <c r="G20">
-        <v>0.72701486886408817</v>
+        <v>0.24199198370472061</v>
       </c>
       <c r="H20">
-        <v>5.5781860820391195E-2</v>
+        <v>-0.42120885752989512</v>
       </c>
       <c r="I20">
-        <v>0.61195599173192672</v>
+        <v>-7.8392146350653294E-2</v>
       </c>
       <c r="J20">
-        <v>0.84043247140420241</v>
+        <v>-0.40593414222644297</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-4.465279797969475E-2</v>
+        <v>-0.67135654145155554</v>
       </c>
       <c r="B21">
-        <v>0.21515072622511111</v>
+        <v>0.59260256803227296</v>
       </c>
       <c r="C21">
-        <v>-0.45720342090012533</v>
+        <v>-0.52267812762383181</v>
       </c>
       <c r="D21">
-        <v>0.68654091928743</v>
+        <v>3.8402283444742384E-2</v>
       </c>
       <c r="E21">
-        <v>-1.0358890065737951E-2</v>
+        <v>-0.11268780987908779</v>
       </c>
       <c r="F21">
-        <v>0.57954423560407775</v>
+        <v>0.32572215735427557</v>
       </c>
       <c r="G21">
-        <v>0.9073542848591819</v>
+        <v>-0.31056324720235334</v>
       </c>
       <c r="H21">
-        <v>-0.17487904085486539</v>
+        <v>0.32710947158144554</v>
       </c>
       <c r="I21">
-        <v>-0.34630280059579699</v>
+        <v>-0.98530831970655142</v>
       </c>
       <c r="J21">
-        <v>-0.51982405225501827</v>
+        <v>-0.82755629817100285</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-0.29712329782841296</v>
+        <v>0.57807764463379252</v>
       </c>
       <c r="B22">
-        <v>0.12657530654363516</v>
+        <v>0.61560983772574629</v>
       </c>
       <c r="C22">
-        <v>9.6263400136429287E-4</v>
+        <v>0.12623705377880384</v>
       </c>
       <c r="D22">
-        <v>-0.78937980521126183</v>
+        <v>0.41411991404539189</v>
       </c>
       <c r="E22">
-        <v>0.65685830164085512</v>
+        <v>0.99497369913226263</v>
       </c>
       <c r="F22">
-        <v>0.25074418188329312</v>
+        <v>-0.29190643690506307</v>
       </c>
       <c r="G22">
-        <v>0.18035456776379727</v>
+        <v>0.91129130203088093</v>
       </c>
       <c r="H22">
-        <v>-0.50396542593151239</v>
+        <v>0.89815253741152201</v>
       </c>
       <c r="I22">
-        <v>0.26904749975880526</v>
+        <v>0.82022237012146926</v>
       </c>
       <c r="J22">
-        <v>0.98047623065404887</v>
+        <v>0.7764185750419802</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-0.40606361968874993</v>
+        <v>-0.67404050019097184</v>
       </c>
       <c r="B23">
-        <v>-0.39772385697303886</v>
+        <v>-0.54873121411016756</v>
       </c>
       <c r="C23">
-        <v>-0.51796557823957967</v>
+        <v>-0.5416120610404459</v>
       </c>
       <c r="D23">
-        <v>-2.7658957121307667E-2</v>
+        <v>-0.98721368215422223</v>
       </c>
       <c r="E23">
-        <v>0.19945878786137636</v>
+        <v>-0.98272052808945631</v>
       </c>
       <c r="F23">
-        <v>-0.18753122900388258</v>
+        <v>0.19971006855941803</v>
       </c>
       <c r="G23">
-        <v>0.77755600860101404</v>
+        <v>-0.43600037340048992</v>
       </c>
       <c r="H23">
-        <v>-0.2892150626065465</v>
+        <v>-0.74284093522545258</v>
       </c>
       <c r="I23">
-        <v>0.82193441570275039</v>
+        <v>-0.29668698404834243</v>
       </c>
       <c r="J23">
-        <v>-0.21838729911504179</v>
+        <v>-0.77126885780174237</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.21919589190199043</v>
+        <v>0.70754781425522106</v>
       </c>
       <c r="B24">
-        <v>-0.58596222191502856</v>
+        <v>0.61009562000330442</v>
       </c>
       <c r="C24">
-        <v>-0.45583246029395569</v>
+        <v>0.46687172054402509</v>
       </c>
       <c r="D24">
-        <v>-0.40942714499442279</v>
+        <v>-0.70822988065736858</v>
       </c>
       <c r="E24">
-        <v>-6.9257943242546319E-2</v>
+        <v>0.2870492185515458</v>
       </c>
       <c r="F24">
-        <v>-8.1396977507689733E-2</v>
+        <v>-0.1235358850834106</v>
       </c>
       <c r="G24">
-        <v>-0.33472343592094189</v>
+        <v>0.92251752351261085</v>
       </c>
       <c r="H24">
-        <v>-0.36094368899668899</v>
+        <v>-0.70595836116205379</v>
       </c>
       <c r="I24">
-        <v>-0.72531397205800685</v>
+        <v>0.93342601037824591</v>
       </c>
       <c r="J24">
-        <v>-0.56487384854132316</v>
+        <v>-0.34896278894140753</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0.11004228580800743</v>
+        <v>-0.94263542888863106</v>
       </c>
       <c r="B25">
-        <v>0.67868437524004688</v>
+        <v>-0.45655822658085804</v>
       </c>
       <c r="C25">
-        <v>0.59316384433038538</v>
+        <v>0.86108419415358872</v>
       </c>
       <c r="D25">
-        <v>0.57383656379427483</v>
+        <v>0.58030561139482073</v>
       </c>
       <c r="E25">
-        <v>-0.64790125123869446</v>
+        <v>-0.68772085938342864</v>
       </c>
       <c r="F25">
-        <v>0.86476941580251732</v>
+        <v>0.72131017202171543</v>
       </c>
       <c r="G25">
-        <v>-0.88581197349092644</v>
+        <v>-0.23834293079597696</v>
       </c>
       <c r="H25">
-        <v>0.56499203663858266</v>
+        <v>-0.65360862307529421</v>
       </c>
       <c r="I25">
-        <v>-0.61517458336331921</v>
+        <v>0.92073722955488557</v>
       </c>
       <c r="J25">
-        <v>-0.38666654199803968</v>
+        <v>0.12932485665845919</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-0.24664301143991627</v>
+        <v>-0.90257876626789268</v>
       </c>
       <c r="B26">
-        <v>0.64347103023010277</v>
+        <v>0.3509237488364701</v>
       </c>
       <c r="C26">
-        <v>-9.3222187998720771E-2</v>
+        <v>0.72737358699832366</v>
       </c>
       <c r="D26">
-        <v>-0.35409184539249822</v>
+        <v>-0.91880962127161636</v>
       </c>
       <c r="E26">
-        <v>-0.53158030303722248</v>
+        <v>0.56325390233785189</v>
       </c>
       <c r="F26">
-        <v>0.63481418130459721</v>
+        <v>-0.87780583329881878</v>
       </c>
       <c r="G26">
-        <v>0.72566456868001838</v>
+        <v>-0.56383905727977113</v>
       </c>
       <c r="H26">
-        <v>-0.14765227140303386</v>
+        <v>-0.33450954388306248</v>
       </c>
       <c r="I26">
-        <v>-1.2708192254261794E-2</v>
+        <v>-0.54473961243640567</v>
       </c>
       <c r="J26">
-        <v>0.23965923331567746</v>
+        <v>0.38621628983257167</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.61385554215933502</v>
+        <v>0.90595749887822141</v>
       </c>
       <c r="B27">
-        <v>0.29720215951933915</v>
+        <v>0.42371844446096113</v>
       </c>
       <c r="C27">
-        <v>-0.56348639831063718</v>
+        <v>0.70195036171471847</v>
       </c>
       <c r="D27">
-        <v>-0.59304510216225115</v>
+        <v>0.99167682757373099</v>
       </c>
       <c r="E27">
-        <v>0.91151110589237716</v>
+        <v>-0.13844858575334693</v>
       </c>
       <c r="F27">
-        <v>7.2938511525060284E-2</v>
+        <v>-0.93621028406157603</v>
       </c>
       <c r="G27">
-        <v>-0.90326879529832105</v>
+        <v>-0.6735931642454499</v>
       </c>
       <c r="H27">
-        <v>0.55434906371895931</v>
+        <v>0.77075485198029081</v>
       </c>
       <c r="I27">
-        <v>0.62723856966587266</v>
+        <v>-5.8299891627799638E-2</v>
       </c>
       <c r="J27">
-        <v>-0.38776020234901126</v>
+        <v>-0.85596252931474393</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.94640250138814552</v>
+        <v>0.32446843087059357</v>
       </c>
       <c r="B28">
-        <v>0.96428971231050542</v>
+        <v>7.5500735647752629E-2</v>
       </c>
       <c r="C28">
-        <v>0.91380491282653231</v>
+        <v>4.6057142774299238E-2</v>
       </c>
       <c r="D28">
-        <v>0.59698837602152988</v>
+        <v>0.82633188163072546</v>
       </c>
       <c r="E28">
-        <v>-0.76453274498520429</v>
+        <v>0.80947380675729308</v>
       </c>
       <c r="F28">
-        <v>0.96056657507537602</v>
+        <v>-0.57567714848046503</v>
       </c>
       <c r="G28">
-        <v>-0.4438454297931701</v>
+        <v>-0.90970994749318945</v>
       </c>
       <c r="H28">
-        <v>0.85669438273641796</v>
+        <v>-0.41113125536902095</v>
       </c>
       <c r="I28">
-        <v>-0.44369127109159556</v>
+        <v>0.86916277858147162</v>
       </c>
       <c r="J28">
-        <v>-0.43824810627686728</v>
+        <v>-0.30291355178437729</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.77630570521874442</v>
+        <v>-0.79742365559490103</v>
       </c>
       <c r="B29">
-        <v>-0.413122562674472</v>
+        <v>-0.38840347976941192</v>
       </c>
       <c r="C29">
-        <v>0.95893759692062941</v>
+        <v>-0.52028729466150014</v>
       </c>
       <c r="D29">
-        <v>-0.48907980357665964</v>
+        <v>-0.54448756269763665</v>
       </c>
       <c r="E29">
-        <v>-0.77595800605374277</v>
+        <v>0.20477013368955188</v>
       </c>
       <c r="F29">
-        <v>-0.36944307100424395</v>
+        <v>-5.0907375486882747E-2</v>
       </c>
       <c r="G29">
-        <v>0.62390498792109372</v>
+        <v>-0.92038568603921811</v>
       </c>
       <c r="H29">
-        <v>0.49406660218279291</v>
+        <v>0.89060424984771869</v>
       </c>
       <c r="I29">
-        <v>-0.39150072259469459</v>
+        <v>0.72503102270052988</v>
       </c>
       <c r="J29">
-        <v>4.6202559708945747E-2</v>
+        <v>0.62893189801365579</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.93261451149719887</v>
+        <v>0.39839922105933107</v>
       </c>
       <c r="B30">
-        <v>0.77579272243638897</v>
+        <v>-0.20233674732736365</v>
       </c>
       <c r="C30">
-        <v>0.9429474155421127</v>
+        <v>-2.2632273751421687E-2</v>
       </c>
       <c r="D30">
-        <v>-0.62402356553553662</v>
+        <v>-0.88341059202827554</v>
       </c>
       <c r="E30">
-        <v>-0.65207585731747708</v>
+        <v>-0.3957821535629415</v>
       </c>
       <c r="F30">
-        <v>0.77209818875952063</v>
+        <v>0.56622793437228058</v>
       </c>
       <c r="G30">
-        <v>6.356381840990967E-2</v>
+        <v>-0.52614947890259389</v>
       </c>
       <c r="H30">
-        <v>0.98080069222321076</v>
+        <v>0.37600371046218378</v>
       </c>
       <c r="I30">
-        <v>-0.64513891499879938</v>
+        <v>8.40311286255052E-2</v>
       </c>
       <c r="J30">
-        <v>-0.82361474341511531</v>
+        <v>-0.40779513548206509</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>-0.93348158257231084</v>
+        <v>-0.51665747169458598</v>
       </c>
       <c r="B31">
-        <v>-0.80102870707478646</v>
+        <v>-6.1630448362326958E-2</v>
       </c>
       <c r="C31">
-        <v>-0.79698466701879733</v>
+        <v>0.92298743659151017</v>
       </c>
       <c r="D31">
-        <v>-0.32874701684739965</v>
+        <v>0.87276310357767573</v>
       </c>
       <c r="E31">
-        <v>-7.6655666254893421E-3</v>
+        <v>0.91591415838210677</v>
       </c>
       <c r="F31">
-        <v>-0.30489639574525962</v>
+        <v>0.13106616414587424</v>
       </c>
       <c r="G31">
-        <v>-0.73425930867025413</v>
+        <v>-0.42324207228278604</v>
       </c>
       <c r="H31">
-        <v>-0.931748208856367</v>
+        <v>0.39781468554871952</v>
       </c>
       <c r="I31">
-        <v>0.4711415839582605</v>
+        <v>-0.90936927981119275</v>
       </c>
       <c r="J31">
-        <v>0.91850097547848175</v>
+        <v>0.50741390027433197</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.80534582592292747</v>
+        <v>0.5784566562400778</v>
       </c>
       <c r="B32">
-        <v>-0.26083984215720113</v>
+        <v>0.96439450578219144</v>
       </c>
       <c r="C32">
-        <v>0.39110438072359288</v>
+        <v>0.54773201060269705</v>
       </c>
       <c r="D32">
-        <v>-0.76570617406351693</v>
+        <v>0.16649431430405409</v>
       </c>
       <c r="E32">
-        <v>0.1344207443711406</v>
+        <v>0.68737794838863164</v>
       </c>
       <c r="F32">
-        <v>0.55470682294450158</v>
+        <v>0.12476609343247243</v>
       </c>
       <c r="G32">
-        <v>-0.18361438869763394</v>
+        <v>-0.52207571091429195</v>
       </c>
       <c r="H32">
-        <v>-0.37372232339787287</v>
+        <v>0.98634329150604072</v>
       </c>
       <c r="I32">
-        <v>0.87421196426490166</v>
+        <v>0.60684434680520871</v>
       </c>
       <c r="J32">
-        <v>-0.54612191234142604</v>
+        <v>0.22091875370597755</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.95385329415510833</v>
+        <v>-0.410817079284024</v>
       </c>
       <c r="B33">
-        <v>7.5053966480339643E-2</v>
+        <v>-0.86102327766611908</v>
       </c>
       <c r="C33">
-        <v>0.79463012025468394</v>
+        <v>0.41427996092239605</v>
       </c>
       <c r="D33">
-        <v>0.71115450694812721</v>
+        <v>0.623989550776616</v>
       </c>
       <c r="E33">
-        <v>-0.87916494360901931</v>
+        <v>0.19697398935558014</v>
       </c>
       <c r="F33">
-        <v>0.94591965869763917</v>
+        <v>-0.92936583770469927</v>
       </c>
       <c r="G33">
-        <v>-0.23782491484319079</v>
+        <v>-0.76873172905069032</v>
       </c>
       <c r="H33">
-        <v>0.93958015366115899</v>
+        <v>-0.87460216393639834</v>
       </c>
       <c r="I33">
-        <v>-0.62986198803031834</v>
+        <v>-0.76950845697990455</v>
       </c>
       <c r="J33">
-        <v>0.62692500820095609</v>
+        <v>-0.64051832114676333</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>-0.20471124048778327</v>
+        <v>0.47050040407908233</v>
       </c>
       <c r="B34">
-        <v>0.33462886543847475</v>
+        <v>0.7745120079022092</v>
       </c>
       <c r="C34">
-        <v>0.53075156340704255</v>
+        <v>-0.44736764849799715</v>
       </c>
       <c r="D34">
-        <v>0.63429229274577126</v>
+        <v>0.93291329940924128</v>
       </c>
       <c r="E34">
-        <v>0.7039224927307256</v>
+        <v>-0.96756703540185685</v>
       </c>
       <c r="F34">
-        <v>-0.77993617623436795</v>
+        <v>-0.32406556485684468</v>
       </c>
       <c r="G34">
-        <v>0.84547992785836734</v>
+        <v>0.69056837270817961</v>
       </c>
       <c r="H34">
-        <v>-0.51148156866546435</v>
+        <v>-0.45338584914008756</v>
       </c>
       <c r="I34">
-        <v>0.59351519395763075</v>
+        <v>0.82035444134955615</v>
       </c>
       <c r="J34">
-        <v>0.33969375939902952</v>
+        <v>-0.73379062537979545</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.86857886226797265</v>
+        <v>0.49502832742667074</v>
       </c>
       <c r="B35">
-        <v>0.10424440576447139</v>
+        <v>0.4651242927118559</v>
       </c>
       <c r="C35">
-        <v>0.12991045363048215</v>
+        <v>-0.16675493137527389</v>
       </c>
       <c r="D35">
-        <v>0.16460420310073745</v>
+        <v>0.56255082535857936</v>
       </c>
       <c r="E35">
-        <v>-0.60600821447205344</v>
+        <v>0.16333148223136756</v>
       </c>
       <c r="F35">
-        <v>0.69553977484879637</v>
+        <v>0.81879811648473444</v>
       </c>
       <c r="G35">
-        <v>-0.12540915165330796</v>
+        <v>-0.35094155098558832</v>
       </c>
       <c r="H35">
-        <v>0.62470536906517837</v>
+        <v>-3.1068065953914127E-2</v>
       </c>
       <c r="I35">
-        <v>-0.98425488134845018</v>
+        <v>0.6381561392670968</v>
       </c>
       <c r="J35">
-        <v>-0.61816068897134957</v>
+        <v>-0.36732222878784104</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.93793844109780866</v>
+        <v>-0.95692855739663552</v>
       </c>
       <c r="B36">
-        <v>0.11365135140877103</v>
+        <v>0.36564818947728439</v>
       </c>
       <c r="C36">
-        <v>0.90333940902942711</v>
+        <v>-0.53365392554945179</v>
       </c>
       <c r="D36">
-        <v>0.66157983309282897</v>
+        <v>-0.7657095157958973</v>
       </c>
       <c r="E36">
-        <v>-0.94344553482384208</v>
+        <v>-0.22375769672973914</v>
       </c>
       <c r="F36">
-        <v>0.7532230288379842</v>
+        <v>0.65758452716828319</v>
       </c>
       <c r="G36">
-        <v>-1.2745888752792861E-2</v>
+        <v>0.9118893082481172</v>
       </c>
       <c r="H36">
-        <v>0.4796453679290138</v>
+        <v>0.56497209557217876</v>
       </c>
       <c r="I36">
-        <v>-0.64226616204990494</v>
+        <v>-0.69587948142558842</v>
       </c>
       <c r="J36">
-        <v>-0.22539671440499098</v>
+        <v>0.80899691994509515</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>-0.93176706476306748</v>
+        <v>0.70220899432729611</v>
       </c>
       <c r="B37">
-        <v>0.90153876941670485</v>
+        <v>-0.76670286184189285</v>
       </c>
       <c r="C37">
-        <v>-0.43342989272240345</v>
+        <v>-0.79219295989599403</v>
       </c>
       <c r="D37">
-        <v>-0.29273207590586031</v>
+        <v>0.73619827020268136</v>
       </c>
       <c r="E37">
-        <v>0.80010302786715326</v>
+        <v>0.23151831368427209</v>
       </c>
       <c r="F37">
-        <v>-0.64611464741573821</v>
+        <v>-0.15970314401944594</v>
       </c>
       <c r="G37">
-        <v>-0.38736234583853785</v>
+        <v>0.9011668314312814</v>
       </c>
       <c r="H37">
-        <v>-0.43882341309903344</v>
+        <v>0.77950167902620282</v>
       </c>
       <c r="I37">
-        <v>0.79321360646572181</v>
+        <v>0.77389444325279855</v>
       </c>
       <c r="J37">
-        <v>-0.73361337794522163</v>
+        <v>-0.24864146906937973</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.45879276690047011</v>
+        <v>-0.70762601067517272</v>
       </c>
       <c r="B38">
-        <v>0.91407252613579071</v>
+        <v>0.39547574772729882</v>
       </c>
       <c r="C38">
-        <v>0.63335769037468326</v>
+        <v>-0.61417914015602837</v>
       </c>
       <c r="D38">
-        <v>-0.34266912552221329</v>
+        <v>2.3709364085611029E-2</v>
       </c>
       <c r="E38">
-        <v>0.70158807426780667</v>
+        <v>-0.57589209649430062</v>
       </c>
       <c r="F38">
-        <v>0.65154294003998092</v>
+        <v>-0.79225701626546818</v>
       </c>
       <c r="G38">
-        <v>-0.81706247305659496</v>
+        <v>0.19426833079674902</v>
       </c>
       <c r="H38">
-        <v>0.68706668671681481</v>
+        <v>-0.51098180020965822</v>
       </c>
       <c r="I38">
-        <v>-0.57547328832281897</v>
+        <v>0.6373106622119763</v>
       </c>
       <c r="J38">
-        <v>-0.35864009475453429</v>
+        <v>-0.68640704455480028</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>-0.58953164732376029</v>
+        <v>0.98297246412683248</v>
       </c>
       <c r="B39">
-        <v>-0.46718638953448288</v>
+        <v>-0.71467050931817699</v>
       </c>
       <c r="C39">
-        <v>-0.57587287468893855</v>
+        <v>-0.78413269821980203</v>
       </c>
       <c r="D39">
-        <v>0.50019510800001055</v>
+        <v>0.5821807907564398</v>
       </c>
       <c r="E39">
-        <v>0.12881201237707307</v>
+        <v>0.91244372020539088</v>
       </c>
       <c r="F39">
-        <v>-0.78953298908624281</v>
+        <v>-0.9168060899116236</v>
       </c>
       <c r="G39">
-        <v>0.46332543041246399</v>
+        <v>-0.71578253984969031</v>
       </c>
       <c r="H39">
-        <v>-0.2916612471563092</v>
+        <v>-0.89728992389359064</v>
       </c>
       <c r="I39">
-        <v>-0.38253193258701718</v>
+        <v>-0.83649137091175629</v>
       </c>
       <c r="J39">
-        <v>-0.26205754040065471</v>
+        <v>-0.99697753575434511</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0.4964237176422065</v>
+        <v>0.64080826389061996</v>
       </c>
       <c r="B40">
-        <v>-0.89432904980332362</v>
+        <v>-0.3082021523518913</v>
       </c>
       <c r="C40">
-        <v>-0.79472374469235019</v>
+        <v>-0.79835661251574863</v>
       </c>
       <c r="D40">
-        <v>-0.95597515925111642</v>
+        <v>0.35781586398246079</v>
       </c>
       <c r="E40">
-        <v>-0.71473407509520692</v>
+        <v>0.74316640117457122</v>
       </c>
       <c r="F40">
-        <v>-0.17295777423724915</v>
+        <v>0.84176065354591545</v>
       </c>
       <c r="G40">
-        <v>0.87959653274456762</v>
+        <v>0.50639048321373603</v>
       </c>
       <c r="H40">
-        <v>-0.52733157470792758</v>
+        <v>0.21368216850279442</v>
       </c>
       <c r="I40">
-        <v>0.39462973860122197</v>
+        <v>0.27984061033515895</v>
       </c>
       <c r="J40">
-        <v>0.81676590083711331</v>
+        <v>-0.27358026566882415</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>-0.83333335678787057</v>
+        <v>-0.41334715569141312</v>
       </c>
       <c r="B41">
-        <v>-0.86033638436220283</v>
+        <v>0.87498263882552929</v>
       </c>
       <c r="C41">
-        <v>-0.85560547788021024</v>
+        <v>-0.74817227604652037</v>
       </c>
       <c r="D41">
-        <v>0.87412507116645444</v>
+        <v>-0.42295390775489217</v>
       </c>
       <c r="E41">
-        <v>-0.29820861150610128</v>
+        <v>8.5128131382806962E-2</v>
       </c>
       <c r="F41">
-        <v>-0.50830683334983562</v>
+        <v>0.75086297763919141</v>
       </c>
       <c r="G41">
-        <v>0.73182248633450542</v>
+        <v>0.89624828221473862</v>
       </c>
       <c r="H41">
-        <v>-0.97194431503995038</v>
+        <v>-0.18054002350319082</v>
       </c>
       <c r="I41">
-        <v>3.9965755325599227E-2</v>
+        <v>-0.14770948393211381</v>
       </c>
       <c r="J41">
-        <v>0.71501211654510899</v>
+        <v>0.51184197736414816</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0.57661796977304736</v>
+        <v>-0.96386756939768292</v>
       </c>
       <c r="B42">
-        <v>0.64411734273935484</v>
+        <v>-0.99543459265499146</v>
       </c>
       <c r="C42">
-        <v>0.76844857762918095</v>
+        <v>-0.15884131261500103</v>
       </c>
       <c r="D42">
-        <v>-0.60653841099721661</v>
+        <v>-0.5611075024769222</v>
       </c>
       <c r="E42">
-        <v>-0.85980228392137659</v>
+        <v>-0.59543990549034631</v>
       </c>
       <c r="F42">
-        <v>0.14800824885796665</v>
+        <v>-0.73290934689477794</v>
       </c>
       <c r="G42">
-        <v>-7.6099069433036792E-2</v>
+        <v>-0.51270308499358985</v>
       </c>
       <c r="H42">
-        <v>0.44540445912808679</v>
+        <v>0.47249544598311549</v>
       </c>
       <c r="I42">
-        <v>0.5213549396200573</v>
+        <v>-0.57140197683905514</v>
       </c>
       <c r="J42">
-        <v>-0.19612511786182732</v>
+        <v>-0.92534234472186094</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>-0.64345488061842959</v>
+        <v>-0.15571674232406477</v>
       </c>
       <c r="B43">
-        <v>-0.83145741860203448</v>
+        <v>-0.12338397579141511</v>
       </c>
       <c r="C43">
-        <v>-0.77159072117301064</v>
+        <v>-0.10235765787660124</v>
       </c>
       <c r="D43">
-        <v>0.6593114576336403</v>
+        <v>-0.5400310989168351</v>
       </c>
       <c r="E43">
-        <v>0.70681297088480033</v>
+        <v>-0.8320155265594843</v>
       </c>
       <c r="F43">
-        <v>-0.82180045597567686</v>
+        <v>-0.29830756903792155</v>
       </c>
       <c r="G43">
-        <v>0.57806813170712179</v>
+        <v>-0.81262602186742949</v>
       </c>
       <c r="H43">
-        <v>-0.81966512610362541</v>
+        <v>0.58737964332972437</v>
       </c>
       <c r="I43">
-        <v>0.76180584323811174</v>
+        <v>0.14113808350845791</v>
       </c>
       <c r="J43">
-        <v>0.28616461077877642</v>
+        <v>0.62719285987956286</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0.29242968704464511</v>
+        <v>-0.82339941201723155</v>
       </c>
       <c r="B44">
-        <v>0.92620314135020687</v>
+        <v>-0.79328804283286491</v>
       </c>
       <c r="C44">
-        <v>0.65066349364521525</v>
+        <v>-0.3169856850257402</v>
       </c>
       <c r="D44">
-        <v>0.91601119654157159</v>
+        <v>-0.75718032817061298</v>
       </c>
       <c r="E44">
-        <v>-0.32727367679616115</v>
+        <v>0.65003191044705055</v>
       </c>
       <c r="F44">
-        <v>-0.33196968437528379</v>
+        <v>-0.78794600304939955</v>
       </c>
       <c r="G44">
-        <v>-0.98559864149196175</v>
+        <v>0.85906381572493096</v>
       </c>
       <c r="H44">
-        <v>0.57550431946624314</v>
+        <v>-0.20034913163934018</v>
       </c>
       <c r="I44">
-        <v>-0.11234957885807774</v>
+        <v>-0.48477460401934819</v>
       </c>
       <c r="J44">
-        <v>-0.87246687361560582</v>
+        <v>0.14779007411041409</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1.4739689231184086E-2</v>
+        <v>0.44560307403686428</v>
       </c>
       <c r="B45">
-        <v>0.27575349886770339</v>
+        <v>0.983514709924455</v>
       </c>
       <c r="C45">
-        <v>0.75472444867239896</v>
+        <v>0.52348879154210082</v>
       </c>
       <c r="D45">
-        <v>-0.36381995506029957</v>
+        <v>0.78141075130725668</v>
       </c>
       <c r="E45">
-        <v>-0.32936929390286718</v>
+        <v>0.38250671703021616</v>
       </c>
       <c r="F45">
-        <v>0.55882692448877558</v>
+        <v>0.79653075500563075</v>
       </c>
       <c r="G45">
-        <v>-0.36242835491195724</v>
+        <v>0.79876879039958593</v>
       </c>
       <c r="H45">
-        <v>0.28275899197939758</v>
+        <v>0.87664503729050158</v>
       </c>
       <c r="I45">
-        <v>-0.20004470406963842</v>
+        <v>0.93578432448983617</v>
       </c>
       <c r="J45">
-        <v>-0.73141431221651432</v>
+        <v>4.2398392862620593E-2</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>-0.34042982679528422</v>
+        <v>-0.94122179785329507</v>
       </c>
       <c r="B46">
-        <v>0.12633842733816961</v>
+        <v>0.27025688350883131</v>
       </c>
       <c r="C46">
-        <v>-0.59661774716371052</v>
+        <v>-0.50152461991648878</v>
       </c>
       <c r="D46">
-        <v>7.1582787603688039E-2</v>
+        <v>0.76423358774062788</v>
       </c>
       <c r="E46">
-        <v>0.7146301346170415</v>
+        <v>-0.36009204984347271</v>
       </c>
       <c r="F46">
-        <v>-0.31271881684065167</v>
+        <v>0.88589695854585915</v>
       </c>
       <c r="G46">
-        <v>-0.47061178962777683</v>
+        <v>0.81113623795422529</v>
       </c>
       <c r="H46">
-        <v>-7.0530636041171033E-2</v>
+        <v>-0.58240231096989181</v>
       </c>
       <c r="I46">
-        <v>-0.10516618115120895</v>
+        <v>7.6112403029071546E-2</v>
       </c>
       <c r="J46">
-        <v>0.36460695404977633</v>
+        <v>-0.93442660451054815</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>-0.15228471969566085</v>
+        <v>0.97485610136453693</v>
       </c>
       <c r="B47">
-        <v>-0.77078550469476137</v>
+        <v>-0.15674616507329261</v>
       </c>
       <c r="C47">
-        <v>-0.62863284314449575</v>
+        <v>0.77837776745060361</v>
       </c>
       <c r="D47">
-        <v>-0.70865244012893025</v>
+        <v>0.47239075254109114</v>
       </c>
       <c r="E47">
-        <v>0.40458844098477009</v>
+        <v>0.41898544628356532</v>
       </c>
       <c r="F47">
-        <v>0.42827245354292481</v>
+        <v>0.49306874913600335</v>
       </c>
       <c r="G47">
-        <v>0.36446607656980018</v>
+        <v>0.32269326305970014</v>
       </c>
       <c r="H47">
-        <v>0.28141574814272702</v>
+        <v>0.7682073171127981</v>
       </c>
       <c r="I47">
-        <v>0.43381606310427789</v>
+        <v>0.58609273186126076</v>
       </c>
       <c r="J47">
-        <v>0.76263951730584245</v>
+        <v>-0.47420822590673617</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>-0.22654280461286799</v>
+        <v>7.4912011407282653E-2</v>
       </c>
       <c r="B48">
-        <v>0.31543291505919968</v>
+        <v>-0.28667027807823053</v>
       </c>
       <c r="C48">
-        <v>0.92884690019090821</v>
+        <v>0.10213098610351561</v>
       </c>
       <c r="D48">
-        <v>-0.34348918633445208</v>
+        <v>0.33766273059204632</v>
       </c>
       <c r="E48">
-        <v>-0.32710814806229666</v>
+        <v>1.4716388941372118E-2</v>
       </c>
       <c r="F48">
-        <v>0.44494516934719358</v>
+        <v>-0.20339575017161607</v>
       </c>
       <c r="G48">
-        <v>-0.20464198812833362</v>
+        <v>-0.57222119700660012</v>
       </c>
       <c r="H48">
-        <v>8.3661117427819912E-2</v>
+        <v>-0.92740212959920032</v>
       </c>
       <c r="I48">
-        <v>-0.27997943570675188</v>
+        <v>-0.95229456581642857</v>
       </c>
       <c r="J48">
-        <v>-0.48338079596212491</v>
+        <v>-0.70825464634470703</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>-0.52578596759411689</v>
+        <v>0.50259853213113892</v>
       </c>
       <c r="B49">
-        <v>-0.96559857818358119</v>
+        <v>-0.27705985211466916</v>
       </c>
       <c r="C49">
-        <v>-0.76812898325692869</v>
+        <v>-0.1286008788941842</v>
       </c>
       <c r="D49">
-        <v>0.35981323680317706</v>
+        <v>8.7353457710280316E-2</v>
       </c>
       <c r="E49">
-        <v>0.25548328774760248</v>
+        <v>0.95472027574434226</v>
       </c>
       <c r="F49">
-        <v>-0.8888409164941975</v>
+        <v>-0.87849627122037111</v>
       </c>
       <c r="G49">
-        <v>0.84698134041085682</v>
+        <v>0.1469081201077288</v>
       </c>
       <c r="H49">
-        <v>-0.9757159961819124</v>
+        <v>-0.83762116815952314</v>
       </c>
       <c r="I49">
-        <v>0.77460507259342481</v>
+        <v>0.75406879014086814</v>
       </c>
       <c r="J49">
-        <v>0.90607474240020214</v>
+        <v>0.96351859910715909</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>-0.93399007097971865</v>
+        <v>-0.29333808175885207</v>
       </c>
       <c r="B50">
-        <v>0.29272890521606587</v>
+        <v>0.17187467072290993</v>
       </c>
       <c r="C50">
-        <v>-0.32461712818963745</v>
+        <v>0.98061444060551994</v>
       </c>
       <c r="D50">
-        <v>-0.76024481992587778</v>
+        <v>-0.79719603855166743</v>
       </c>
       <c r="E50">
-        <v>0.44312452889192694</v>
+        <v>-0.11993441069364712</v>
       </c>
       <c r="F50">
-        <v>-0.33277474773882965</v>
+        <v>-0.64767914440173457</v>
       </c>
       <c r="G50">
-        <v>-0.32536992171867979</v>
+        <v>-0.88026366255832467</v>
       </c>
       <c r="H50">
-        <v>-0.55762533061048969</v>
+        <v>-0.77674292043443083</v>
       </c>
       <c r="I50">
-        <v>-8.5497652104381497E-2</v>
+        <v>-4.3994556603300865E-2</v>
       </c>
       <c r="J50">
-        <v>-0.73530299458830151</v>
+        <v>-0.30476764183114285</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>-5.1594281296610742E-2</v>
+        <v>-0.56128768884841496</v>
       </c>
       <c r="B51">
-        <v>0.57043795989667734</v>
+        <v>0.98619835917834497</v>
       </c>
       <c r="C51">
-        <v>0.64885482044007603</v>
+        <v>0.8455133756876928</v>
       </c>
       <c r="D51">
-        <v>-0.82959026449212891</v>
+        <v>8.238825761734235E-2</v>
       </c>
       <c r="E51">
-        <v>-0.9463917515062038</v>
+        <v>-0.78280790070988204</v>
       </c>
       <c r="F51">
-        <v>0.61435347374635896</v>
+        <v>0.20629554694298324</v>
       </c>
       <c r="G51">
-        <v>-0.98117157587701775</v>
+        <v>0.83874794217217519</v>
       </c>
       <c r="H51">
-        <v>0.54609213391691092</v>
+        <v>0.50754012757580114</v>
       </c>
       <c r="I51">
-        <v>-0.78188159299598348</v>
+        <v>0.78303610028684034</v>
       </c>
       <c r="J51">
-        <v>-0.60017957498350238</v>
+        <v>0.81281496265913844</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>-0.50247167016611793</v>
+        <v>-0.1683633238817262</v>
       </c>
       <c r="B52">
-        <v>-0.76328353128731141</v>
+        <v>0.13618665454413359</v>
       </c>
       <c r="C52">
-        <v>-0.3303527634735669</v>
+        <v>-0.94390319430671155</v>
       </c>
       <c r="D52">
-        <v>-0.81907570574338096</v>
+        <v>-0.61265849320840449</v>
       </c>
       <c r="E52">
-        <v>0.78192298085896828</v>
+        <v>-0.93075681833649826</v>
       </c>
       <c r="F52">
-        <v>-0.62584839831798278</v>
+        <v>0.54260635132976909</v>
       </c>
       <c r="G52">
-        <v>0.58019930861511926</v>
+        <v>-0.67853416896102825</v>
       </c>
       <c r="H52">
-        <v>-0.74400596703681865</v>
+        <v>-0.53733947869909926</v>
       </c>
       <c r="I52">
-        <v>0.31038195940182289</v>
+        <v>-0.88913299301376647</v>
       </c>
       <c r="J52">
-        <v>-0.51101392877257945</v>
+        <v>-0.62501391069348389</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>0.2690961615909096</v>
+        <v>-0.91862057530785979</v>
       </c>
       <c r="B53">
-        <v>-0.44886883612138273</v>
+        <v>-0.31007125700982263</v>
       </c>
       <c r="C53">
-        <v>0.40582688077236528</v>
+        <v>-0.9148773829475374</v>
       </c>
       <c r="D53">
-        <v>-0.91845857068253434</v>
+        <v>-0.43247459553944612</v>
       </c>
       <c r="E53">
-        <v>-0.74799453248374326</v>
+        <v>-0.27389608950023081</v>
       </c>
       <c r="F53">
-        <v>0.42095624041753738</v>
+        <v>-0.2924084137184666</v>
       </c>
       <c r="G53">
-        <v>-0.73212156461708</v>
+        <v>-0.89760068448900021</v>
       </c>
       <c r="H53">
-        <v>0.40093730634838587</v>
+        <v>-0.9726052136368678</v>
       </c>
       <c r="I53">
-        <v>-0.41878494765335045</v>
+        <v>-0.84284821438855295</v>
       </c>
       <c r="J53">
-        <v>0.30883245693311356</v>
+        <v>0.19992946080954771</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>0.74780125331549563</v>
+        <v>0.62881111633979625</v>
       </c>
       <c r="B54">
-        <v>6.5202314153652061E-2</v>
+        <v>0.71017273071034448</v>
       </c>
       <c r="C54">
-        <v>0.90909384814219862</v>
+        <v>-0.51315698613802918</v>
       </c>
       <c r="D54">
-        <v>-0.30619950610823454</v>
+        <v>0.66595296329817344</v>
       </c>
       <c r="E54">
-        <v>-0.40700892097159808</v>
+        <v>0.92457118539175431</v>
       </c>
       <c r="F54">
-        <v>0.75618772842165671</v>
+        <v>-0.18342315082009109</v>
       </c>
       <c r="G54">
-        <v>-0.52804506301595355</v>
+        <v>3.813103699860336E-2</v>
       </c>
       <c r="H54">
-        <v>-6.1884534261641727E-2</v>
+        <v>-0.12869840087637474</v>
       </c>
       <c r="I54">
-        <v>-0.79627535303937214</v>
+        <v>0.95873671072112965</v>
       </c>
       <c r="J54">
-        <v>-0.50650607391933755</v>
+        <v>-0.43003632781346973</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>0.88298363685758363</v>
+        <v>0.59606860508212045</v>
       </c>
       <c r="B55">
-        <v>0.89767226519854249</v>
+        <v>-0.36638887321045366</v>
       </c>
       <c r="C55">
-        <v>0.93855456891022826</v>
+        <v>0.94762755238195795</v>
       </c>
       <c r="D55">
-        <v>-0.86604078666479578</v>
+        <v>-0.13660460676748276</v>
       </c>
       <c r="E55">
-        <v>-0.70745915087403788</v>
+        <v>-0.19405815538521598</v>
       </c>
       <c r="F55">
-        <v>0.73586674618944548</v>
+        <v>4.6528353670861153E-2</v>
       </c>
       <c r="G55">
-        <v>0.44288024511989549</v>
+        <v>-0.7098273122553741</v>
       </c>
       <c r="H55">
-        <v>0.91149673929036867</v>
+        <v>0.75474217576344893</v>
       </c>
       <c r="I55">
-        <v>-0.9702818122580873</v>
+        <v>-0.29728735902028336</v>
       </c>
       <c r="J55">
-        <v>-0.97935654278856787</v>
+        <v>0.56456184732769688</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>-0.76296910736593904</v>
+        <v>-0.90754860610234456</v>
       </c>
       <c r="B56">
-        <v>-0.57991065846432299</v>
+        <v>0.13668850593106655</v>
       </c>
       <c r="C56">
-        <v>-0.10571596572038085</v>
+        <v>0.90124481769386111</v>
       </c>
       <c r="D56">
-        <v>-0.38176546553773999</v>
+        <v>-0.38994359425873903</v>
       </c>
       <c r="E56">
-        <v>0.96850872302021052</v>
+        <v>-0.88847492821520901</v>
       </c>
       <c r="F56">
-        <v>-0.85154455955878516</v>
+        <v>0.45203424414741716</v>
       </c>
       <c r="G56">
-        <v>0.98623747179679166</v>
+        <v>0.98902894543898323</v>
       </c>
       <c r="H56">
-        <v>-0.84883833314465529</v>
+        <v>0.8197806602209845</v>
       </c>
       <c r="I56">
-        <v>0.89151052084941396</v>
+        <v>0.73120097946763274</v>
       </c>
       <c r="J56">
-        <v>0.95212135018306698</v>
+        <v>0.66387673213983689</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>-0.77730361502584988</v>
+        <v>0.72548723677521765</v>
       </c>
       <c r="B57">
-        <v>0.15551525599913954</v>
+        <v>0.76026109994103208</v>
       </c>
       <c r="C57">
-        <v>-0.25460795723975516</v>
+        <v>-0.48559748701955263</v>
       </c>
       <c r="D57">
-        <v>-0.78505898817304431</v>
+        <v>-0.26004966984777611</v>
       </c>
       <c r="E57">
-        <v>3.144552623510076E-2</v>
+        <v>0.53493462859090213</v>
       </c>
       <c r="F57">
-        <v>-0.4738625388906656</v>
+        <v>-0.18366630740634607</v>
       </c>
       <c r="G57">
-        <v>0.4241656196377766</v>
+        <v>-0.16373174647170574</v>
       </c>
       <c r="H57">
-        <v>0.18558299220730368</v>
+        <v>0.28520123042279111</v>
       </c>
       <c r="I57">
-        <v>0.79838841551551476</v>
+        <v>-0.36287588119957304</v>
       </c>
       <c r="J57">
-        <v>-0.19229775220826034</v>
+        <v>0.53296055341801662</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0.79326028534590076</v>
+        <v>2.2095448292042984E-2</v>
       </c>
       <c r="B58">
-        <v>0.9434795107690418</v>
+        <v>-0.46070779780166488</v>
       </c>
       <c r="C58">
-        <v>0.40377428285104866</v>
+        <v>0.57179475490046094</v>
       </c>
       <c r="D58">
-        <v>-4.506381855635179E-2</v>
+        <v>-0.68370560768373712</v>
       </c>
       <c r="E58">
-        <v>0.7116524614014994</v>
+        <v>0.25991471129973676</v>
       </c>
       <c r="F58">
-        <v>0.57412749315944689</v>
+        <v>-0.12532145638425043</v>
       </c>
       <c r="G58">
-        <v>-0.1182143310032307</v>
+        <v>-0.53709859150565142</v>
       </c>
       <c r="H58">
-        <v>0.5896003378195398</v>
+        <v>-0.66262271497262304</v>
       </c>
       <c r="I58">
-        <v>3.4289223730583795E-2</v>
+        <v>-0.23671021784520274</v>
       </c>
       <c r="J58">
-        <v>0.50070663679262106</v>
+        <v>0.93133401199538435</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0.40360571620644037</v>
+        <v>0.99513146144853737</v>
       </c>
       <c r="B59">
-        <v>0.34721424094709918</v>
+        <v>0.50671904011513424</v>
       </c>
       <c r="C59">
-        <v>0.10118205592643197</v>
+        <v>0.37630356165689144</v>
       </c>
       <c r="D59">
-        <v>0.42048912455134335</v>
+        <v>0.9756821564226883</v>
       </c>
       <c r="E59">
-        <v>0.83020633235269869</v>
+        <v>0.90189258753965051</v>
       </c>
       <c r="F59">
-        <v>-5.3109453473016335E-2</v>
+        <v>-8.4887315954048387E-2</v>
       </c>
       <c r="G59">
-        <v>0.36875931813802465</v>
+        <v>0.38793738371270525</v>
       </c>
       <c r="H59">
-        <v>0.59771955298741131</v>
+        <v>0.99391976960507988</v>
       </c>
       <c r="I59">
-        <v>0.10255962408746179</v>
+        <v>0.98073446501254791</v>
       </c>
       <c r="J59">
-        <v>0.89585783171987854</v>
+        <v>-3.1175155600510526E-2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>0.72619191234890146</v>
+        <v>-8.2820271121723271E-2</v>
       </c>
       <c r="B60">
-        <v>0.94867555753122135</v>
+        <v>-0.68978181436278274</v>
       </c>
       <c r="C60">
-        <v>0.95729747002432641</v>
+        <v>5.918386561602549E-2</v>
       </c>
       <c r="D60">
-        <v>0.38529309060503414</v>
+        <v>-0.32364185250401584</v>
       </c>
       <c r="E60">
-        <v>-0.91576294787290091</v>
+        <v>0.77170003850715441</v>
       </c>
       <c r="F60">
-        <v>0.97762580866253812</v>
+        <v>0.4435901064703493</v>
       </c>
       <c r="G60">
-        <v>-0.63353182592887958</v>
+        <v>0.87640808812985349</v>
       </c>
       <c r="H60">
-        <v>0.95959098456335878</v>
+        <v>0.80038856512035705</v>
       </c>
       <c r="I60">
-        <v>-0.95126611478168133</v>
+        <v>0.852184377977246</v>
       </c>
       <c r="J60">
-        <v>-0.83540985979866567</v>
+        <v>-0.33963756948509027</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>2.5191815855002752E-2</v>
+        <v>0.4937937672455312</v>
       </c>
       <c r="B61">
-        <v>0.38840020051851748</v>
+        <v>-0.70716861943140885</v>
       </c>
       <c r="C61">
-        <v>0.92715068802753864</v>
+        <v>0.81380266364350828</v>
       </c>
       <c r="D61">
-        <v>-0.31892551938500879</v>
+        <v>0.71858158832903396</v>
       </c>
       <c r="E61">
-        <v>0.42294959378127817</v>
+        <v>-0.74853644165162114</v>
       </c>
       <c r="F61">
-        <v>0.59073505093925571</v>
+        <v>0.83185649272534157</v>
       </c>
       <c r="G61">
-        <v>-0.73228773067875841</v>
+        <v>-0.50811940861149008</v>
       </c>
       <c r="H61">
-        <v>0.8051309606127296</v>
+        <v>0.74469829876854909</v>
       </c>
       <c r="I61">
-        <v>0.24362725743332761</v>
+        <v>-0.7508006380225416</v>
       </c>
       <c r="J61">
-        <v>0.47080614915239472</v>
+        <v>0.96329220505409263</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>0.90435277447339157</v>
+        <v>0.41235422081975437</v>
       </c>
       <c r="B62">
-        <v>-0.5187432099344691</v>
+        <v>0.19013410228935954</v>
       </c>
       <c r="C62">
-        <v>0.83058054886157129</v>
+        <v>-0.44658041634330486</v>
       </c>
       <c r="D62">
-        <v>0.14921283830279145</v>
+        <v>8.5050342534796528E-2</v>
       </c>
       <c r="E62">
-        <v>-0.17395510817132859</v>
+        <v>0.92162560310574504</v>
       </c>
       <c r="F62">
-        <v>0.60397057678775512</v>
+        <v>0.42030175378114409</v>
       </c>
       <c r="G62">
-        <v>-0.15378253399366074</v>
+        <v>1.5736279026671823E-2</v>
       </c>
       <c r="H62">
-        <v>0.53791379493424518</v>
+        <v>0.43690983237562064</v>
       </c>
       <c r="I62">
-        <v>-7.6838100230461392E-2</v>
+        <v>-0.73125160697576497</v>
       </c>
       <c r="J62">
-        <v>-0.71892472921693917</v>
+        <v>0.61386215022986623</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>-0.31901133414233218</v>
+        <v>0.47501219458748617</v>
       </c>
       <c r="B63">
-        <v>-0.78430735412972896</v>
+        <v>-0.31035387210546844</v>
       </c>
       <c r="C63">
-        <v>-0.64956239252308501</v>
+        <v>0.68099597014350277</v>
       </c>
       <c r="D63">
-        <v>-0.85146734498811227</v>
+        <v>0.11578137446836159</v>
       </c>
       <c r="E63">
-        <v>0.1741925592284253</v>
+        <v>0.46449782499304321</v>
       </c>
       <c r="F63">
-        <v>-0.29063872954546588</v>
+        <v>-0.90943487709436543</v>
       </c>
       <c r="G63">
-        <v>0.50432129033223583</v>
+        <v>0.12693091612767562</v>
       </c>
       <c r="H63">
-        <v>-0.77391649248299688</v>
+        <v>0.7548638929389806</v>
       </c>
       <c r="I63">
-        <v>0.26229683955639033</v>
+        <v>-0.31360252515013665</v>
       </c>
       <c r="J63">
-        <v>0.24460419142584047</v>
+        <v>0.41397374632237804</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>0.63753288207421932</v>
+        <v>0.48430560652884652</v>
       </c>
       <c r="B64">
-        <v>0.22444248924416926</v>
+        <v>-0.81292202702873617</v>
       </c>
       <c r="C64">
-        <v>0.52160537964412645</v>
+        <v>-0.89126734060444779</v>
       </c>
       <c r="D64">
-        <v>0.36386012386853112</v>
+        <v>0.1841984351402475</v>
       </c>
       <c r="E64">
-        <v>-0.106727633908137</v>
+        <v>6.3527474641892318E-2</v>
       </c>
       <c r="F64">
-        <v>3.3668945256767613E-2</v>
+        <v>7.4003036823662924E-2</v>
       </c>
       <c r="G64">
-        <v>9.6253371283106487E-2</v>
+        <v>-1.6548325503721224E-2</v>
       </c>
       <c r="H64">
-        <v>-0.48476055141927987</v>
+        <v>-0.86756281132038171</v>
       </c>
       <c r="I64">
-        <v>-0.54983400673766913</v>
+        <v>-0.63191904202772697</v>
       </c>
       <c r="J64">
-        <v>-0.12771249787724975</v>
+        <v>0.27625699157024464</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>0.62387165964475799</v>
+        <v>-0.19830927294941733</v>
       </c>
       <c r="B65">
-        <v>0.9380662568491559</v>
+        <v>-0.74438308445139567</v>
       </c>
       <c r="C65">
-        <v>0.65248251423387738</v>
+        <v>-0.77093065155528206</v>
       </c>
       <c r="D65">
-        <v>0.87343286774950013</v>
+        <v>-0.50636357643523933</v>
       </c>
       <c r="E65">
-        <v>-0.79670169824977966</v>
+        <v>-0.73091510330433784</v>
       </c>
       <c r="F65">
-        <v>0.84911720310859118</v>
+        <v>0.22368069299808535</v>
       </c>
       <c r="G65">
-        <v>-0.63633515113745276</v>
+        <v>0.98487025525591831</v>
       </c>
       <c r="H65">
-        <v>0.81876312177564459</v>
+        <v>0.97215966819190325</v>
       </c>
       <c r="I65">
-        <v>-0.75340342705392283</v>
+        <v>0.25793119788726854</v>
       </c>
       <c r="J65">
-        <v>-0.33033360200695255</v>
+        <v>0.63057514722268893</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>0.34588238828979373</v>
+        <v>0.28237411636836257</v>
       </c>
       <c r="B66">
-        <v>-0.36243182109976613</v>
+        <v>-0.79183868966226167</v>
       </c>
       <c r="C66">
-        <v>5.796026804065231E-2</v>
+        <v>-0.82387503745300139</v>
       </c>
       <c r="D66">
-        <v>-0.47689732299357201</v>
+        <v>0.37067281819576564</v>
       </c>
       <c r="E66">
-        <v>5.7347548639276574E-2</v>
+        <v>0.40373649379069326</v>
       </c>
       <c r="F66">
-        <v>-0.33279306110541779</v>
+        <v>0.81143133401413758</v>
       </c>
       <c r="G66">
-        <v>-0.50608416708708726</v>
+        <v>-0.85889524492300584</v>
       </c>
       <c r="H66">
-        <v>-0.28814708582957571</v>
+        <v>-0.83781448928276359</v>
       </c>
       <c r="I66">
-        <v>-0.12808459012326628</v>
+        <v>0.48481390618542358</v>
       </c>
       <c r="J66">
-        <v>-0.50971104227954556</v>
+        <v>0.5058978001371941</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>-0.27577633522946265</v>
+        <v>0.90824908537707416</v>
       </c>
       <c r="B67">
-        <v>-0.63419271270152056</v>
+        <v>0.12565288777480504</v>
       </c>
       <c r="C67">
-        <v>-0.33002825293481403</v>
+        <v>0.64486807653258382</v>
       </c>
       <c r="D67">
-        <v>-0.71213333166108173</v>
+        <v>-0.83552920133728592</v>
       </c>
       <c r="E67">
-        <v>-0.21798393605896974</v>
+        <v>0.57938928571471338</v>
       </c>
       <c r="F67">
-        <v>-0.81678756881518089</v>
+        <v>-0.54589551067985487</v>
       </c>
       <c r="G67">
-        <v>-0.65256643386578572</v>
+        <v>0.29927473985987019</v>
       </c>
       <c r="H67">
-        <v>-0.32780536938328297</v>
+        <v>0.60103705346571112</v>
       </c>
       <c r="I67">
-        <v>0.86839031394729105</v>
+        <v>-0.63519614227847965</v>
       </c>
       <c r="J67">
-        <v>0.80320764649435983</v>
+        <v>0.69331127217472011</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>0.81445460338702658</v>
+        <v>-0.82153645577048451</v>
       </c>
       <c r="B68">
-        <v>0.59091668206607895</v>
+        <v>0.81843181038866464</v>
       </c>
       <c r="C68">
-        <v>1.411078416352649E-2</v>
+        <v>-0.8011082351080937</v>
       </c>
       <c r="D68">
-        <v>0.78280210459455146</v>
+        <v>-0.33979889001430919</v>
       </c>
       <c r="E68">
-        <v>-0.85302843774516512</v>
+        <v>0.25474574338555495</v>
       </c>
       <c r="F68">
-        <v>0.90207628843311161</v>
+        <v>0.99137090252374838</v>
       </c>
       <c r="G68">
-        <v>-0.8633631122237948</v>
+        <v>0.13502371409377315</v>
       </c>
       <c r="H68">
-        <v>0.81512454610091178</v>
+        <v>-0.4715713715675135</v>
       </c>
       <c r="I68">
-        <v>-0.20589501189559431</v>
+        <v>-0.51370558627876917</v>
       </c>
       <c r="J68">
-        <v>0.68663444533937479</v>
+        <v>-3.618376181704893E-2</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>5.4984917729355258E-2</v>
+        <v>0.45369232522979519</v>
       </c>
       <c r="B69">
-        <v>0.52366938959665155</v>
+        <v>0.97794590905538603</v>
       </c>
       <c r="C69">
-        <v>-0.58945066177849359</v>
+        <v>0.82244851465828528</v>
       </c>
       <c r="D69">
-        <v>0.69304876110438529</v>
+        <v>0.53123429017539969</v>
       </c>
       <c r="E69">
-        <v>0.32059280039804311</v>
+        <v>-6.5956345976425509E-2</v>
       </c>
       <c r="F69">
-        <v>-0.79696929679344564</v>
+        <v>0.91100826194301421</v>
       </c>
       <c r="G69">
-        <v>0.63069129049421424</v>
+        <v>-0.85325229238745748</v>
       </c>
       <c r="H69">
-        <v>-0.85164396953013832</v>
+        <v>0.66081620103089367</v>
       </c>
       <c r="I69">
-        <v>0.9204701987396563</v>
+        <v>0.86211017939021373</v>
       </c>
       <c r="J69">
-        <v>0.69682584981425921</v>
+        <v>0.69368910100406667</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>-0.42959533358636881</v>
+        <v>-1.931218615961814E-2</v>
       </c>
       <c r="B70">
-        <v>-0.91433440677797195</v>
+        <v>0.77474189320659526</v>
       </c>
       <c r="C70">
-        <v>-0.71840351298013116</v>
+        <v>0.80656340159411255</v>
       </c>
       <c r="D70">
-        <v>0.73940519050270859</v>
+        <v>0.57155824069013539</v>
       </c>
       <c r="E70">
-        <v>0.9433887676620234</v>
+        <v>-0.34296628440764976</v>
       </c>
       <c r="F70">
-        <v>-0.60878318437631473</v>
+        <v>-0.90808230041551607</v>
       </c>
       <c r="G70">
-        <v>-0.10474300835130504</v>
+        <v>0.78136067306316714</v>
       </c>
       <c r="H70">
-        <v>-0.57630734402307759</v>
+        <v>-0.14068784601987</v>
       </c>
       <c r="I70">
-        <v>0.4086744010892005</v>
+        <v>0.49754973400691049</v>
       </c>
       <c r="J70">
-        <v>0.87522646211919308</v>
+        <v>0.67987194602837375</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>0.92223081258861828</v>
+        <v>-0.64373288560934638</v>
       </c>
       <c r="B71">
-        <v>-0.6188580335307301</v>
+        <v>-0.13516959505192605</v>
       </c>
       <c r="C71">
-        <v>-0.7075139524036278</v>
+        <v>-0.83519856333584097</v>
       </c>
       <c r="D71">
-        <v>-0.29972793150260441</v>
+        <v>-0.10445335628219417</v>
       </c>
       <c r="E71">
-        <v>-0.27760691250504355</v>
+        <v>-0.25073357581837391</v>
       </c>
       <c r="F71">
-        <v>0.23039082908313596</v>
+        <v>0.91289879752883718</v>
       </c>
       <c r="G71">
-        <v>0.66986098703737029</v>
+        <v>1.915663609468156E-3</v>
       </c>
       <c r="H71">
-        <v>-3.56680120126254E-2</v>
+        <v>-0.68673908230074676</v>
       </c>
       <c r="I71">
-        <v>-0.69341846630575754</v>
+        <v>-7.494336443968147E-2</v>
       </c>
       <c r="J71">
-        <v>-0.74274070528635794</v>
+        <v>-0.95267619899371858</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>-0.91682813481876846</v>
+        <v>0.24408025384068921</v>
       </c>
       <c r="B72">
-        <v>-0.83803781596074578</v>
+        <v>-5.4542170197063693E-2</v>
       </c>
       <c r="C72">
-        <v>-0.16341045078473806</v>
+        <v>0.73276914919568226</v>
       </c>
       <c r="D72">
-        <v>-0.53413973613687005</v>
+        <v>-0.80659748303227186</v>
       </c>
       <c r="E72">
-        <v>-0.38262095326604439</v>
+        <v>0.96767009909197366</v>
       </c>
       <c r="F72">
-        <v>0.14262031713024165</v>
+        <v>0.96711454452257994</v>
       </c>
       <c r="G72">
-        <v>-0.58649732001358235</v>
+        <v>2.9331343753657358E-2</v>
       </c>
       <c r="H72">
-        <v>0.48283703853449494</v>
+        <v>0.73802639726737129</v>
       </c>
       <c r="I72">
-        <v>-0.36050288127755142</v>
+        <v>0.25496016814509997</v>
       </c>
       <c r="J72">
-        <v>0.193389874152012</v>
+        <v>0.9577325519268679</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>-0.55871754936442675</v>
+        <v>-0.42994951394916453</v>
       </c>
       <c r="B73">
-        <v>-0.53879063471681488</v>
+        <v>0.35958850472619125</v>
       </c>
       <c r="C73">
-        <v>-0.79893044153135662</v>
+        <v>6.6791750106322727E-3</v>
       </c>
       <c r="D73">
-        <v>-0.60674232499967751</v>
+        <v>-5.6012992667046319E-2</v>
       </c>
       <c r="E73">
-        <v>-0.93581569273424559</v>
+        <v>-0.39375941497067057</v>
       </c>
       <c r="F73">
-        <v>-0.32918249324540616</v>
+        <v>0.48728186597634587</v>
       </c>
       <c r="G73">
-        <v>-0.19613279707249934</v>
+        <v>0.65293879399442889</v>
       </c>
       <c r="H73">
-        <v>7.7229059956914411E-3</v>
+        <v>0.24808185222680412</v>
       </c>
       <c r="I73">
-        <v>-0.74000552509024409</v>
+        <v>0.58412783606188612</v>
       </c>
       <c r="J73">
-        <v>0.16069044341516411</v>
+        <v>-0.40813540109777074</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>0.76113003774652332</v>
+        <v>0.13442118387813068</v>
       </c>
       <c r="B74">
-        <v>0.57964969836553337</v>
+        <v>0.90634910238111288</v>
       </c>
       <c r="C74">
-        <v>0.74571185231977555</v>
+        <v>0.37605840394326057</v>
       </c>
       <c r="D74">
-        <v>0.34885349247876069</v>
+        <v>-8.4489433067703207E-2</v>
       </c>
       <c r="E74">
-        <v>-0.69477297845079899</v>
+        <v>0.21914797832084423</v>
       </c>
       <c r="F74">
-        <v>0.78053895770856974</v>
+        <v>0.5432235169444013</v>
       </c>
       <c r="G74">
-        <v>-0.77740474055686204</v>
+        <v>0.5742283578408508</v>
       </c>
       <c r="H74">
-        <v>0.83388540159391611</v>
+        <v>-0.25016356423234998</v>
       </c>
       <c r="I74">
-        <v>-0.75128787245321438</v>
+        <v>-0.11050980306206447</v>
       </c>
       <c r="J74">
-        <v>0.70453636748377524</v>
+        <v>-0.67854388034342683</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>-0.79051932517349099</v>
+        <v>-0.3776192245379037</v>
       </c>
       <c r="B75">
-        <v>-0.74308749882865321</v>
+        <v>-0.83346684135168136</v>
       </c>
       <c r="C75">
-        <v>-0.65924433630995405</v>
+        <v>7.7180137536450255E-2</v>
       </c>
       <c r="D75">
-        <v>-0.29679890169236806</v>
+        <v>0.89891354707249527</v>
       </c>
       <c r="E75">
-        <v>-0.29000789388558718</v>
+        <v>-0.5135076125181256</v>
       </c>
       <c r="F75">
-        <v>-0.92917783308227553</v>
+        <v>-0.48420838156267038</v>
       </c>
       <c r="G75">
-        <v>-0.13463838480453419</v>
+        <v>-0.17650415571000119</v>
       </c>
       <c r="H75">
-        <v>-0.57147314296872587</v>
+        <v>0.65721846928074157</v>
       </c>
       <c r="I75">
-        <v>-0.46893288157206181</v>
+        <v>0.30189554034353611</v>
       </c>
       <c r="J75">
-        <v>0.55462951012253636</v>
+        <v>0.48202857056551879</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>-0.94012397389755165</v>
+        <v>-0.41449321017593288</v>
       </c>
       <c r="B76">
-        <v>-0.13435905826502703</v>
+        <v>0.85590905967042474</v>
       </c>
       <c r="C76">
-        <v>-0.80875372764837439</v>
+        <v>-0.40648877602791272</v>
       </c>
       <c r="D76">
-        <v>0.28012811312309832</v>
+        <v>-0.45224746301929619</v>
       </c>
       <c r="E76">
-        <v>0.12558700123531644</v>
+        <v>0.5084139568085585</v>
       </c>
       <c r="F76">
-        <v>5.9584566767251095E-2</v>
+        <v>0.38016298929590842</v>
       </c>
       <c r="G76">
-        <v>0.21751581506118328</v>
+        <v>-0.9395372759124011</v>
       </c>
       <c r="H76">
-        <v>-0.6941669009305812</v>
+        <v>-0.93549908266808346</v>
       </c>
       <c r="I76">
-        <v>0.42455741335533165</v>
+        <v>-0.45475610019932711</v>
       </c>
       <c r="J76">
-        <v>0.47027521667126981</v>
+        <v>0.83443585289273792</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>-0.46404502889546773</v>
+        <v>0.33674893059407018</v>
       </c>
       <c r="B77">
-        <v>0.99129142026757433</v>
+        <v>-0.50559651693358054</v>
       </c>
       <c r="C77">
-        <v>0.89377878261429222</v>
+        <v>4.1391351758048443E-2</v>
       </c>
       <c r="D77">
-        <v>-0.10770690578203412</v>
+        <v>0.32296346896872846</v>
       </c>
       <c r="E77">
-        <v>0.74046726133038254</v>
+        <v>0.90706808502599756</v>
       </c>
       <c r="F77">
-        <v>0.22430496521482754</v>
+        <v>2.3923457295836094E-2</v>
       </c>
       <c r="G77">
-        <v>3.330584764423572E-2</v>
+        <v>-5.098267819697605E-3</v>
       </c>
       <c r="H77">
-        <v>0.7953938331887811</v>
+        <v>-0.85006298233541122</v>
       </c>
       <c r="I77">
-        <v>6.2909584567054824E-2</v>
+        <v>-0.35343026857703957</v>
       </c>
       <c r="J77">
-        <v>-0.53133217250376041</v>
+        <v>0.44371360591680592</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>-0.18480110453964921</v>
+        <v>0.41477391822392456</v>
       </c>
       <c r="B78">
-        <v>0.32361450135642389</v>
+        <v>-0.93890791974536225</v>
       </c>
       <c r="C78">
-        <v>0.6256337022950742</v>
+        <v>0.74484632952499896</v>
       </c>
       <c r="D78">
-        <v>0.883856047354453</v>
+        <v>-0.55690243524035532</v>
       </c>
       <c r="E78">
-        <v>0.52501368509302082</v>
+        <v>0.8848595696657614</v>
       </c>
       <c r="F78">
-        <v>0.54674386328034652</v>
+        <v>0.92192346865640007</v>
       </c>
       <c r="G78">
-        <v>0.58612681866320315</v>
+        <v>-2.01294922885965E-3</v>
       </c>
       <c r="H78">
-        <v>-0.42544385789541395</v>
+        <v>-0.28357817377684974</v>
       </c>
       <c r="I78">
-        <v>-0.55357130563710166</v>
+        <v>0.26524728377206525</v>
       </c>
       <c r="J78">
-        <v>-0.23754549211869175</v>
+        <v>0.77629630373685621</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>0.88306068600422483</v>
+        <v>-0.92139145038466408</v>
       </c>
       <c r="B79">
-        <v>0.78259369851966798</v>
+        <v>0.1347911598243369</v>
       </c>
       <c r="C79">
-        <v>0.93222236658889879</v>
+        <v>0.754459926755082</v>
       </c>
       <c r="D79">
-        <v>-0.89803547352005841</v>
+        <v>0.32302254303492001</v>
       </c>
       <c r="E79">
-        <v>-0.87432725113722587</v>
+        <v>0.63707761173320243</v>
       </c>
       <c r="F79">
-        <v>0.53765273393021862</v>
+        <v>-0.36678983169507329</v>
       </c>
       <c r="G79">
-        <v>-0.9371705952096635</v>
+        <v>-0.75641079223776242</v>
       </c>
       <c r="H79">
-        <v>0.92192178998510954</v>
+        <v>-0.66688077401278745</v>
       </c>
       <c r="I79">
-        <v>-0.9803738012958606</v>
+        <v>-0.95938410844810873</v>
       </c>
       <c r="J79">
-        <v>-0.83985136237004432</v>
+        <v>-0.79634457330654917</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>0.80737388458194559</v>
+        <v>-6.5546118507907262E-3</v>
       </c>
       <c r="B80">
-        <v>-0.49798447099437382</v>
+        <v>-0.58312912169889952</v>
       </c>
       <c r="C80">
-        <v>0.1621425763538748</v>
+        <v>0.31838126459506333</v>
       </c>
       <c r="D80">
-        <v>0.98987048998962435</v>
+        <v>0.77436795473175124</v>
       </c>
       <c r="E80">
-        <v>0.25215405890736409</v>
+        <v>-0.1578008449023752</v>
       </c>
       <c r="F80">
-        <v>0.72377350045744071</v>
+        <v>-8.1721506180330132E-3</v>
       </c>
       <c r="G80">
-        <v>-0.6950092797959988</v>
+        <v>0.73649804281528519</v>
       </c>
       <c r="H80">
-        <v>0.34533177834180767</v>
+        <v>0.15829842890193402</v>
       </c>
       <c r="I80">
-        <v>-0.19883787787493334</v>
+        <v>-0.8924776979724891</v>
       </c>
       <c r="J80">
-        <v>0.72014078967687212</v>
+        <v>0.24660271677043663</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>-0.85857683614223634</v>
+        <v>-0.66570052087653597</v>
       </c>
       <c r="B81">
-        <v>-0.4439036366924215</v>
+        <v>-0.50376301983062366</v>
       </c>
       <c r="C81">
-        <v>-0.52178324840368595</v>
+        <v>-0.69983185010746041</v>
       </c>
       <c r="D81">
-        <v>0.68500643888109625</v>
+        <v>-0.85349407509748321</v>
       </c>
       <c r="E81">
-        <v>0.57838718780808207</v>
+        <v>-0.92804020189300163</v>
       </c>
       <c r="F81">
-        <v>-0.44357208544908272</v>
+        <v>-0.8831725807052192</v>
       </c>
       <c r="G81">
-        <v>-0.36392539411191238</v>
+        <v>0.48120033023617714</v>
       </c>
       <c r="H81">
-        <v>-0.4918344014344268</v>
+        <v>0.36811875826953039</v>
       </c>
       <c r="I81">
-        <v>-0.42122243090597145</v>
+        <v>-0.65303218738376223</v>
       </c>
       <c r="J81">
-        <v>-0.39790831825700151</v>
+        <v>-0.46504414854445164</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>-0.99242063788154489</v>
+        <v>-0.30463727507400251</v>
       </c>
       <c r="B82">
-        <v>-0.98700600034990682</v>
+        <v>-0.80676779934458154</v>
       </c>
       <c r="C82">
-        <v>-0.98524447378162583</v>
+        <v>-0.89564164758233633</v>
       </c>
       <c r="D82">
-        <v>-0.87646609201743975</v>
+        <v>-0.50136480713991749</v>
       </c>
       <c r="E82">
-        <v>0.98265396832519647</v>
+        <v>0.85227948551143984</v>
       </c>
       <c r="F82">
-        <v>-0.98234354571753102</v>
+        <v>-0.51890955184768917</v>
       </c>
       <c r="G82">
-        <v>0.73490477519878095</v>
+        <v>0.61759551181539807</v>
       </c>
       <c r="H82">
-        <v>-0.98872304571722158</v>
+        <v>0.53312694774565994</v>
       </c>
       <c r="I82">
-        <v>0.9903079056074171</v>
+        <v>-0.71661786216740642</v>
       </c>
       <c r="J82">
-        <v>0.13724161193379769</v>
+        <v>-0.14730739112345356</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>0.10968524532607947</v>
+        <v>0.72414203918234643</v>
       </c>
       <c r="B83">
-        <v>-0.20983686254898457</v>
+        <v>0.80459274437215389</v>
       </c>
       <c r="C83">
-        <v>-0.15787972496198568</v>
+        <v>-0.94756760695583386</v>
       </c>
       <c r="D83">
-        <v>0.83171947607881291</v>
+        <v>-0.14381175184764908</v>
       </c>
       <c r="E83">
-        <v>0.84983985357801384</v>
+        <v>-0.15510496002835134</v>
       </c>
       <c r="F83">
-        <v>-8.6750763293880095E-2</v>
+        <v>-0.97076571482990193</v>
       </c>
       <c r="G83">
-        <v>0.73673871186021145</v>
+        <v>0.71771755241091872</v>
       </c>
       <c r="H83">
-        <v>-0.34929023327725811</v>
+        <v>0.34619621868963013</v>
       </c>
       <c r="I83">
-        <v>-0.65096955566856884</v>
+        <v>-0.18245242126774636</v>
       </c>
       <c r="J83">
-        <v>0.49381329875843349</v>
+        <v>-0.42758679533186372</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0.45237825594628184</v>
+        <v>0.92242325164213246</v>
       </c>
       <c r="B84">
-        <v>-0.41654391864850654</v>
+        <v>-0.38604957461178324</v>
       </c>
       <c r="C84">
-        <v>-0.24056542204541229</v>
+        <v>-0.59677244012016639</v>
       </c>
       <c r="D84">
-        <v>-0.43893610584140391</v>
+        <v>1.2853045799699574E-2</v>
       </c>
       <c r="E84">
-        <v>-0.53006899635542837</v>
+        <v>-0.84994978554578693</v>
       </c>
       <c r="F84">
-        <v>-6.4053100289449827E-2</v>
+        <v>-0.89243422593197341</v>
       </c>
       <c r="G84">
-        <v>0.32227772556889084</v>
+        <v>0.40403717799024391</v>
       </c>
       <c r="H84">
-        <v>0.66325008733541435</v>
+        <v>0.42266158144639981</v>
       </c>
       <c r="I84">
-        <v>2.5005259351080937E-2</v>
+        <v>-0.82400970277019769</v>
       </c>
       <c r="J84">
-        <v>7.4050317324194259E-2</v>
+        <v>-0.51468873944329674</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>-9.1402723133016395E-2</v>
+        <v>-0.37772094186069671</v>
       </c>
       <c r="B85">
-        <v>0.31109363355082176</v>
+        <v>0.66478162252051831</v>
       </c>
       <c r="C85">
-        <v>-4.5229112814403845E-2</v>
+        <v>0.97031820903104049</v>
       </c>
       <c r="D85">
-        <v>0.93619567616041599</v>
+        <v>-8.5580394797382109E-2</v>
       </c>
       <c r="E85">
-        <v>-0.12603434502916197</v>
+        <v>0.47465349627842285</v>
       </c>
       <c r="F85">
-        <v>0.55023887128604476</v>
+        <v>0.96237893836561184</v>
       </c>
       <c r="G85">
-        <v>-0.6344916211522118</v>
+        <v>0.11905250262602787</v>
       </c>
       <c r="H85">
-        <v>-0.18286010738529168</v>
+        <v>0.35786081104357143</v>
       </c>
       <c r="I85">
-        <v>0.48590340002369486</v>
+        <v>-0.69416627840228318</v>
       </c>
       <c r="J85">
-        <v>-0.79453724878185439</v>
+        <v>-0.84223234933881819</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>0.58053728877231092</v>
+        <v>0.73787867046576061</v>
       </c>
       <c r="B86">
-        <v>8.9205222510666149E-2</v>
+        <v>0.95261814345123097</v>
       </c>
       <c r="C86">
-        <v>0.29371503077734429</v>
+        <v>0.94683360866040445</v>
       </c>
       <c r="D86">
-        <v>-0.72278071122080356</v>
+        <v>-0.17853024387634467</v>
       </c>
       <c r="E86">
-        <v>-0.63876361921101676</v>
+        <v>0.65823932003180152</v>
       </c>
       <c r="F86">
-        <v>-0.68929348234827859</v>
+        <v>0.9285108881271974</v>
       </c>
       <c r="G86">
-        <v>-0.583188161823194</v>
+        <v>-0.64490903919212417</v>
       </c>
       <c r="H86">
-        <v>0.39305478181428116</v>
+        <v>-0.62373973722023757</v>
       </c>
       <c r="I86">
-        <v>-0.73034707790990372</v>
+        <v>-0.90893425214015955</v>
       </c>
       <c r="J86">
-        <v>-0.71933286778990413</v>
+        <v>-0.86232799090858481</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>0.79744139981290263</v>
+        <v>-7.5966112973886279E-2</v>
       </c>
       <c r="B87">
-        <v>0.90850763586340511</v>
+        <v>-0.16481642396139828</v>
       </c>
       <c r="C87">
-        <v>0.18670779637129464</v>
+        <v>-0.78225635965078677</v>
       </c>
       <c r="D87">
-        <v>-0.33097075418890498</v>
+        <v>6.6745467317964324E-2</v>
       </c>
       <c r="E87">
-        <v>-0.84895201066922465</v>
+        <v>-0.50498865794841608</v>
       </c>
       <c r="F87">
-        <v>0.93243858884639697</v>
+        <v>0.45976034164062074</v>
       </c>
       <c r="G87">
-        <v>-0.93177536239758796</v>
+        <v>-0.49446441800733121</v>
       </c>
       <c r="H87">
-        <v>0.86986104672782716</v>
+        <v>0.48489511577600458</v>
       </c>
       <c r="I87">
-        <v>-0.86846241248260481</v>
+        <v>0.74456738067433803</v>
       </c>
       <c r="J87">
-        <v>-0.95374228635041258</v>
+        <v>-0.66617135457839816</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0.98144776095887643</v>
+        <v>8.572470892235777E-2</v>
       </c>
       <c r="B88">
-        <v>0.96314656531232912</v>
+        <v>0.54492621716717571</v>
       </c>
       <c r="C88">
-        <v>0.52476508678516964</v>
+        <v>0.23562259165892829</v>
       </c>
       <c r="D88">
-        <v>0.74794633105237407</v>
+        <v>0.91263797734715557</v>
       </c>
       <c r="E88">
-        <v>-0.91890076536353893</v>
+        <v>-0.83748459752607252</v>
       </c>
       <c r="F88">
-        <v>0.99458502301238194</v>
+        <v>-0.25678511868035819</v>
       </c>
       <c r="G88">
-        <v>-0.79994151756272436</v>
+        <v>0.56213288008298556</v>
       </c>
       <c r="H88">
-        <v>0.9880460769721704</v>
+        <v>0.20351500866641722</v>
       </c>
       <c r="I88">
-        <v>-0.42524823418842694</v>
+        <v>0.72502524317657835</v>
       </c>
       <c r="J88">
-        <v>-0.86488901988693601</v>
+        <v>0.45898130898279516</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>-0.46111775465360494</v>
+        <v>-0.25442688009220427</v>
       </c>
       <c r="B89">
-        <v>-0.27154809561129378</v>
+        <v>-0.73455895925228154</v>
       </c>
       <c r="C89">
-        <v>-0.3800050072618672</v>
+        <v>0.40073849820732249</v>
       </c>
       <c r="D89">
-        <v>0.28178593968008725</v>
+        <v>-0.29669152902052953</v>
       </c>
       <c r="E89">
-        <v>0.66433978824142559</v>
+        <v>0.54229612675724415</v>
       </c>
       <c r="F89">
-        <v>-0.4029588713685941</v>
+        <v>0.27789307601205321</v>
       </c>
       <c r="G89">
-        <v>0.70124988495295359</v>
+        <v>-0.80642071222474976</v>
       </c>
       <c r="H89">
-        <v>0.40096467165097738</v>
+        <v>-2.2557050332439047E-2</v>
       </c>
       <c r="I89">
-        <v>0.67447344794749375</v>
+        <v>3.1217520452290638E-2</v>
       </c>
       <c r="J89">
-        <v>0.46527945522930142</v>
+        <v>-4.0071521319958607E-2</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0.4302026293247776</v>
+        <v>0.92093271831115553</v>
       </c>
       <c r="B90">
-        <v>0.4849453332764414</v>
+        <v>-0.29786037678782717</v>
       </c>
       <c r="C90">
-        <v>0.83004860486597887</v>
+        <v>-0.86280996079371741</v>
       </c>
       <c r="D90">
-        <v>-0.58441316403215537</v>
+        <v>-0.73472126332850107</v>
       </c>
       <c r="E90">
-        <v>-0.66573330963675903</v>
+        <v>-0.56585765044799852</v>
       </c>
       <c r="F90">
-        <v>0.93341156928392077</v>
+        <v>-0.50410813430696755</v>
       </c>
       <c r="G90">
-        <v>-0.79384217188090722</v>
+        <v>-0.98350801288486978</v>
       </c>
       <c r="H90">
-        <v>0.71116652152166238</v>
+        <v>0.32214298211938236</v>
       </c>
       <c r="I90">
-        <v>-0.64675756522776884</v>
+        <v>-0.80797379807175007</v>
       </c>
       <c r="J90">
-        <v>-0.21999415070045819</v>
+        <v>-0.93307088409854799</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>0.80757573062395671</v>
+        <v>-4.4009235077728616E-2</v>
       </c>
       <c r="B91">
-        <v>0.18275361617131097</v>
+        <v>-0.54875173648166142</v>
       </c>
       <c r="C91">
-        <v>0.65028281989987324</v>
+        <v>-0.86077600113716546</v>
       </c>
       <c r="D91">
-        <v>-0.28609696337209123</v>
+        <v>-0.99185730006374095</v>
       </c>
       <c r="E91">
-        <v>-0.52866645194451689</v>
+        <v>-0.12423098392169334</v>
       </c>
       <c r="F91">
-        <v>0.67657904623578591</v>
+        <v>-0.38877142374532653</v>
       </c>
       <c r="G91">
-        <v>0.90990952572994699</v>
+        <v>-0.82907188978962076</v>
       </c>
       <c r="H91">
-        <v>0.90537976228358574</v>
+        <v>-0.98711712055077971</v>
       </c>
       <c r="I91">
-        <v>-0.17999974015687994</v>
+        <v>-0.68498215033945287</v>
       </c>
       <c r="J91">
-        <v>0.89611095917997152</v>
+        <v>0.82706998837371914</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>-0.70062278863370298</v>
+        <v>-0.88064330733754204</v>
       </c>
       <c r="B92">
-        <v>-0.58239825157661684</v>
+        <v>-0.93322211880982353</v>
       </c>
       <c r="C92">
-        <v>-0.92439850164838289</v>
+        <v>-0.76504878937272436</v>
       </c>
       <c r="D92">
-        <v>-0.84030982627378759</v>
+        <v>-0.99073900974633822</v>
       </c>
       <c r="E92">
-        <v>-0.28942511585908909</v>
+        <v>-0.89582043146901902</v>
       </c>
       <c r="F92">
-        <v>-0.84371446386677851</v>
+        <v>-9.4579829000826066E-2</v>
       </c>
       <c r="G92">
-        <v>0.10325434732835115</v>
+        <v>0.22082970059246892</v>
       </c>
       <c r="H92">
-        <v>-0.87658082631981304</v>
+        <v>-0.79236005607333837</v>
       </c>
       <c r="I92">
-        <v>0.7166468083369395</v>
+        <v>0.89600246208133794</v>
       </c>
       <c r="J92">
-        <v>0.88586182205070962</v>
+        <v>-0.75810418105483113</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>-0.24760349227236406</v>
+        <v>-0.72442778817490916</v>
       </c>
       <c r="B93">
-        <v>0.70417093833261046</v>
+        <v>-0.43732363957978998</v>
       </c>
       <c r="C93">
-        <v>0.83169109182004131</v>
+        <v>0.63282323102768467</v>
       </c>
       <c r="D93">
-        <v>-0.87554359386510383</v>
+        <v>0.90281705150768521</v>
       </c>
       <c r="E93">
-        <v>-0.95007733567333408</v>
+        <v>0.37325988666184606</v>
       </c>
       <c r="F93">
-        <v>0.33292827878199244</v>
+        <v>-0.4946093691587452</v>
       </c>
       <c r="G93">
-        <v>-0.75163959256209933</v>
+        <v>-0.74221062128384818</v>
       </c>
       <c r="H93">
-        <v>0.65525607888151616</v>
+        <v>0.8237321384501517</v>
       </c>
       <c r="I93">
-        <v>-0.70551347790641528</v>
+        <v>0.14011219517448753</v>
       </c>
       <c r="J93">
-        <v>-0.98728547853547099</v>
+        <v>-0.24663532244392811</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>-0.57577615953378936</v>
+        <v>0.5475700967767817</v>
       </c>
       <c r="B94">
-        <v>-0.438372801187076</v>
+        <v>0.74610233860083364</v>
       </c>
       <c r="C94">
-        <v>-0.69121662677898787</v>
+        <v>-0.67548719753403241</v>
       </c>
       <c r="D94">
-        <v>-0.14735703793475594</v>
+        <v>-0.73395084621234508</v>
       </c>
       <c r="E94">
-        <v>-0.36800657871017195</v>
+        <v>0.75979554403314953</v>
       </c>
       <c r="F94">
-        <v>-0.13475094716832656</v>
+        <v>0.91855682154639706</v>
       </c>
       <c r="G94">
-        <v>-0.75824153187622323</v>
+        <v>0.84830276747852529</v>
       </c>
       <c r="H94">
-        <v>0.13846597241062333</v>
+        <v>0.69753714079842788</v>
       </c>
       <c r="I94">
-        <v>0.48678872944077639</v>
+        <v>0.72973626732721708</v>
       </c>
       <c r="J94">
-        <v>-0.89169943469286361</v>
+        <v>0.94709157047815273</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>4.1483564032397072E-2</v>
+        <v>0.24818505807194055</v>
       </c>
       <c r="B95">
-        <v>-0.43170635105814259</v>
+        <v>-0.21266982956477207</v>
       </c>
       <c r="C95">
-        <v>-0.22293810275537479</v>
+        <v>0.42487116279812115</v>
       </c>
       <c r="D95">
-        <v>0.68400168190758837</v>
+        <v>0.6556415386463107</v>
       </c>
       <c r="E95">
-        <v>-0.41443679713427517</v>
+        <v>-0.99745751120850634</v>
       </c>
       <c r="F95">
-        <v>-0.56896302581776681</v>
+        <v>0.9567820541399743</v>
       </c>
       <c r="G95">
-        <v>0.13984111119342563</v>
+        <v>0.78202369236417779</v>
       </c>
       <c r="H95">
-        <v>-0.7806797105705392</v>
+        <v>0.87488041095821556</v>
       </c>
       <c r="I95">
-        <v>0.53464767996496554</v>
+        <v>0.95048983980905399</v>
       </c>
       <c r="J95">
-        <v>-3.2627621296688836E-2</v>
+        <v>0.90024190134474968</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>-0.86562322096183286</v>
+        <v>-0.50875002809648562</v>
       </c>
       <c r="B96">
-        <v>-0.82623970131162183</v>
+        <v>-0.92771891755142832</v>
       </c>
       <c r="C96">
-        <v>-0.68980125565648098</v>
+        <v>0.23965741575583238</v>
       </c>
       <c r="D96">
-        <v>-0.80130672177485296</v>
+        <v>0.18499900270506128</v>
       </c>
       <c r="E96">
-        <v>0.86350680924619228</v>
+        <v>9.536675445212428E-2</v>
       </c>
       <c r="F96">
-        <v>-0.73266008373513902</v>
+        <v>-0.85044812158013272</v>
       </c>
       <c r="G96">
-        <v>-0.85738414384243278</v>
+        <v>0.48084260823218378</v>
       </c>
       <c r="H96">
-        <v>-0.67297110859568676</v>
+        <v>-0.71701982258686592</v>
       </c>
       <c r="I96">
-        <v>0.59203186212724601</v>
+        <v>-0.25429959850190131</v>
       </c>
       <c r="J96">
-        <v>-0.52957432927781567</v>
+        <v>-0.186239044605085</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>-0.50729603824867409</v>
+        <v>0.66790294592645649</v>
       </c>
       <c r="B97">
-        <v>-0.12740519423573393</v>
+        <v>-0.70537058789441998</v>
       </c>
       <c r="C97">
-        <v>-0.44231018822369328</v>
+        <v>-0.60290211915244063</v>
       </c>
       <c r="D97">
-        <v>0.94781547362615781</v>
+        <v>-0.38176710048993578</v>
       </c>
       <c r="E97">
-        <v>0.39777342920958603</v>
+        <v>0.47035105947147454</v>
       </c>
       <c r="F97">
-        <v>-0.59779251782022758</v>
+        <v>-0.97380833954251211</v>
       </c>
       <c r="G97">
-        <v>-0.38319415115743999</v>
+        <v>-0.89476715889701364</v>
       </c>
       <c r="H97">
-        <v>-0.82675564353561581</v>
+        <v>-0.97785102015681458</v>
       </c>
       <c r="I97">
-        <v>-0.54476539768995713</v>
+        <v>-0.77437241935515966</v>
       </c>
       <c r="J97">
-        <v>-0.55129973499521501</v>
+        <v>-0.9641288100538119</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>-3.1634155336393778E-2</v>
+        <v>0.49879751089883401</v>
       </c>
       <c r="B98">
-        <v>0.63191871383353393</v>
+        <v>-0.31111321062951414</v>
       </c>
       <c r="C98">
-        <v>0.52042619331549556</v>
+        <v>-0.93240647521342601</v>
       </c>
       <c r="D98">
-        <v>-0.65392317424613267</v>
+        <v>-0.93810879608648134</v>
       </c>
       <c r="E98">
-        <v>0.38781242260507831</v>
+        <v>-0.7004059462000306</v>
       </c>
       <c r="F98">
-        <v>0.41721693772473833</v>
+        <v>-0.61791348984511418</v>
       </c>
       <c r="G98">
-        <v>-0.24196512699676626</v>
+        <v>-0.98291020214649283</v>
       </c>
       <c r="H98">
-        <v>0.8267643367936568</v>
+        <v>-0.97818537415667473</v>
       </c>
       <c r="I98">
-        <v>-0.88804195269489383</v>
+        <v>-0.66677853629499051</v>
       </c>
       <c r="J98">
-        <v>-0.35109994396445998</v>
+        <v>-0.9364901099220313</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>0.44669341070222324</v>
+        <v>0.87562282175792217</v>
       </c>
       <c r="B99">
-        <v>0.89607360469466601</v>
+        <v>-0.94288796182593582</v>
       </c>
       <c r="C99">
-        <v>0.96760417964636192</v>
+        <v>-0.3104450032916749</v>
       </c>
       <c r="D99">
-        <v>0.95449093762105419</v>
+        <v>0.52048925948654157</v>
       </c>
       <c r="E99">
-        <v>-0.3485684264726997</v>
+        <v>-0.64888401600709977</v>
       </c>
       <c r="F99">
-        <v>0.91248342534647509</v>
+        <v>-0.88467605578644792</v>
       </c>
       <c r="G99">
-        <v>-0.88628336904688876</v>
+        <v>-0.95659627204080144</v>
       </c>
       <c r="H99">
-        <v>0.7330618355224886</v>
+        <v>-0.35077092482416211</v>
       </c>
       <c r="I99">
-        <v>-0.98907094530204787</v>
+        <v>-0.96124787945593748</v>
       </c>
       <c r="J99">
-        <v>-0.98791061152733894</v>
+        <v>8.90607856377649E-2</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>0.19694235684470066</v>
+        <v>-0.82855576036066569</v>
       </c>
       <c r="B100">
-        <v>-0.28965559163792542</v>
+        <v>0.75011690501898987</v>
       </c>
       <c r="C100">
-        <v>-0.84040889920945916</v>
+        <v>-0.94756007717729906</v>
       </c>
       <c r="D100">
-        <v>-0.58080342259768925</v>
+        <v>4.2918791041556152E-2</v>
       </c>
       <c r="E100">
-        <v>-0.36520915410310012</v>
+        <v>0.16785792489639501</v>
       </c>
       <c r="F100">
-        <v>-0.65325240523188677</v>
+        <v>0.76763385098865711</v>
       </c>
       <c r="G100">
-        <v>0.98591294147359954</v>
+        <v>0.5416731269665529</v>
       </c>
       <c r="H100">
-        <v>2.1048643125647949E-2</v>
+        <v>0.12765313908135487</v>
       </c>
       <c r="I100">
-        <v>0.87007334226768185</v>
+        <v>0.70760206346166155</v>
       </c>
       <c r="J100">
-        <v>0.73286243967763476</v>
+        <v>0.90440415697203158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>